<commit_message>
Update in WebAppData file to Electric Vehicles Sales Mandate description
</commit_message>
<xml_diff>
--- a/WebAppData.xlsx
+++ b/WebAppData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swenzel\Dropbox (Energy Innovation)\My PC (energy044)\Documents\GitHub_Repositories\eps-alberta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD1486C3-E2C5-47ED-BF6E-21AD679E097E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{540BD43F-311C-4EF0-919C-713863B20E84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12600" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4110,13 +4110,13 @@
     <t>**Description:** This policy causes government to pay for the specified percentage of the purchase price of new battery electric passenger LDVs.  This is in addition to EV subsidies that exist in the BAU case.  // **Guidance for setting values:** In Canada, several provinces have EV subsidy programs, paying for between $5000 and $14000 of the cost of a new EV.  This is roughly between 10% and 35% of the cost of a new EV.</t>
   </si>
   <si>
-    <t>**Description:** This policy requires the specified percentage of newly sold vehicles of the selected type(s) to consist of battery electric vehicles. If that percentage would already be achieved through BAU sales plus the effects of other policies, such as an EV subsidy, this policy has no effect. Manufactures may meet a sales standard through techniques such as more heavily marketing electric vehicles, lowering the price of electric vehicles, or raising the price of non-electric vehicles. // **Guidance for setting values:** // **LDVs:** Under the Pan-Canadian Framework, Canada has a target of a 30% market share for electric vehicles among new on-road vehicles by 2030. // **HDVs:** Under the Pan-Canadian Framework, Canada has a target of a 30% market share for electric vehicles among new on-road vehicles by 2030. // **Passenger Motorbikes:** Under the Pan-Canadian Framework, Canada has a target of a 30% market share for electric vehicles among new on-road vehicles by 2030.</t>
-  </si>
-  <si>
     <t>It matches policies to the listing in the "PolicyLevers" tab using the "Vensim Variable Name" column.</t>
   </si>
   <si>
     <t>This tab contains information about each policy that does not vary by subscripted element of that policy.</t>
+  </si>
+  <si>
+    <t>**Description:** This policy requires the specified percentage of newly sold vehicles of the selected type(s) to consist of battery electric vehicles. If that percentage would already be achieved through BAU sales plus the effects of other policies, such as an EV subsidy, this policy has no effect. Manufactures may meet a sales standard through techniques such as more heavily marketing electric vehicles, lowering the price of electric vehicles, or raising the price of non-electric vehicles. // **Guidance for setting values:** Under the Pan-Canadian Framework, Canada has a target of a 30% market share for electric vehicles among new on-road vehicles by 2030.</t>
   </si>
 </sst>
 </file>
@@ -5337,9 +5337,6 @@
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -5348,6 +5345,9 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -6416,8 +6416,8 @@
   </sheetPr>
   <dimension ref="A1:N105"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -6438,7 +6438,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A1" s="190" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
       <c r="B1" s="188"/>
       <c r="C1" s="188"/>
@@ -6456,7 +6456,7 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A2" s="189" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
       <c r="B2" s="188"/>
       <c r="C2" s="188"/>
@@ -6621,7 +6621,7 @@
         <v>579</v>
       </c>
       <c r="J6" s="169" t="s">
-        <v>1212</v>
+        <v>1214</v>
       </c>
       <c r="K6" s="75" t="s">
         <v>580</v>
@@ -9836,7 +9836,7 @@
       </c>
       <c r="P9" s="195" t="str">
         <f>INDEX('Policy Characteristics'!J:J,MATCH($C9,'Policy Characteristics'!$C:$C,0))</f>
-        <v>**Description:** This policy requires the specified percentage of newly sold vehicles of the selected type(s) to consist of battery electric vehicles. If that percentage would already be achieved through BAU sales plus the effects of other policies, such as an EV subsidy, this policy has no effect. Manufactures may meet a sales standard through techniques such as more heavily marketing electric vehicles, lowering the price of electric vehicles, or raising the price of non-electric vehicles. // **Guidance for setting values:** // **LDVs:** Under the Pan-Canadian Framework, Canada has a target of a 30% market share for electric vehicles among new on-road vehicles by 2030. // **HDVs:** Under the Pan-Canadian Framework, Canada has a target of a 30% market share for electric vehicles among new on-road vehicles by 2030. // **Passenger Motorbikes:** Under the Pan-Canadian Framework, Canada has a target of a 30% market share for electric vehicles among new on-road vehicles by 2030.</v>
+        <v>**Description:** This policy requires the specified percentage of newly sold vehicles of the selected type(s) to consist of battery electric vehicles. If that percentage would already be achieved through BAU sales plus the effects of other policies, such as an EV subsidy, this policy has no effect. Manufactures may meet a sales standard through techniques such as more heavily marketing electric vehicles, lowering the price of electric vehicles, or raising the price of non-electric vehicles. // **Guidance for setting values:** Under the Pan-Canadian Framework, Canada has a target of a 30% market share for electric vehicles among new on-road vehicles by 2030.</v>
       </c>
       <c r="Q9" s="75" t="s">
         <v>580</v>
@@ -9904,7 +9904,7 @@
       </c>
       <c r="P10" s="195" t="str">
         <f>INDEX('Policy Characteristics'!J:J,MATCH($C10,'Policy Characteristics'!$C:$C,0))</f>
-        <v>**Description:** This policy requires the specified percentage of newly sold vehicles of the selected type(s) to consist of battery electric vehicles. If that percentage would already be achieved through BAU sales plus the effects of other policies, such as an EV subsidy, this policy has no effect. Manufactures may meet a sales standard through techniques such as more heavily marketing electric vehicles, lowering the price of electric vehicles, or raising the price of non-electric vehicles. // **Guidance for setting values:** // **LDVs:** Under the Pan-Canadian Framework, Canada has a target of a 30% market share for electric vehicles among new on-road vehicles by 2030. // **HDVs:** Under the Pan-Canadian Framework, Canada has a target of a 30% market share for electric vehicles among new on-road vehicles by 2030. // **Passenger Motorbikes:** Under the Pan-Canadian Framework, Canada has a target of a 30% market share for electric vehicles among new on-road vehicles by 2030.</v>
+        <v>**Description:** This policy requires the specified percentage of newly sold vehicles of the selected type(s) to consist of battery electric vehicles. If that percentage would already be achieved through BAU sales plus the effects of other policies, such as an EV subsidy, this policy has no effect. Manufactures may meet a sales standard through techniques such as more heavily marketing electric vehicles, lowering the price of electric vehicles, or raising the price of non-electric vehicles. // **Guidance for setting values:** Under the Pan-Canadian Framework, Canada has a target of a 30% market share for electric vehicles among new on-road vehicles by 2030.</v>
       </c>
       <c r="Q10" s="63" t="str">
         <f t="shared" si="4"/>
@@ -9974,7 +9974,7 @@
       </c>
       <c r="P11" s="195" t="str">
         <f>INDEX('Policy Characteristics'!J:J,MATCH($C11,'Policy Characteristics'!$C:$C,0))</f>
-        <v>**Description:** This policy requires the specified percentage of newly sold vehicles of the selected type(s) to consist of battery electric vehicles. If that percentage would already be achieved through BAU sales plus the effects of other policies, such as an EV subsidy, this policy has no effect. Manufactures may meet a sales standard through techniques such as more heavily marketing electric vehicles, lowering the price of electric vehicles, or raising the price of non-electric vehicles. // **Guidance for setting values:** // **LDVs:** Under the Pan-Canadian Framework, Canada has a target of a 30% market share for electric vehicles among new on-road vehicles by 2030. // **HDVs:** Under the Pan-Canadian Framework, Canada has a target of a 30% market share for electric vehicles among new on-road vehicles by 2030. // **Passenger Motorbikes:** Under the Pan-Canadian Framework, Canada has a target of a 30% market share for electric vehicles among new on-road vehicles by 2030.</v>
+        <v>**Description:** This policy requires the specified percentage of newly sold vehicles of the selected type(s) to consist of battery electric vehicles. If that percentage would already be achieved through BAU sales plus the effects of other policies, such as an EV subsidy, this policy has no effect. Manufactures may meet a sales standard through techniques such as more heavily marketing electric vehicles, lowering the price of electric vehicles, or raising the price of non-electric vehicles. // **Guidance for setting values:** Under the Pan-Canadian Framework, Canada has a target of a 30% market share for electric vehicles among new on-road vehicles by 2030.</v>
       </c>
       <c r="Q11" s="63" t="str">
         <f t="shared" si="4"/>
@@ -10044,7 +10044,7 @@
       </c>
       <c r="P12" s="195" t="str">
         <f>INDEX('Policy Characteristics'!J:J,MATCH($C12,'Policy Characteristics'!$C:$C,0))</f>
-        <v>**Description:** This policy requires the specified percentage of newly sold vehicles of the selected type(s) to consist of battery electric vehicles. If that percentage would already be achieved through BAU sales plus the effects of other policies, such as an EV subsidy, this policy has no effect. Manufactures may meet a sales standard through techniques such as more heavily marketing electric vehicles, lowering the price of electric vehicles, or raising the price of non-electric vehicles. // **Guidance for setting values:** // **LDVs:** Under the Pan-Canadian Framework, Canada has a target of a 30% market share for electric vehicles among new on-road vehicles by 2030. // **HDVs:** Under the Pan-Canadian Framework, Canada has a target of a 30% market share for electric vehicles among new on-road vehicles by 2030. // **Passenger Motorbikes:** Under the Pan-Canadian Framework, Canada has a target of a 30% market share for electric vehicles among new on-road vehicles by 2030.</v>
+        <v>**Description:** This policy requires the specified percentage of newly sold vehicles of the selected type(s) to consist of battery electric vehicles. If that percentage would already be achieved through BAU sales plus the effects of other policies, such as an EV subsidy, this policy has no effect. Manufactures may meet a sales standard through techniques such as more heavily marketing electric vehicles, lowering the price of electric vehicles, or raising the price of non-electric vehicles. // **Guidance for setting values:** Under the Pan-Canadian Framework, Canada has a target of a 30% market share for electric vehicles among new on-road vehicles by 2030.</v>
       </c>
       <c r="Q12" s="63" t="str">
         <f t="shared" si="4"/>
@@ -10100,7 +10100,7 @@
       <c r="O13" s="55"/>
       <c r="P13" s="195" t="str">
         <f>INDEX('Policy Characteristics'!J:J,MATCH($C13,'Policy Characteristics'!$C:$C,0))</f>
-        <v>**Description:** This policy requires the specified percentage of newly sold vehicles of the selected type(s) to consist of battery electric vehicles. If that percentage would already be achieved through BAU sales plus the effects of other policies, such as an EV subsidy, this policy has no effect. Manufactures may meet a sales standard through techniques such as more heavily marketing electric vehicles, lowering the price of electric vehicles, or raising the price of non-electric vehicles. // **Guidance for setting values:** // **LDVs:** Under the Pan-Canadian Framework, Canada has a target of a 30% market share for electric vehicles among new on-road vehicles by 2030. // **HDVs:** Under the Pan-Canadian Framework, Canada has a target of a 30% market share for electric vehicles among new on-road vehicles by 2030. // **Passenger Motorbikes:** Under the Pan-Canadian Framework, Canada has a target of a 30% market share for electric vehicles among new on-road vehicles by 2030.</v>
+        <v>**Description:** This policy requires the specified percentage of newly sold vehicles of the selected type(s) to consist of battery electric vehicles. If that percentage would already be achieved through BAU sales plus the effects of other policies, such as an EV subsidy, this policy has no effect. Manufactures may meet a sales standard through techniques such as more heavily marketing electric vehicles, lowering the price of electric vehicles, or raising the price of non-electric vehicles. // **Guidance for setting values:** Under the Pan-Canadian Framework, Canada has a target of a 30% market share for electric vehicles among new on-road vehicles by 2030.</v>
       </c>
       <c r="Q13" s="75"/>
       <c r="R13" s="75"/>
@@ -10150,7 +10150,7 @@
       <c r="O14" s="55"/>
       <c r="P14" s="195" t="str">
         <f>INDEX('Policy Characteristics'!J:J,MATCH($C14,'Policy Characteristics'!$C:$C,0))</f>
-        <v>**Description:** This policy requires the specified percentage of newly sold vehicles of the selected type(s) to consist of battery electric vehicles. If that percentage would already be achieved through BAU sales plus the effects of other policies, such as an EV subsidy, this policy has no effect. Manufactures may meet a sales standard through techniques such as more heavily marketing electric vehicles, lowering the price of electric vehicles, or raising the price of non-electric vehicles. // **Guidance for setting values:** // **LDVs:** Under the Pan-Canadian Framework, Canada has a target of a 30% market share for electric vehicles among new on-road vehicles by 2030. // **HDVs:** Under the Pan-Canadian Framework, Canada has a target of a 30% market share for electric vehicles among new on-road vehicles by 2030. // **Passenger Motorbikes:** Under the Pan-Canadian Framework, Canada has a target of a 30% market share for electric vehicles among new on-road vehicles by 2030.</v>
+        <v>**Description:** This policy requires the specified percentage of newly sold vehicles of the selected type(s) to consist of battery electric vehicles. If that percentage would already be achieved through BAU sales plus the effects of other policies, such as an EV subsidy, this policy has no effect. Manufactures may meet a sales standard through techniques such as more heavily marketing electric vehicles, lowering the price of electric vehicles, or raising the price of non-electric vehicles. // **Guidance for setting values:** Under the Pan-Canadian Framework, Canada has a target of a 30% market share for electric vehicles among new on-road vehicles by 2030.</v>
       </c>
       <c r="Q14" s="75"/>
       <c r="R14" s="75"/>
@@ -10200,7 +10200,7 @@
       <c r="O15" s="55"/>
       <c r="P15" s="195" t="str">
         <f>INDEX('Policy Characteristics'!J:J,MATCH($C15,'Policy Characteristics'!$C:$C,0))</f>
-        <v>**Description:** This policy requires the specified percentage of newly sold vehicles of the selected type(s) to consist of battery electric vehicles. If that percentage would already be achieved through BAU sales plus the effects of other policies, such as an EV subsidy, this policy has no effect. Manufactures may meet a sales standard through techniques such as more heavily marketing electric vehicles, lowering the price of electric vehicles, or raising the price of non-electric vehicles. // **Guidance for setting values:** // **LDVs:** Under the Pan-Canadian Framework, Canada has a target of a 30% market share for electric vehicles among new on-road vehicles by 2030. // **HDVs:** Under the Pan-Canadian Framework, Canada has a target of a 30% market share for electric vehicles among new on-road vehicles by 2030. // **Passenger Motorbikes:** Under the Pan-Canadian Framework, Canada has a target of a 30% market share for electric vehicles among new on-road vehicles by 2030.</v>
+        <v>**Description:** This policy requires the specified percentage of newly sold vehicles of the selected type(s) to consist of battery electric vehicles. If that percentage would already be achieved through BAU sales plus the effects of other policies, such as an EV subsidy, this policy has no effect. Manufactures may meet a sales standard through techniques such as more heavily marketing electric vehicles, lowering the price of electric vehicles, or raising the price of non-electric vehicles. // **Guidance for setting values:** Under the Pan-Canadian Framework, Canada has a target of a 30% market share for electric vehicles among new on-road vehicles by 2030.</v>
       </c>
       <c r="Q15" s="75"/>
       <c r="R15" s="75"/>
@@ -10250,7 +10250,7 @@
       <c r="O16" s="55"/>
       <c r="P16" s="195" t="str">
         <f>INDEX('Policy Characteristics'!J:J,MATCH($C16,'Policy Characteristics'!$C:$C,0))</f>
-        <v>**Description:** This policy requires the specified percentage of newly sold vehicles of the selected type(s) to consist of battery electric vehicles. If that percentage would already be achieved through BAU sales plus the effects of other policies, such as an EV subsidy, this policy has no effect. Manufactures may meet a sales standard through techniques such as more heavily marketing electric vehicles, lowering the price of electric vehicles, or raising the price of non-electric vehicles. // **Guidance for setting values:** // **LDVs:** Under the Pan-Canadian Framework, Canada has a target of a 30% market share for electric vehicles among new on-road vehicles by 2030. // **HDVs:** Under the Pan-Canadian Framework, Canada has a target of a 30% market share for electric vehicles among new on-road vehicles by 2030. // **Passenger Motorbikes:** Under the Pan-Canadian Framework, Canada has a target of a 30% market share for electric vehicles among new on-road vehicles by 2030.</v>
+        <v>**Description:** This policy requires the specified percentage of newly sold vehicles of the selected type(s) to consist of battery electric vehicles. If that percentage would already be achieved through BAU sales plus the effects of other policies, such as an EV subsidy, this policy has no effect. Manufactures may meet a sales standard through techniques such as more heavily marketing electric vehicles, lowering the price of electric vehicles, or raising the price of non-electric vehicles. // **Guidance for setting values:** Under the Pan-Canadian Framework, Canada has a target of a 30% market share for electric vehicles among new on-road vehicles by 2030.</v>
       </c>
       <c r="Q16" s="75"/>
       <c r="R16" s="75"/>
@@ -10300,7 +10300,7 @@
       <c r="O17" s="55"/>
       <c r="P17" s="195" t="str">
         <f>INDEX('Policy Characteristics'!J:J,MATCH($C17,'Policy Characteristics'!$C:$C,0))</f>
-        <v>**Description:** This policy requires the specified percentage of newly sold vehicles of the selected type(s) to consist of battery electric vehicles. If that percentage would already be achieved through BAU sales plus the effects of other policies, such as an EV subsidy, this policy has no effect. Manufactures may meet a sales standard through techniques such as more heavily marketing electric vehicles, lowering the price of electric vehicles, or raising the price of non-electric vehicles. // **Guidance for setting values:** // **LDVs:** Under the Pan-Canadian Framework, Canada has a target of a 30% market share for electric vehicles among new on-road vehicles by 2030. // **HDVs:** Under the Pan-Canadian Framework, Canada has a target of a 30% market share for electric vehicles among new on-road vehicles by 2030. // **Passenger Motorbikes:** Under the Pan-Canadian Framework, Canada has a target of a 30% market share for electric vehicles among new on-road vehicles by 2030.</v>
+        <v>**Description:** This policy requires the specified percentage of newly sold vehicles of the selected type(s) to consist of battery electric vehicles. If that percentage would already be achieved through BAU sales plus the effects of other policies, such as an EV subsidy, this policy has no effect. Manufactures may meet a sales standard through techniques such as more heavily marketing electric vehicles, lowering the price of electric vehicles, or raising the price of non-electric vehicles. // **Guidance for setting values:** Under the Pan-Canadian Framework, Canada has a target of a 30% market share for electric vehicles among new on-road vehicles by 2030.</v>
       </c>
       <c r="Q17" s="75"/>
       <c r="R17" s="75"/>
@@ -10350,7 +10350,7 @@
       <c r="O18" s="55"/>
       <c r="P18" s="195" t="str">
         <f>INDEX('Policy Characteristics'!J:J,MATCH($C18,'Policy Characteristics'!$C:$C,0))</f>
-        <v>**Description:** This policy requires the specified percentage of newly sold vehicles of the selected type(s) to consist of battery electric vehicles. If that percentage would already be achieved through BAU sales plus the effects of other policies, such as an EV subsidy, this policy has no effect. Manufactures may meet a sales standard through techniques such as more heavily marketing electric vehicles, lowering the price of electric vehicles, or raising the price of non-electric vehicles. // **Guidance for setting values:** // **LDVs:** Under the Pan-Canadian Framework, Canada has a target of a 30% market share for electric vehicles among new on-road vehicles by 2030. // **HDVs:** Under the Pan-Canadian Framework, Canada has a target of a 30% market share for electric vehicles among new on-road vehicles by 2030. // **Passenger Motorbikes:** Under the Pan-Canadian Framework, Canada has a target of a 30% market share for electric vehicles among new on-road vehicles by 2030.</v>
+        <v>**Description:** This policy requires the specified percentage of newly sold vehicles of the selected type(s) to consist of battery electric vehicles. If that percentage would already be achieved through BAU sales plus the effects of other policies, such as an EV subsidy, this policy has no effect. Manufactures may meet a sales standard through techniques such as more heavily marketing electric vehicles, lowering the price of electric vehicles, or raising the price of non-electric vehicles. // **Guidance for setting values:** Under the Pan-Canadian Framework, Canada has a target of a 30% market share for electric vehicles among new on-road vehicles by 2030.</v>
       </c>
       <c r="Q18" s="75"/>
       <c r="R18" s="75"/>
@@ -10414,7 +10414,7 @@
       </c>
       <c r="P19" s="195" t="str">
         <f>INDEX('Policy Characteristics'!J:J,MATCH($C19,'Policy Characteristics'!$C:$C,0))</f>
-        <v>**Description:** This policy requires the specified percentage of newly sold vehicles of the selected type(s) to consist of battery electric vehicles. If that percentage would already be achieved through BAU sales plus the effects of other policies, such as an EV subsidy, this policy has no effect. Manufactures may meet a sales standard through techniques such as more heavily marketing electric vehicles, lowering the price of electric vehicles, or raising the price of non-electric vehicles. // **Guidance for setting values:** // **LDVs:** Under the Pan-Canadian Framework, Canada has a target of a 30% market share for electric vehicles among new on-road vehicles by 2030. // **HDVs:** Under the Pan-Canadian Framework, Canada has a target of a 30% market share for electric vehicles among new on-road vehicles by 2030. // **Passenger Motorbikes:** Under the Pan-Canadian Framework, Canada has a target of a 30% market share for electric vehicles among new on-road vehicles by 2030.</v>
+        <v>**Description:** This policy requires the specified percentage of newly sold vehicles of the selected type(s) to consist of battery electric vehicles. If that percentage would already be achieved through BAU sales plus the effects of other policies, such as an EV subsidy, this policy has no effect. Manufactures may meet a sales standard through techniques such as more heavily marketing electric vehicles, lowering the price of electric vehicles, or raising the price of non-electric vehicles. // **Guidance for setting values:** Under the Pan-Canadian Framework, Canada has a target of a 30% market share for electric vehicles among new on-road vehicles by 2030.</v>
       </c>
       <c r="Q19" s="63" t="str">
         <f t="shared" ref="Q19:R19" si="6">Q$9</f>
@@ -10470,7 +10470,7 @@
       <c r="O20" s="55"/>
       <c r="P20" s="195" t="str">
         <f>INDEX('Policy Characteristics'!J:J,MATCH($C20,'Policy Characteristics'!$C:$C,0))</f>
-        <v>**Description:** This policy requires the specified percentage of newly sold vehicles of the selected type(s) to consist of battery electric vehicles. If that percentage would already be achieved through BAU sales plus the effects of other policies, such as an EV subsidy, this policy has no effect. Manufactures may meet a sales standard through techniques such as more heavily marketing electric vehicles, lowering the price of electric vehicles, or raising the price of non-electric vehicles. // **Guidance for setting values:** // **LDVs:** Under the Pan-Canadian Framework, Canada has a target of a 30% market share for electric vehicles among new on-road vehicles by 2030. // **HDVs:** Under the Pan-Canadian Framework, Canada has a target of a 30% market share for electric vehicles among new on-road vehicles by 2030. // **Passenger Motorbikes:** Under the Pan-Canadian Framework, Canada has a target of a 30% market share for electric vehicles among new on-road vehicles by 2030.</v>
+        <v>**Description:** This policy requires the specified percentage of newly sold vehicles of the selected type(s) to consist of battery electric vehicles. If that percentage would already be achieved through BAU sales plus the effects of other policies, such as an EV subsidy, this policy has no effect. Manufactures may meet a sales standard through techniques such as more heavily marketing electric vehicles, lowering the price of electric vehicles, or raising the price of non-electric vehicles. // **Guidance for setting values:** Under the Pan-Canadian Framework, Canada has a target of a 30% market share for electric vehicles among new on-road vehicles by 2030.</v>
       </c>
       <c r="Q20" s="75"/>
       <c r="R20" s="75"/>
@@ -31733,13 +31733,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A1" s="196" t="s">
+      <c r="A1" s="199" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="196"/>
-      <c r="C1" s="196"/>
-      <c r="D1" s="196"/>
-      <c r="E1" s="196"/>
+      <c r="B1" s="199"/>
+      <c r="C1" s="199"/>
+      <c r="D1" s="199"/>
+      <c r="E1" s="199"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A2" s="200" t="s">
@@ -31808,13 +31808,13 @@
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A60" s="196" t="s">
+      <c r="A60" s="199" t="s">
         <v>198</v>
       </c>
-      <c r="B60" s="196"/>
-      <c r="C60" s="196"/>
-      <c r="D60" s="196"/>
-      <c r="E60" s="196"/>
+      <c r="B60" s="199"/>
+      <c r="C60" s="199"/>
+      <c r="D60" s="199"/>
+      <c r="E60" s="199"/>
     </row>
     <row r="85" spans="1:39" s="12" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A85" s="9" t="s">
@@ -31919,13 +31919,13 @@
       </c>
     </row>
     <row r="89" spans="1:39" x14ac:dyDescent="0.75">
-      <c r="A89" s="196" t="s">
+      <c r="A89" s="199" t="s">
         <v>199</v>
       </c>
-      <c r="B89" s="196"/>
-      <c r="C89" s="196"/>
-      <c r="D89" s="196"/>
-      <c r="E89" s="196"/>
+      <c r="B89" s="199"/>
+      <c r="C89" s="199"/>
+      <c r="D89" s="199"/>
+      <c r="E89" s="199"/>
     </row>
     <row r="90" spans="1:39" x14ac:dyDescent="0.75">
       <c r="A90" s="9">
@@ -32012,13 +32012,13 @@
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A98" s="196" t="s">
+      <c r="A98" s="199" t="s">
         <v>200</v>
       </c>
-      <c r="B98" s="196"/>
-      <c r="C98" s="196"/>
-      <c r="D98" s="196"/>
-      <c r="E98" s="196"/>
+      <c r="B98" s="199"/>
+      <c r="C98" s="199"/>
+      <c r="D98" s="199"/>
+      <c r="E98" s="199"/>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A99" s="17">
@@ -32102,13 +32102,13 @@
       <c r="A108" s="20"/>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A109" s="196" t="s">
+      <c r="A109" s="199" t="s">
         <v>202</v>
       </c>
-      <c r="B109" s="196"/>
-      <c r="C109" s="196"/>
-      <c r="D109" s="196"/>
-      <c r="E109" s="196"/>
+      <c r="B109" s="199"/>
+      <c r="C109" s="199"/>
+      <c r="D109" s="199"/>
+      <c r="E109" s="199"/>
     </row>
     <row r="110" spans="1:5" ht="15.5" thickBot="1" x14ac:dyDescent="0.9"/>
     <row r="111" spans="1:5" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
@@ -32121,13 +32121,13 @@
       </c>
     </row>
     <row r="113" spans="1:14" x14ac:dyDescent="0.75">
-      <c r="A113" s="196" t="s">
+      <c r="A113" s="199" t="s">
         <v>201</v>
       </c>
-      <c r="B113" s="196"/>
-      <c r="C113" s="196"/>
-      <c r="D113" s="196"/>
-      <c r="E113" s="196"/>
+      <c r="B113" s="199"/>
+      <c r="C113" s="199"/>
+      <c r="D113" s="199"/>
+      <c r="E113" s="199"/>
     </row>
     <row r="114" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A114" s="17">
@@ -32208,13 +32208,13 @@
       </c>
     </row>
     <row r="124" spans="1:14" x14ac:dyDescent="0.75">
-      <c r="A124" s="196" t="s">
+      <c r="A124" s="199" t="s">
         <v>482</v>
       </c>
-      <c r="B124" s="196"/>
-      <c r="C124" s="196"/>
-      <c r="D124" s="196"/>
-      <c r="E124" s="196"/>
+      <c r="B124" s="199"/>
+      <c r="C124" s="199"/>
+      <c r="D124" s="199"/>
+      <c r="E124" s="199"/>
       <c r="L124" s="21"/>
     </row>
     <row r="125" spans="1:14" x14ac:dyDescent="0.75">
@@ -32305,13 +32305,13 @@
       <c r="C133" s="15"/>
     </row>
     <row r="134" spans="1:14" x14ac:dyDescent="0.75">
-      <c r="A134" s="196" t="s">
+      <c r="A134" s="199" t="s">
         <v>115</v>
       </c>
-      <c r="B134" s="196"/>
-      <c r="C134" s="196"/>
-      <c r="D134" s="196"/>
-      <c r="E134" s="196"/>
+      <c r="B134" s="199"/>
+      <c r="C134" s="199"/>
+      <c r="D134" s="199"/>
+      <c r="E134" s="199"/>
     </row>
     <row r="135" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A135" s="27" t="s">
@@ -32326,25 +32326,25 @@
     </row>
     <row r="136" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A136" s="29"/>
-      <c r="B136" s="197" t="s">
+      <c r="B136" s="196" t="s">
         <v>502</v>
       </c>
-      <c r="C136" s="198"/>
-      <c r="D136" s="198"/>
-      <c r="E136" s="199"/>
+      <c r="C136" s="197"/>
+      <c r="D136" s="197"/>
+      <c r="E136" s="198"/>
       <c r="F136" s="28"/>
       <c r="G136" s="28"/>
     </row>
     <row r="137" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A137" s="30"/>
-      <c r="B137" s="197" t="s">
+      <c r="B137" s="196" t="s">
         <v>503</v>
       </c>
-      <c r="C137" s="199"/>
-      <c r="D137" s="197" t="s">
+      <c r="C137" s="198"/>
+      <c r="D137" s="196" t="s">
         <v>504</v>
       </c>
-      <c r="E137" s="199"/>
+      <c r="E137" s="198"/>
       <c r="F137" s="28"/>
       <c r="G137" s="28"/>
     </row>
@@ -32891,13 +32891,13 @@
       <c r="G163" s="28"/>
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A165" s="196" t="s">
+      <c r="A165" s="199" t="s">
         <v>205</v>
       </c>
-      <c r="B165" s="196"/>
-      <c r="C165" s="196"/>
-      <c r="D165" s="196"/>
-      <c r="E165" s="196"/>
+      <c r="B165" s="199"/>
+      <c r="C165" s="199"/>
+      <c r="D165" s="199"/>
+      <c r="E165" s="199"/>
     </row>
     <row r="166" spans="1:7" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
       <c r="A166" s="23" t="s">
@@ -32920,10 +32920,10 @@
       <c r="B168" s="46"/>
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A169" s="196" t="s">
+      <c r="A169" s="199" t="s">
         <v>490</v>
       </c>
-      <c r="B169" s="196"/>
+      <c r="B169" s="199"/>
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A170" s="23" t="s">
@@ -32955,13 +32955,13 @@
       <c r="B173" s="46"/>
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A174" s="196" t="s">
+      <c r="A174" s="199" t="s">
         <v>215</v>
       </c>
-      <c r="B174" s="196"/>
-      <c r="C174" s="196"/>
-      <c r="D174" s="196"/>
-      <c r="E174" s="196"/>
+      <c r="B174" s="199"/>
+      <c r="C174" s="199"/>
+      <c r="D174" s="199"/>
+      <c r="E174" s="199"/>
     </row>
     <row r="175" spans="1:7" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
       <c r="A175" s="23" t="s">
@@ -32981,13 +32981,13 @@
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A178" s="196" t="s">
+      <c r="A178" s="199" t="s">
         <v>208</v>
       </c>
-      <c r="B178" s="196"/>
-      <c r="C178" s="196"/>
-      <c r="D178" s="196"/>
-      <c r="E178" s="196"/>
+      <c r="B178" s="199"/>
+      <c r="C178" s="199"/>
+      <c r="D178" s="199"/>
+      <c r="E178" s="199"/>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A179" s="25" t="s">
@@ -33015,13 +33015,13 @@
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A183" s="196" t="s">
+      <c r="A183" s="199" t="s">
         <v>210</v>
       </c>
-      <c r="B183" s="196"/>
-      <c r="C183" s="196"/>
-      <c r="D183" s="196"/>
-      <c r="E183" s="196"/>
+      <c r="B183" s="199"/>
+      <c r="C183" s="199"/>
+      <c r="D183" s="199"/>
+      <c r="E183" s="199"/>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A184" s="23" t="s">
@@ -33076,13 +33076,13 @@
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A191" s="196" t="s">
+      <c r="A191" s="199" t="s">
         <v>227</v>
       </c>
-      <c r="B191" s="196"/>
-      <c r="C191" s="196"/>
-      <c r="D191" s="196"/>
-      <c r="E191" s="196"/>
+      <c r="B191" s="199"/>
+      <c r="C191" s="199"/>
+      <c r="D191" s="199"/>
+      <c r="E191" s="199"/>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A192" s="21" t="s">
@@ -33142,6 +33142,12 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A191:E191"/>
+    <mergeCell ref="A165:E165"/>
+    <mergeCell ref="A178:E178"/>
+    <mergeCell ref="A183:E183"/>
+    <mergeCell ref="A174:E174"/>
+    <mergeCell ref="A169:B169"/>
     <mergeCell ref="B136:E136"/>
     <mergeCell ref="B137:C137"/>
     <mergeCell ref="D137:E137"/>
@@ -33156,12 +33162,6 @@
     <mergeCell ref="A113:E113"/>
     <mergeCell ref="A109:E109"/>
     <mergeCell ref="A124:E124"/>
-    <mergeCell ref="A191:E191"/>
-    <mergeCell ref="A165:E165"/>
-    <mergeCell ref="A178:E178"/>
-    <mergeCell ref="A183:E183"/>
-    <mergeCell ref="A174:E174"/>
-    <mergeCell ref="A169:B169"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
Description text fix for conventional pollutant standard in WebAppData file
</commit_message>
<xml_diff>
--- a/WebAppData.xlsx
+++ b/WebAppData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swenzel\Dropbox (Energy Innovation)\My PC (energy044)\Documents\GitHub_Repositories\eps-alberta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{540BD43F-311C-4EF0-919C-713863B20E84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{712EF7AE-778F-43A3-B971-2CBEAA7AEE95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12600" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -257,7 +257,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5446" uniqueCount="1215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5446" uniqueCount="1216">
   <si>
     <t>Short Name</t>
   </si>
@@ -4117,6 +4117,9 @@
   </si>
   <si>
     <t>**Description:** This policy requires the specified percentage of newly sold vehicles of the selected type(s) to consist of battery electric vehicles. If that percentage would already be achieved through BAU sales plus the effects of other policies, such as an EV subsidy, this policy has no effect. Manufactures may meet a sales standard through techniques such as more heavily marketing electric vehicles, lowering the price of electric vehicles, or raising the price of non-electric vehicles. // **Guidance for setting values:** Under the Pan-Canadian Framework, Canada has a target of a 30% market share for electric vehicles among new on-road vehicles by 2030.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">**Description:** This policy represents strengthening standards for the selected pollutant(s) emitted by the selected vehicle type(s).  Conventional pollutants' most important, harmful impacts are on human health rather than on climate change. // **Guidance for setting values:** In Canada, the 24-hour national ambient air quality standard (Canadian Ambient Air Quality Standards – CAAQS) for PM2.5, the most harmful type of particulate for human health, is 28 µg/m^3 for the period 2015-2020. </t>
   </si>
 </sst>
 </file>
@@ -5337,6 +5340,9 @@
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -5345,9 +5351,6 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -6416,8 +6419,8 @@
   </sheetPr>
   <dimension ref="A1:N105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J59" sqref="J59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -6545,7 +6548,7 @@
         <v>1023</v>
       </c>
       <c r="J4" s="169" t="s">
-        <v>1116</v>
+        <v>1215</v>
       </c>
       <c r="K4" s="75" t="s">
         <v>1024</v>
@@ -6712,7 +6715,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="159.5" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:14" ht="169.25" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A9" s="169" t="s">
         <v>4</v>
       </c>
@@ -9233,31 +9236,31 @@
     <row r="78" spans="1:14" ht="44.4" customHeight="1" x14ac:dyDescent="0.75"/>
     <row r="79" spans="1:14" ht="44.4" customHeight="1" x14ac:dyDescent="0.75"/>
     <row r="80" spans="1:14" ht="44.4" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="81" s="97" customFormat="1" ht="44.4" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="82" s="97" customFormat="1" ht="44.4" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="83" s="97" customFormat="1" ht="44.4" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="84" s="97" customFormat="1" ht="44.4" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="85" s="97" customFormat="1" ht="44.4" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="86" s="97" customFormat="1" ht="44.4" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="87" s="97" customFormat="1" ht="44.4" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="88" s="97" customFormat="1" ht="44.4" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="89" s="97" customFormat="1" ht="44.4" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="90" s="97" customFormat="1" ht="44.4" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="91" s="97" customFormat="1" ht="44.4" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="92" s="97" customFormat="1" ht="44.4" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="93" s="97" customFormat="1" ht="44.4" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="94" s="97" customFormat="1" ht="44.4" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="95" s="97" customFormat="1" ht="44.4" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="96" s="97" customFormat="1" ht="44.4" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="97" s="97" customFormat="1" ht="44.4" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="98" s="97" customFormat="1" ht="44.4" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="99" s="97" customFormat="1" ht="44.4" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="100" s="97" customFormat="1" ht="44.4" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="101" s="97" customFormat="1" ht="44.4" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="102" s="97" customFormat="1" ht="44.4" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="103" s="97" customFormat="1" ht="44.4" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="104" s="97" customFormat="1" ht="44.4" customHeight="1" x14ac:dyDescent="0.75"/>
-    <row r="105" s="97" customFormat="1" ht="44.4" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="81" ht="44.4" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="82" ht="44.4" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="83" ht="44.4" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="84" ht="44.4" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="85" ht="44.4" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="86" ht="44.4" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="87" ht="44.4" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="88" ht="44.4" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="89" ht="44.4" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="90" ht="44.4" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="91" ht="44.4" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="92" ht="44.4" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="93" ht="44.4" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="94" ht="44.4" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="95" ht="44.4" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="96" ht="44.4" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="97" ht="44.4" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="98" ht="44.4" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="99" ht="44.4" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="100" ht="44.4" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="101" ht="44.4" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="102" ht="44.4" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="103" ht="44.4" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="104" ht="44.4" customHeight="1" x14ac:dyDescent="0.75"/>
+    <row r="105" ht="44.4" customHeight="1" x14ac:dyDescent="0.75"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="N47" r:id="rId1" display="https://www.fas.org/sgp/crs/misc/R40562.pdf, p.3, paragraph 1" xr:uid="{8A7D8EE0-6399-42B9-9F66-1CC80D94621D}"/>
@@ -9271,9 +9274,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:T327"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A197" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M95" sqref="M95"/>
+    <sheetView topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -9402,7 +9405,7 @@
       </c>
       <c r="P2" s="195" t="str">
         <f>INDEX('Policy Characteristics'!J:J,MATCH($C2,'Policy Characteristics'!$C:$C,0))</f>
-        <v xml:space="preserve">**Description:** This policy represents strengthening the standards for regulated pollutants other than greenhouse gases (such as NOx or particulate matter) for LDVs.  Conventional pollutants' most important, harmful impacts are on human health rather than on climate change. // **Guidance for setting values:** In Canada, the 24-hour national ambient air quality standard (Canadian Ambient Air Quality Standards – CAAQS) for PM2.5, the most harmful type of particulate for human health, is 28 µg/m^3 for the period 2015-2020. </v>
+        <v xml:space="preserve">**Description:** This policy represents strengthening standards for the selected pollutant(s) emitted by the selected vehicle type(s).  Conventional pollutants' most important, harmful impacts are on human health rather than on climate change. // **Guidance for setting values:** In Canada, the 24-hour national ambient air quality standard (Canadian Ambient Air Quality Standards – CAAQS) for PM2.5, the most harmful type of particulate for human health, is 28 µg/m^3 for the period 2015-2020. </v>
       </c>
       <c r="Q2" s="75" t="s">
         <v>1024</v>
@@ -9465,7 +9468,7 @@
       </c>
       <c r="P3" s="195" t="str">
         <f>INDEX('Policy Characteristics'!J:J,MATCH($C3,'Policy Characteristics'!$C:$C,0))</f>
-        <v xml:space="preserve">**Description:** This policy represents strengthening the standards for regulated pollutants other than greenhouse gases (such as NOx or particulate matter) for LDVs.  Conventional pollutants' most important, harmful impacts are on human health rather than on climate change. // **Guidance for setting values:** In Canada, the 24-hour national ambient air quality standard (Canadian Ambient Air Quality Standards – CAAQS) for PM2.5, the most harmful type of particulate for human health, is 28 µg/m^3 for the period 2015-2020. </v>
+        <v xml:space="preserve">**Description:** This policy represents strengthening standards for the selected pollutant(s) emitted by the selected vehicle type(s).  Conventional pollutants' most important, harmful impacts are on human health rather than on climate change. // **Guidance for setting values:** In Canada, the 24-hour national ambient air quality standard (Canadian Ambient Air Quality Standards – CAAQS) for PM2.5, the most harmful type of particulate for human health, is 28 µg/m^3 for the period 2015-2020. </v>
       </c>
       <c r="Q3" s="5" t="str">
         <f t="shared" si="1"/>
@@ -9530,7 +9533,7 @@
       </c>
       <c r="P4" s="195" t="str">
         <f>INDEX('Policy Characteristics'!J:J,MATCH($C4,'Policy Characteristics'!$C:$C,0))</f>
-        <v xml:space="preserve">**Description:** This policy represents strengthening the standards for regulated pollutants other than greenhouse gases (such as NOx or particulate matter) for LDVs.  Conventional pollutants' most important, harmful impacts are on human health rather than on climate change. // **Guidance for setting values:** In Canada, the 24-hour national ambient air quality standard (Canadian Ambient Air Quality Standards – CAAQS) for PM2.5, the most harmful type of particulate for human health, is 28 µg/m^3 for the period 2015-2020. </v>
+        <v xml:space="preserve">**Description:** This policy represents strengthening standards for the selected pollutant(s) emitted by the selected vehicle type(s).  Conventional pollutants' most important, harmful impacts are on human health rather than on climate change. // **Guidance for setting values:** In Canada, the 24-hour national ambient air quality standard (Canadian Ambient Air Quality Standards – CAAQS) for PM2.5, the most harmful type of particulate for human health, is 28 µg/m^3 for the period 2015-2020. </v>
       </c>
       <c r="Q4" s="5" t="str">
         <f t="shared" si="1"/>
@@ -9595,7 +9598,7 @@
       </c>
       <c r="P5" s="195" t="str">
         <f>INDEX('Policy Characteristics'!J:J,MATCH($C5,'Policy Characteristics'!$C:$C,0))</f>
-        <v xml:space="preserve">**Description:** This policy represents strengthening the standards for regulated pollutants other than greenhouse gases (such as NOx or particulate matter) for LDVs.  Conventional pollutants' most important, harmful impacts are on human health rather than on climate change. // **Guidance for setting values:** In Canada, the 24-hour national ambient air quality standard (Canadian Ambient Air Quality Standards – CAAQS) for PM2.5, the most harmful type of particulate for human health, is 28 µg/m^3 for the period 2015-2020. </v>
+        <v xml:space="preserve">**Description:** This policy represents strengthening standards for the selected pollutant(s) emitted by the selected vehicle type(s).  Conventional pollutants' most important, harmful impacts are on human health rather than on climate change. // **Guidance for setting values:** In Canada, the 24-hour national ambient air quality standard (Canadian Ambient Air Quality Standards – CAAQS) for PM2.5, the most harmful type of particulate for human health, is 28 µg/m^3 for the period 2015-2020. </v>
       </c>
       <c r="Q5" s="5" t="str">
         <f t="shared" si="1"/>
@@ -9660,7 +9663,7 @@
       </c>
       <c r="P6" s="195" t="str">
         <f>INDEX('Policy Characteristics'!J:J,MATCH($C6,'Policy Characteristics'!$C:$C,0))</f>
-        <v xml:space="preserve">**Description:** This policy represents strengthening the standards for regulated pollutants other than greenhouse gases (such as NOx or particulate matter) for LDVs.  Conventional pollutants' most important, harmful impacts are on human health rather than on climate change. // **Guidance for setting values:** In Canada, the 24-hour national ambient air quality standard (Canadian Ambient Air Quality Standards – CAAQS) for PM2.5, the most harmful type of particulate for human health, is 28 µg/m^3 for the period 2015-2020. </v>
+        <v xml:space="preserve">**Description:** This policy represents strengthening standards for the selected pollutant(s) emitted by the selected vehicle type(s).  Conventional pollutants' most important, harmful impacts are on human health rather than on climate change. // **Guidance for setting values:** In Canada, the 24-hour national ambient air quality standard (Canadian Ambient Air Quality Standards – CAAQS) for PM2.5, the most harmful type of particulate for human health, is 28 µg/m^3 for the period 2015-2020. </v>
       </c>
       <c r="Q6" s="5" t="str">
         <f t="shared" si="1"/>
@@ -9725,7 +9728,7 @@
       </c>
       <c r="P7" s="195" t="str">
         <f>INDEX('Policy Characteristics'!J:J,MATCH($C7,'Policy Characteristics'!$C:$C,0))</f>
-        <v xml:space="preserve">**Description:** This policy represents strengthening the standards for regulated pollutants other than greenhouse gases (such as NOx or particulate matter) for LDVs.  Conventional pollutants' most important, harmful impacts are on human health rather than on climate change. // **Guidance for setting values:** In Canada, the 24-hour national ambient air quality standard (Canadian Ambient Air Quality Standards – CAAQS) for PM2.5, the most harmful type of particulate for human health, is 28 µg/m^3 for the period 2015-2020. </v>
+        <v xml:space="preserve">**Description:** This policy represents strengthening standards for the selected pollutant(s) emitted by the selected vehicle type(s).  Conventional pollutants' most important, harmful impacts are on human health rather than on climate change. // **Guidance for setting values:** In Canada, the 24-hour national ambient air quality standard (Canadian Ambient Air Quality Standards – CAAQS) for PM2.5, the most harmful type of particulate for human health, is 28 µg/m^3 for the period 2015-2020. </v>
       </c>
       <c r="Q7" s="5" t="str">
         <f t="shared" si="1"/>
@@ -9847,7 +9850,7 @@
       <c r="S9" s="83"/>
       <c r="T9" s="10"/>
     </row>
-    <row r="10" spans="1:20" s="3" customFormat="1" ht="162.25" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:20" s="3" customFormat="1" ht="103.25" x14ac:dyDescent="0.75">
       <c r="A10" s="57" t="str">
         <f>A$9</f>
         <v>Transportation</v>
@@ -9917,7 +9920,7 @@
       <c r="S10" s="83"/>
       <c r="T10" s="10"/>
     </row>
-    <row r="11" spans="1:20" s="3" customFormat="1" ht="162.25" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:20" s="3" customFormat="1" ht="103.25" x14ac:dyDescent="0.75">
       <c r="A11" s="57" t="str">
         <f t="shared" ref="A11:A20" si="5">A$9</f>
         <v>Transportation</v>
@@ -9987,7 +9990,7 @@
       <c r="S11" s="83"/>
       <c r="T11" s="10"/>
     </row>
-    <row r="12" spans="1:20" s="3" customFormat="1" ht="162.25" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:20" s="3" customFormat="1" ht="103.25" x14ac:dyDescent="0.75">
       <c r="A12" s="57" t="str">
         <f t="shared" si="5"/>
         <v>Transportation</v>
@@ -10057,7 +10060,7 @@
       <c r="S12" s="83"/>
       <c r="T12" s="10"/>
     </row>
-    <row r="13" spans="1:20" s="3" customFormat="1" ht="162.25" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:20" s="3" customFormat="1" ht="103.25" x14ac:dyDescent="0.75">
       <c r="A13" s="57" t="str">
         <f t="shared" si="5"/>
         <v>Transportation</v>
@@ -10107,7 +10110,7 @@
       <c r="S13" s="83"/>
       <c r="T13" s="10"/>
     </row>
-    <row r="14" spans="1:20" s="3" customFormat="1" ht="162.25" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:20" s="3" customFormat="1" ht="103.25" x14ac:dyDescent="0.75">
       <c r="A14" s="57" t="str">
         <f t="shared" si="5"/>
         <v>Transportation</v>
@@ -10157,7 +10160,7 @@
       <c r="S14" s="83"/>
       <c r="T14" s="10"/>
     </row>
-    <row r="15" spans="1:20" s="3" customFormat="1" ht="162.25" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:20" s="3" customFormat="1" ht="103.25" x14ac:dyDescent="0.75">
       <c r="A15" s="57" t="str">
         <f t="shared" si="5"/>
         <v>Transportation</v>
@@ -10207,7 +10210,7 @@
       <c r="S15" s="83"/>
       <c r="T15" s="10"/>
     </row>
-    <row r="16" spans="1:20" s="3" customFormat="1" ht="162.25" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:20" s="3" customFormat="1" ht="103.25" x14ac:dyDescent="0.75">
       <c r="A16" s="57" t="str">
         <f t="shared" si="5"/>
         <v>Transportation</v>
@@ -10257,7 +10260,7 @@
       <c r="S16" s="83"/>
       <c r="T16" s="10"/>
     </row>
-    <row r="17" spans="1:20" s="3" customFormat="1" ht="162.25" x14ac:dyDescent="0.75">
+    <row r="17" spans="1:20" s="3" customFormat="1" ht="103.25" x14ac:dyDescent="0.75">
       <c r="A17" s="57" t="str">
         <f t="shared" si="5"/>
         <v>Transportation</v>
@@ -10307,7 +10310,7 @@
       <c r="S17" s="83"/>
       <c r="T17" s="10"/>
     </row>
-    <row r="18" spans="1:20" s="3" customFormat="1" ht="162.25" x14ac:dyDescent="0.75">
+    <row r="18" spans="1:20" s="3" customFormat="1" ht="103.25" x14ac:dyDescent="0.75">
       <c r="A18" s="57" t="str">
         <f t="shared" si="5"/>
         <v>Transportation</v>
@@ -10357,7 +10360,7 @@
       <c r="S18" s="83"/>
       <c r="T18" s="10"/>
     </row>
-    <row r="19" spans="1:20" s="3" customFormat="1" ht="162.25" x14ac:dyDescent="0.75">
+    <row r="19" spans="1:20" s="3" customFormat="1" ht="103.25" x14ac:dyDescent="0.75">
       <c r="A19" s="57" t="str">
         <f t="shared" si="5"/>
         <v>Transportation</v>
@@ -10427,7 +10430,7 @@
       <c r="S19" s="83"/>
       <c r="T19" s="10"/>
     </row>
-    <row r="20" spans="1:20" s="3" customFormat="1" ht="162.25" x14ac:dyDescent="0.75">
+    <row r="20" spans="1:20" s="3" customFormat="1" ht="103.25" x14ac:dyDescent="0.75">
       <c r="A20" s="57" t="str">
         <f t="shared" si="5"/>
         <v>Transportation</v>
@@ -31733,13 +31736,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A1" s="199" t="s">
+      <c r="A1" s="196" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="199"/>
-      <c r="C1" s="199"/>
-      <c r="D1" s="199"/>
-      <c r="E1" s="199"/>
+      <c r="B1" s="196"/>
+      <c r="C1" s="196"/>
+      <c r="D1" s="196"/>
+      <c r="E1" s="196"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A2" s="200" t="s">
@@ -31808,13 +31811,13 @@
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A60" s="199" t="s">
+      <c r="A60" s="196" t="s">
         <v>198</v>
       </c>
-      <c r="B60" s="199"/>
-      <c r="C60" s="199"/>
-      <c r="D60" s="199"/>
-      <c r="E60" s="199"/>
+      <c r="B60" s="196"/>
+      <c r="C60" s="196"/>
+      <c r="D60" s="196"/>
+      <c r="E60" s="196"/>
     </row>
     <row r="85" spans="1:39" s="12" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A85" s="9" t="s">
@@ -31919,13 +31922,13 @@
       </c>
     </row>
     <row r="89" spans="1:39" x14ac:dyDescent="0.75">
-      <c r="A89" s="199" t="s">
+      <c r="A89" s="196" t="s">
         <v>199</v>
       </c>
-      <c r="B89" s="199"/>
-      <c r="C89" s="199"/>
-      <c r="D89" s="199"/>
-      <c r="E89" s="199"/>
+      <c r="B89" s="196"/>
+      <c r="C89" s="196"/>
+      <c r="D89" s="196"/>
+      <c r="E89" s="196"/>
     </row>
     <row r="90" spans="1:39" x14ac:dyDescent="0.75">
       <c r="A90" s="9">
@@ -32012,13 +32015,13 @@
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A98" s="199" t="s">
+      <c r="A98" s="196" t="s">
         <v>200</v>
       </c>
-      <c r="B98" s="199"/>
-      <c r="C98" s="199"/>
-      <c r="D98" s="199"/>
-      <c r="E98" s="199"/>
+      <c r="B98" s="196"/>
+      <c r="C98" s="196"/>
+      <c r="D98" s="196"/>
+      <c r="E98" s="196"/>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A99" s="17">
@@ -32102,13 +32105,13 @@
       <c r="A108" s="20"/>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A109" s="199" t="s">
+      <c r="A109" s="196" t="s">
         <v>202</v>
       </c>
-      <c r="B109" s="199"/>
-      <c r="C109" s="199"/>
-      <c r="D109" s="199"/>
-      <c r="E109" s="199"/>
+      <c r="B109" s="196"/>
+      <c r="C109" s="196"/>
+      <c r="D109" s="196"/>
+      <c r="E109" s="196"/>
     </row>
     <row r="110" spans="1:5" ht="15.5" thickBot="1" x14ac:dyDescent="0.9"/>
     <row r="111" spans="1:5" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
@@ -32121,13 +32124,13 @@
       </c>
     </row>
     <row r="113" spans="1:14" x14ac:dyDescent="0.75">
-      <c r="A113" s="199" t="s">
+      <c r="A113" s="196" t="s">
         <v>201</v>
       </c>
-      <c r="B113" s="199"/>
-      <c r="C113" s="199"/>
-      <c r="D113" s="199"/>
-      <c r="E113" s="199"/>
+      <c r="B113" s="196"/>
+      <c r="C113" s="196"/>
+      <c r="D113" s="196"/>
+      <c r="E113" s="196"/>
     </row>
     <row r="114" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A114" s="17">
@@ -32208,13 +32211,13 @@
       </c>
     </row>
     <row r="124" spans="1:14" x14ac:dyDescent="0.75">
-      <c r="A124" s="199" t="s">
+      <c r="A124" s="196" t="s">
         <v>482</v>
       </c>
-      <c r="B124" s="199"/>
-      <c r="C124" s="199"/>
-      <c r="D124" s="199"/>
-      <c r="E124" s="199"/>
+      <c r="B124" s="196"/>
+      <c r="C124" s="196"/>
+      <c r="D124" s="196"/>
+      <c r="E124" s="196"/>
       <c r="L124" s="21"/>
     </row>
     <row r="125" spans="1:14" x14ac:dyDescent="0.75">
@@ -32305,13 +32308,13 @@
       <c r="C133" s="15"/>
     </row>
     <row r="134" spans="1:14" x14ac:dyDescent="0.75">
-      <c r="A134" s="199" t="s">
+      <c r="A134" s="196" t="s">
         <v>115</v>
       </c>
-      <c r="B134" s="199"/>
-      <c r="C134" s="199"/>
-      <c r="D134" s="199"/>
-      <c r="E134" s="199"/>
+      <c r="B134" s="196"/>
+      <c r="C134" s="196"/>
+      <c r="D134" s="196"/>
+      <c r="E134" s="196"/>
     </row>
     <row r="135" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A135" s="27" t="s">
@@ -32326,25 +32329,25 @@
     </row>
     <row r="136" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A136" s="29"/>
-      <c r="B136" s="196" t="s">
+      <c r="B136" s="197" t="s">
         <v>502</v>
       </c>
-      <c r="C136" s="197"/>
-      <c r="D136" s="197"/>
-      <c r="E136" s="198"/>
+      <c r="C136" s="198"/>
+      <c r="D136" s="198"/>
+      <c r="E136" s="199"/>
       <c r="F136" s="28"/>
       <c r="G136" s="28"/>
     </row>
     <row r="137" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A137" s="30"/>
-      <c r="B137" s="196" t="s">
+      <c r="B137" s="197" t="s">
         <v>503</v>
       </c>
-      <c r="C137" s="198"/>
-      <c r="D137" s="196" t="s">
+      <c r="C137" s="199"/>
+      <c r="D137" s="197" t="s">
         <v>504</v>
       </c>
-      <c r="E137" s="198"/>
+      <c r="E137" s="199"/>
       <c r="F137" s="28"/>
       <c r="G137" s="28"/>
     </row>
@@ -32891,13 +32894,13 @@
       <c r="G163" s="28"/>
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A165" s="199" t="s">
+      <c r="A165" s="196" t="s">
         <v>205</v>
       </c>
-      <c r="B165" s="199"/>
-      <c r="C165" s="199"/>
-      <c r="D165" s="199"/>
-      <c r="E165" s="199"/>
+      <c r="B165" s="196"/>
+      <c r="C165" s="196"/>
+      <c r="D165" s="196"/>
+      <c r="E165" s="196"/>
     </row>
     <row r="166" spans="1:7" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
       <c r="A166" s="23" t="s">
@@ -32920,10 +32923,10 @@
       <c r="B168" s="46"/>
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A169" s="199" t="s">
+      <c r="A169" s="196" t="s">
         <v>490</v>
       </c>
-      <c r="B169" s="199"/>
+      <c r="B169" s="196"/>
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A170" s="23" t="s">
@@ -32955,13 +32958,13 @@
       <c r="B173" s="46"/>
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A174" s="199" t="s">
+      <c r="A174" s="196" t="s">
         <v>215</v>
       </c>
-      <c r="B174" s="199"/>
-      <c r="C174" s="199"/>
-      <c r="D174" s="199"/>
-      <c r="E174" s="199"/>
+      <c r="B174" s="196"/>
+      <c r="C174" s="196"/>
+      <c r="D174" s="196"/>
+      <c r="E174" s="196"/>
     </row>
     <row r="175" spans="1:7" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
       <c r="A175" s="23" t="s">
@@ -32981,13 +32984,13 @@
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A178" s="199" t="s">
+      <c r="A178" s="196" t="s">
         <v>208</v>
       </c>
-      <c r="B178" s="199"/>
-      <c r="C178" s="199"/>
-      <c r="D178" s="199"/>
-      <c r="E178" s="199"/>
+      <c r="B178" s="196"/>
+      <c r="C178" s="196"/>
+      <c r="D178" s="196"/>
+      <c r="E178" s="196"/>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A179" s="25" t="s">
@@ -33015,13 +33018,13 @@
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A183" s="199" t="s">
+      <c r="A183" s="196" t="s">
         <v>210</v>
       </c>
-      <c r="B183" s="199"/>
-      <c r="C183" s="199"/>
-      <c r="D183" s="199"/>
-      <c r="E183" s="199"/>
+      <c r="B183" s="196"/>
+      <c r="C183" s="196"/>
+      <c r="D183" s="196"/>
+      <c r="E183" s="196"/>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A184" s="23" t="s">
@@ -33076,13 +33079,13 @@
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A191" s="199" t="s">
+      <c r="A191" s="196" t="s">
         <v>227</v>
       </c>
-      <c r="B191" s="199"/>
-      <c r="C191" s="199"/>
-      <c r="D191" s="199"/>
-      <c r="E191" s="199"/>
+      <c r="B191" s="196"/>
+      <c r="C191" s="196"/>
+      <c r="D191" s="196"/>
+      <c r="E191" s="196"/>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A192" s="21" t="s">
@@ -33142,12 +33145,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A191:E191"/>
-    <mergeCell ref="A165:E165"/>
-    <mergeCell ref="A178:E178"/>
-    <mergeCell ref="A183:E183"/>
-    <mergeCell ref="A174:E174"/>
-    <mergeCell ref="A169:B169"/>
     <mergeCell ref="B136:E136"/>
     <mergeCell ref="B137:C137"/>
     <mergeCell ref="D137:E137"/>
@@ -33162,6 +33159,12 @@
     <mergeCell ref="A113:E113"/>
     <mergeCell ref="A109:E109"/>
     <mergeCell ref="A124:E124"/>
+    <mergeCell ref="A191:E191"/>
+    <mergeCell ref="A165:E165"/>
+    <mergeCell ref="A178:E178"/>
+    <mergeCell ref="A183:E183"/>
+    <mergeCell ref="A174:E174"/>
+    <mergeCell ref="A169:B169"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
Updates to carbon tax policy description in WebAppData
</commit_message>
<xml_diff>
--- a/WebAppData.xlsx
+++ b/WebAppData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swenzel\Dropbox (Energy Innovation)\My PC (energy044)\Documents\GitHub_Repositories\eps-alberta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{712EF7AE-778F-43A3-B971-2CBEAA7AEE95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9255780-8773-4AFB-8CEE-8049CEAB5B84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12600" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12600" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="10" r:id="rId1"/>
@@ -4047,9 +4047,6 @@
     <t>**Description:** This policy reduces the subsidies paid for the production of the selected energy source(s) in the BAU case. // **Guidance for setting values:** A value of 100% eliminates subsidies, increasing the price of coal by 8% (varying by sector), natural gas by 3-8% (varying by sector), petroleum gasoline by 1%, petroleum diesel by 2% (varying by sector) in 2050, and jet fuel by 2% (varying by sector) in 2050.</t>
   </si>
   <si>
-    <t>**Description:** This policy applies a price on fuels used in the selected sector(s) based on their greenhouse gas emissions.  It also increases the base cost of capital equipment (e.g., vehicles, power plants, building components) according to their embedded carbon content. When applied to the Industry Sector, the tax **is** levied on greenhouse gas emissions from non-energy industrial and agricultural processes by default, but these emissions sources can be exempted from the tax by enabling the policy lever "Exempt Process Emissions from C Tax." // **Guidance for setting values:** The Canadian government's revised 2016 Social Cost of Carbon estimates for the year 2050 range from CAD$75 in the central estimate to CAD$320 per ton in the 95th percnetile estimate (in inflation-adjusted 2012 Canadian dollars).</t>
-  </si>
-  <si>
     <t>**Description:** This policy reduces fuel consumption by the selected industry by increasing the efficiency of industrial equipment through stronger standards.  The policy setting refers to overall energy use reduction, not the reduction in energy use of newly sold equipment. // **Guidance for setting values:** In 2016, the U.S. Department of Energy developed an industrial energy efficiency potential analysis that suggests a potential improvement rate of 2.4% per year through 2030, instead of a BAU rate of 1.2% per year.  Extended through 2050, this equates to a maximum potential improvement of 33% by 2050 relative to BAU.  The same potential may exist in Alberta.</t>
   </si>
   <si>
@@ -4120,6 +4117,9 @@
   </si>
   <si>
     <t xml:space="preserve">**Description:** This policy represents strengthening standards for the selected pollutant(s) emitted by the selected vehicle type(s).  Conventional pollutants' most important, harmful impacts are on human health rather than on climate change. // **Guidance for setting values:** In Canada, the 24-hour national ambient air quality standard (Canadian Ambient Air Quality Standards – CAAQS) for PM2.5, the most harmful type of particulate for human health, is 28 µg/m^3 for the period 2015-2020. </t>
+  </si>
+  <si>
+    <t>**Description:** This policy applies a tax on fuels used in the selected sector(s) based on their greenhouse gas emissions.  It also increases the base cost of capital equipment (e.g., vehicles, power plants, building components) according to their embedded carbon content. // **Guidance for setting values:** The Canadian government's revised 2016 Social Cost of Carbon estimates for the year 2050 range from CAD$75 in the central estimate to CAD$320 per ton in the 95th percnetile estimate (in inflation-adjusted 2012 Canadian dollars).</t>
   </si>
 </sst>
 </file>
@@ -4821,7 +4821,7 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="201">
+  <cellXfs count="202">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -5340,9 +5340,6 @@
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -5352,8 +5349,14 @@
     <xf numFmtId="0" fontId="13" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="56">
@@ -6419,7 +6422,7 @@
   </sheetPr>
   <dimension ref="A1:N105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="J59" sqref="J59"/>
     </sheetView>
   </sheetViews>
@@ -6441,7 +6444,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A1" s="190" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
       <c r="B1" s="188"/>
       <c r="C1" s="188"/>
@@ -6459,7 +6462,7 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A2" s="189" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
       <c r="B2" s="188"/>
       <c r="C2" s="188"/>
@@ -6548,7 +6551,7 @@
         <v>1023</v>
       </c>
       <c r="J4" s="169" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
       <c r="K4" s="75" t="s">
         <v>1024</v>
@@ -6624,7 +6627,7 @@
         <v>579</v>
       </c>
       <c r="J6" s="169" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
       <c r="K6" s="75" t="s">
         <v>580</v>
@@ -6662,7 +6665,7 @@
         <v>567</v>
       </c>
       <c r="J7" s="169" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
       <c r="K7" s="75" t="s">
         <v>568</v>
@@ -6700,7 +6703,7 @@
         <v>547</v>
       </c>
       <c r="J8" s="169" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="K8" s="169" t="s">
         <v>234</v>
@@ -6744,7 +6747,7 @@
         <v>127</v>
       </c>
       <c r="J9" s="169" t="s">
-        <v>1209</v>
+        <v>1208</v>
       </c>
       <c r="K9" s="169" t="s">
         <v>236</v>
@@ -6822,7 +6825,7 @@
         <v>44</v>
       </c>
       <c r="J11" s="169" t="s">
-        <v>1208</v>
+        <v>1207</v>
       </c>
       <c r="K11" s="169" t="s">
         <v>238</v>
@@ -6863,7 +6866,7 @@
         <v>129</v>
       </c>
       <c r="J12" s="169" t="s">
-        <v>1207</v>
+        <v>1206</v>
       </c>
       <c r="K12" s="169" t="s">
         <v>240</v>
@@ -6901,7 +6904,7 @@
         <v>38</v>
       </c>
       <c r="J13" s="169" t="s">
-        <v>1206</v>
+        <v>1205</v>
       </c>
       <c r="K13" s="169" t="s">
         <v>242</v>
@@ -7105,7 +7108,7 @@
         <v>43</v>
       </c>
       <c r="J18" s="169" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
       <c r="K18" s="169" t="s">
         <v>248</v>
@@ -7149,7 +7152,7 @@
         <v>35</v>
       </c>
       <c r="J19" s="169" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
       <c r="K19" s="169" t="s">
         <v>250</v>
@@ -7187,7 +7190,7 @@
         <v>35</v>
       </c>
       <c r="J20" s="169" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
       <c r="K20" s="169" t="s">
         <v>414</v>
@@ -7225,7 +7228,7 @@
         <v>330</v>
       </c>
       <c r="J21" s="169" t="s">
-        <v>1202</v>
+        <v>1201</v>
       </c>
       <c r="K21" s="169" t="s">
         <v>332</v>
@@ -7265,7 +7268,7 @@
         <v>331</v>
       </c>
       <c r="J22" s="169" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
       <c r="K22" s="169" t="s">
         <v>333</v>
@@ -7373,7 +7376,7 @@
         <v>230</v>
       </c>
       <c r="J25" s="169" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
       <c r="K25" s="169" t="s">
         <v>254</v>
@@ -7417,7 +7420,7 @@
         <v>36</v>
       </c>
       <c r="J26" s="169" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="K26" s="169" t="s">
         <v>256</v>
@@ -7503,7 +7506,7 @@
         <v>35</v>
       </c>
       <c r="J28" s="169" t="s">
-        <v>1198</v>
+        <v>1197</v>
       </c>
       <c r="K28" s="175"/>
       <c r="L28" s="168"/>
@@ -7607,7 +7610,7 @@
         <v>313</v>
       </c>
       <c r="J31" s="169" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
       <c r="K31" s="168" t="s">
         <v>612</v>
@@ -7647,7 +7650,7 @@
         <v>815</v>
       </c>
       <c r="J32" s="169" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
       <c r="K32" s="168" t="s">
         <v>946</v>
@@ -7702,13 +7705,13 @@
         <v>8</v>
       </c>
       <c r="B34" s="169" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
       <c r="C34" s="169" t="s">
         <v>368</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
       <c r="E34" s="4" t="s">
         <v>678</v>
@@ -7726,7 +7729,7 @@
         <v>42</v>
       </c>
       <c r="J34" s="169" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
       <c r="K34" s="169" t="s">
         <v>261</v>
@@ -7763,7 +7766,7 @@
         <v>967</v>
       </c>
       <c r="J35" s="169" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
       <c r="K35" s="169" t="s">
         <v>263</v>
@@ -7928,7 +7931,7 @@
         <v>38</v>
       </c>
       <c r="J39" s="169" t="s">
-        <v>1192</v>
+        <v>1191</v>
       </c>
       <c r="K39" s="169" t="s">
         <v>271</v>
@@ -8703,7 +8706,7 @@
       </c>
       <c r="N58" s="169"/>
     </row>
-    <row r="59" spans="1:14" ht="70.5" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="59" spans="1:14" ht="56.25" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A59" s="169" t="s">
         <v>10</v>
       </c>
@@ -8731,8 +8734,8 @@
       <c r="I59" s="169" t="s">
         <v>981</v>
       </c>
-      <c r="J59" s="169" t="s">
-        <v>1191</v>
+      <c r="J59" s="201" t="s">
+        <v>1215</v>
       </c>
       <c r="K59" s="169" t="s">
         <v>295</v>
@@ -9274,9 +9277,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:T327"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P2" sqref="P2"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A299" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E279" sqref="E279"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -9284,7 +9287,7 @@
     <col min="1" max="2" width="20.1796875" style="4" customWidth="1"/>
     <col min="3" max="3" width="20.1796875" style="2" customWidth="1"/>
     <col min="4" max="7" width="10.1796875" style="4" customWidth="1"/>
-    <col min="8" max="8" width="10.1796875" style="52" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="10.1796875" style="52" customWidth="1"/>
     <col min="9" max="9" width="10.1796875" style="4" customWidth="1"/>
     <col min="10" max="10" width="20.1796875" style="52" customWidth="1"/>
     <col min="11" max="11" width="20.1796875" style="78" customWidth="1"/>
@@ -9361,7 +9364,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="2" spans="1:20" s="3" customFormat="1" ht="88.5" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:20" s="3" customFormat="1" ht="73.75" x14ac:dyDescent="0.75">
       <c r="A2" s="101" t="s">
         <v>4</v>
       </c>
@@ -9415,7 +9418,7 @@
       </c>
       <c r="S2" s="150"/>
     </row>
-    <row r="3" spans="1:20" s="3" customFormat="1" ht="88.5" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:20" s="3" customFormat="1" ht="73.75" x14ac:dyDescent="0.75">
       <c r="A3" s="193" t="str">
         <f>A$2</f>
         <v>Transportation</v>
@@ -9480,7 +9483,7 @@
       </c>
       <c r="S3" s="150"/>
     </row>
-    <row r="4" spans="1:20" s="3" customFormat="1" ht="88.5" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:20" s="3" customFormat="1" ht="73.75" x14ac:dyDescent="0.75">
       <c r="A4" s="193" t="str">
         <f t="shared" ref="A4:A7" si="2">A$2</f>
         <v>Transportation</v>
@@ -9545,7 +9548,7 @@
       </c>
       <c r="S4" s="150"/>
     </row>
-    <row r="5" spans="1:20" s="3" customFormat="1" ht="88.5" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:20" s="3" customFormat="1" ht="73.75" x14ac:dyDescent="0.75">
       <c r="A5" s="193" t="str">
         <f t="shared" si="2"/>
         <v>Transportation</v>
@@ -9610,7 +9613,7 @@
       </c>
       <c r="S5" s="150"/>
     </row>
-    <row r="6" spans="1:20" s="3" customFormat="1" ht="88.5" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:20" s="3" customFormat="1" ht="73.75" x14ac:dyDescent="0.75">
       <c r="A6" s="193" t="str">
         <f t="shared" si="2"/>
         <v>Transportation</v>
@@ -9675,7 +9678,7 @@
       </c>
       <c r="S6" s="150"/>
     </row>
-    <row r="7" spans="1:20" s="3" customFormat="1" ht="88.5" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:20" s="3" customFormat="1" ht="73.75" x14ac:dyDescent="0.75">
       <c r="A7" s="193" t="str">
         <f t="shared" si="2"/>
         <v>Transportation</v>
@@ -21917,7 +21920,7 @@
       </c>
       <c r="P225" s="195" t="str">
         <f>INDEX('Policy Characteristics'!J:J,MATCH($C225,'Policy Characteristics'!$C:$C,0))</f>
-        <v>**Description:** This policy applies a price on fuels used in the selected sector(s) based on their greenhouse gas emissions.  It also increases the base cost of capital equipment (e.g., vehicles, power plants, building components) according to their embedded carbon content. When applied to the Industry Sector, the tax **is** levied on greenhouse gas emissions from non-energy industrial and agricultural processes by default, but these emissions sources can be exempted from the tax by enabling the policy lever "Exempt Process Emissions from C Tax." // **Guidance for setting values:** The Canadian government's revised 2016 Social Cost of Carbon estimates for the year 2050 range from CAD$75 in the central estimate to CAD$320 per ton in the 95th percnetile estimate (in inflation-adjusted 2012 Canadian dollars).</v>
+        <v>**Description:** This policy applies a tax on fuels used in the selected sector(s) based on their greenhouse gas emissions.  It also increases the base cost of capital equipment (e.g., vehicles, power plants, building components) according to their embedded carbon content. // **Guidance for setting values:** The Canadian government's revised 2016 Social Cost of Carbon estimates for the year 2050 range from CAD$75 in the central estimate to CAD$320 per ton in the 95th percnetile estimate (in inflation-adjusted 2012 Canadian dollars).</v>
       </c>
       <c r="Q225" s="55" t="s">
         <v>295</v>
@@ -21985,7 +21988,7 @@
       </c>
       <c r="P226" s="195" t="str">
         <f>INDEX('Policy Characteristics'!J:J,MATCH($C226,'Policy Characteristics'!$C:$C,0))</f>
-        <v>**Description:** This policy applies a price on fuels used in the selected sector(s) based on their greenhouse gas emissions.  It also increases the base cost of capital equipment (e.g., vehicles, power plants, building components) according to their embedded carbon content. When applied to the Industry Sector, the tax **is** levied on greenhouse gas emissions from non-energy industrial and agricultural processes by default, but these emissions sources can be exempted from the tax by enabling the policy lever "Exempt Process Emissions from C Tax." // **Guidance for setting values:** The Canadian government's revised 2016 Social Cost of Carbon estimates for the year 2050 range from CAD$75 in the central estimate to CAD$320 per ton in the 95th percnetile estimate (in inflation-adjusted 2012 Canadian dollars).</v>
+        <v>**Description:** This policy applies a tax on fuels used in the selected sector(s) based on their greenhouse gas emissions.  It also increases the base cost of capital equipment (e.g., vehicles, power plants, building components) according to their embedded carbon content. // **Guidance for setting values:** The Canadian government's revised 2016 Social Cost of Carbon estimates for the year 2050 range from CAD$75 in the central estimate to CAD$320 per ton in the 95th percnetile estimate (in inflation-adjusted 2012 Canadian dollars).</v>
       </c>
       <c r="Q226" s="57" t="str">
         <f t="shared" ref="Q226:R229" si="47">Q$225</f>
@@ -22051,7 +22054,7 @@
       </c>
       <c r="P227" s="195" t="str">
         <f>INDEX('Policy Characteristics'!J:J,MATCH($C227,'Policy Characteristics'!$C:$C,0))</f>
-        <v>**Description:** This policy applies a price on fuels used in the selected sector(s) based on their greenhouse gas emissions.  It also increases the base cost of capital equipment (e.g., vehicles, power plants, building components) according to their embedded carbon content. When applied to the Industry Sector, the tax **is** levied on greenhouse gas emissions from non-energy industrial and agricultural processes by default, but these emissions sources can be exempted from the tax by enabling the policy lever "Exempt Process Emissions from C Tax." // **Guidance for setting values:** The Canadian government's revised 2016 Social Cost of Carbon estimates for the year 2050 range from CAD$75 in the central estimate to CAD$320 per ton in the 95th percnetile estimate (in inflation-adjusted 2012 Canadian dollars).</v>
+        <v>**Description:** This policy applies a tax on fuels used in the selected sector(s) based on their greenhouse gas emissions.  It also increases the base cost of capital equipment (e.g., vehicles, power plants, building components) according to their embedded carbon content. // **Guidance for setting values:** The Canadian government's revised 2016 Social Cost of Carbon estimates for the year 2050 range from CAD$75 in the central estimate to CAD$320 per ton in the 95th percnetile estimate (in inflation-adjusted 2012 Canadian dollars).</v>
       </c>
       <c r="Q227" s="57" t="str">
         <f t="shared" si="47"/>
@@ -22117,7 +22120,7 @@
       </c>
       <c r="P228" s="195" t="str">
         <f>INDEX('Policy Characteristics'!J:J,MATCH($C228,'Policy Characteristics'!$C:$C,0))</f>
-        <v>**Description:** This policy applies a price on fuels used in the selected sector(s) based on their greenhouse gas emissions.  It also increases the base cost of capital equipment (e.g., vehicles, power plants, building components) according to their embedded carbon content. When applied to the Industry Sector, the tax **is** levied on greenhouse gas emissions from non-energy industrial and agricultural processes by default, but these emissions sources can be exempted from the tax by enabling the policy lever "Exempt Process Emissions from C Tax." // **Guidance for setting values:** The Canadian government's revised 2016 Social Cost of Carbon estimates for the year 2050 range from CAD$75 in the central estimate to CAD$320 per ton in the 95th percnetile estimate (in inflation-adjusted 2012 Canadian dollars).</v>
+        <v>**Description:** This policy applies a tax on fuels used in the selected sector(s) based on their greenhouse gas emissions.  It also increases the base cost of capital equipment (e.g., vehicles, power plants, building components) according to their embedded carbon content. // **Guidance for setting values:** The Canadian government's revised 2016 Social Cost of Carbon estimates for the year 2050 range from CAD$75 in the central estimate to CAD$320 per ton in the 95th percnetile estimate (in inflation-adjusted 2012 Canadian dollars).</v>
       </c>
       <c r="Q228" s="57" t="str">
         <f t="shared" si="47"/>
@@ -22183,7 +22186,7 @@
       </c>
       <c r="P229" s="195" t="str">
         <f>INDEX('Policy Characteristics'!J:J,MATCH($C229,'Policy Characteristics'!$C:$C,0))</f>
-        <v>**Description:** This policy applies a price on fuels used in the selected sector(s) based on their greenhouse gas emissions.  It also increases the base cost of capital equipment (e.g., vehicles, power plants, building components) according to their embedded carbon content. When applied to the Industry Sector, the tax **is** levied on greenhouse gas emissions from non-energy industrial and agricultural processes by default, but these emissions sources can be exempted from the tax by enabling the policy lever "Exempt Process Emissions from C Tax." // **Guidance for setting values:** The Canadian government's revised 2016 Social Cost of Carbon estimates for the year 2050 range from CAD$75 in the central estimate to CAD$320 per ton in the 95th percnetile estimate (in inflation-adjusted 2012 Canadian dollars).</v>
+        <v>**Description:** This policy applies a tax on fuels used in the selected sector(s) based on their greenhouse gas emissions.  It also increases the base cost of capital equipment (e.g., vehicles, power plants, building components) according to their embedded carbon content. // **Guidance for setting values:** The Canadian government's revised 2016 Social Cost of Carbon estimates for the year 2050 range from CAD$75 in the central estimate to CAD$320 per ton in the 95th percnetile estimate (in inflation-adjusted 2012 Canadian dollars).</v>
       </c>
       <c r="Q229" s="57" t="str">
         <f t="shared" si="47"/>
@@ -22235,7 +22238,7 @@
       <c r="O230" s="55"/>
       <c r="P230" s="195" t="str">
         <f>INDEX('Policy Characteristics'!J:J,MATCH($C230,'Policy Characteristics'!$C:$C,0))</f>
-        <v>**Description:** This policy applies a price on fuels used in the selected sector(s) based on their greenhouse gas emissions.  It also increases the base cost of capital equipment (e.g., vehicles, power plants, building components) according to their embedded carbon content. When applied to the Industry Sector, the tax **is** levied on greenhouse gas emissions from non-energy industrial and agricultural processes by default, but these emissions sources can be exempted from the tax by enabling the policy lever "Exempt Process Emissions from C Tax." // **Guidance for setting values:** The Canadian government's revised 2016 Social Cost of Carbon estimates for the year 2050 range from CAD$75 in the central estimate to CAD$320 per ton in the 95th percnetile estimate (in inflation-adjusted 2012 Canadian dollars).</v>
+        <v>**Description:** This policy applies a tax on fuels used in the selected sector(s) based on their greenhouse gas emissions.  It also increases the base cost of capital equipment (e.g., vehicles, power plants, building components) according to their embedded carbon content. // **Guidance for setting values:** The Canadian government's revised 2016 Social Cost of Carbon estimates for the year 2050 range from CAD$75 in the central estimate to CAD$320 per ton in the 95th percnetile estimate (in inflation-adjusted 2012 Canadian dollars).</v>
       </c>
       <c r="Q230" s="55"/>
       <c r="R230" s="10"/>
@@ -22281,7 +22284,7 @@
       <c r="O231" s="55"/>
       <c r="P231" s="195" t="str">
         <f>INDEX('Policy Characteristics'!J:J,MATCH($C231,'Policy Characteristics'!$C:$C,0))</f>
-        <v>**Description:** This policy applies a price on fuels used in the selected sector(s) based on their greenhouse gas emissions.  It also increases the base cost of capital equipment (e.g., vehicles, power plants, building components) according to their embedded carbon content. When applied to the Industry Sector, the tax **is** levied on greenhouse gas emissions from non-energy industrial and agricultural processes by default, but these emissions sources can be exempted from the tax by enabling the policy lever "Exempt Process Emissions from C Tax." // **Guidance for setting values:** The Canadian government's revised 2016 Social Cost of Carbon estimates for the year 2050 range from CAD$75 in the central estimate to CAD$320 per ton in the 95th percnetile estimate (in inflation-adjusted 2012 Canadian dollars).</v>
+        <v>**Description:** This policy applies a tax on fuels used in the selected sector(s) based on their greenhouse gas emissions.  It also increases the base cost of capital equipment (e.g., vehicles, power plants, building components) according to their embedded carbon content. // **Guidance for setting values:** The Canadian government's revised 2016 Social Cost of Carbon estimates for the year 2050 range from CAD$75 in the central estimate to CAD$320 per ton in the 95th percnetile estimate (in inflation-adjusted 2012 Canadian dollars).</v>
       </c>
       <c r="Q231" s="55"/>
       <c r="R231" s="10"/>
@@ -31736,13 +31739,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A1" s="196" t="s">
+      <c r="A1" s="199" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="196"/>
-      <c r="C1" s="196"/>
-      <c r="D1" s="196"/>
-      <c r="E1" s="196"/>
+      <c r="B1" s="199"/>
+      <c r="C1" s="199"/>
+      <c r="D1" s="199"/>
+      <c r="E1" s="199"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A2" s="200" t="s">
@@ -31811,13 +31814,13 @@
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A60" s="196" t="s">
+      <c r="A60" s="199" t="s">
         <v>198</v>
       </c>
-      <c r="B60" s="196"/>
-      <c r="C60" s="196"/>
-      <c r="D60" s="196"/>
-      <c r="E60" s="196"/>
+      <c r="B60" s="199"/>
+      <c r="C60" s="199"/>
+      <c r="D60" s="199"/>
+      <c r="E60" s="199"/>
     </row>
     <row r="85" spans="1:39" s="12" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A85" s="9" t="s">
@@ -31922,13 +31925,13 @@
       </c>
     </row>
     <row r="89" spans="1:39" x14ac:dyDescent="0.75">
-      <c r="A89" s="196" t="s">
+      <c r="A89" s="199" t="s">
         <v>199</v>
       </c>
-      <c r="B89" s="196"/>
-      <c r="C89" s="196"/>
-      <c r="D89" s="196"/>
-      <c r="E89" s="196"/>
+      <c r="B89" s="199"/>
+      <c r="C89" s="199"/>
+      <c r="D89" s="199"/>
+      <c r="E89" s="199"/>
     </row>
     <row r="90" spans="1:39" x14ac:dyDescent="0.75">
       <c r="A90" s="9">
@@ -32015,13 +32018,13 @@
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A98" s="196" t="s">
+      <c r="A98" s="199" t="s">
         <v>200</v>
       </c>
-      <c r="B98" s="196"/>
-      <c r="C98" s="196"/>
-      <c r="D98" s="196"/>
-      <c r="E98" s="196"/>
+      <c r="B98" s="199"/>
+      <c r="C98" s="199"/>
+      <c r="D98" s="199"/>
+      <c r="E98" s="199"/>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A99" s="17">
@@ -32105,13 +32108,13 @@
       <c r="A108" s="20"/>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A109" s="196" t="s">
+      <c r="A109" s="199" t="s">
         <v>202</v>
       </c>
-      <c r="B109" s="196"/>
-      <c r="C109" s="196"/>
-      <c r="D109" s="196"/>
-      <c r="E109" s="196"/>
+      <c r="B109" s="199"/>
+      <c r="C109" s="199"/>
+      <c r="D109" s="199"/>
+      <c r="E109" s="199"/>
     </row>
     <row r="110" spans="1:5" ht="15.5" thickBot="1" x14ac:dyDescent="0.9"/>
     <row r="111" spans="1:5" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
@@ -32124,13 +32127,13 @@
       </c>
     </row>
     <row r="113" spans="1:14" x14ac:dyDescent="0.75">
-      <c r="A113" s="196" t="s">
+      <c r="A113" s="199" t="s">
         <v>201</v>
       </c>
-      <c r="B113" s="196"/>
-      <c r="C113" s="196"/>
-      <c r="D113" s="196"/>
-      <c r="E113" s="196"/>
+      <c r="B113" s="199"/>
+      <c r="C113" s="199"/>
+      <c r="D113" s="199"/>
+      <c r="E113" s="199"/>
     </row>
     <row r="114" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A114" s="17">
@@ -32211,13 +32214,13 @@
       </c>
     </row>
     <row r="124" spans="1:14" x14ac:dyDescent="0.75">
-      <c r="A124" s="196" t="s">
+      <c r="A124" s="199" t="s">
         <v>482</v>
       </c>
-      <c r="B124" s="196"/>
-      <c r="C124" s="196"/>
-      <c r="D124" s="196"/>
-      <c r="E124" s="196"/>
+      <c r="B124" s="199"/>
+      <c r="C124" s="199"/>
+      <c r="D124" s="199"/>
+      <c r="E124" s="199"/>
       <c r="L124" s="21"/>
     </row>
     <row r="125" spans="1:14" x14ac:dyDescent="0.75">
@@ -32308,13 +32311,13 @@
       <c r="C133" s="15"/>
     </row>
     <row r="134" spans="1:14" x14ac:dyDescent="0.75">
-      <c r="A134" s="196" t="s">
+      <c r="A134" s="199" t="s">
         <v>115</v>
       </c>
-      <c r="B134" s="196"/>
-      <c r="C134" s="196"/>
-      <c r="D134" s="196"/>
-      <c r="E134" s="196"/>
+      <c r="B134" s="199"/>
+      <c r="C134" s="199"/>
+      <c r="D134" s="199"/>
+      <c r="E134" s="199"/>
     </row>
     <row r="135" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A135" s="27" t="s">
@@ -32329,25 +32332,25 @@
     </row>
     <row r="136" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A136" s="29"/>
-      <c r="B136" s="197" t="s">
+      <c r="B136" s="196" t="s">
         <v>502</v>
       </c>
-      <c r="C136" s="198"/>
-      <c r="D136" s="198"/>
-      <c r="E136" s="199"/>
+      <c r="C136" s="197"/>
+      <c r="D136" s="197"/>
+      <c r="E136" s="198"/>
       <c r="F136" s="28"/>
       <c r="G136" s="28"/>
     </row>
     <row r="137" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A137" s="30"/>
-      <c r="B137" s="197" t="s">
+      <c r="B137" s="196" t="s">
         <v>503</v>
       </c>
-      <c r="C137" s="199"/>
-      <c r="D137" s="197" t="s">
+      <c r="C137" s="198"/>
+      <c r="D137" s="196" t="s">
         <v>504</v>
       </c>
-      <c r="E137" s="199"/>
+      <c r="E137" s="198"/>
       <c r="F137" s="28"/>
       <c r="G137" s="28"/>
     </row>
@@ -32894,13 +32897,13 @@
       <c r="G163" s="28"/>
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A165" s="196" t="s">
+      <c r="A165" s="199" t="s">
         <v>205</v>
       </c>
-      <c r="B165" s="196"/>
-      <c r="C165" s="196"/>
-      <c r="D165" s="196"/>
-      <c r="E165" s="196"/>
+      <c r="B165" s="199"/>
+      <c r="C165" s="199"/>
+      <c r="D165" s="199"/>
+      <c r="E165" s="199"/>
     </row>
     <row r="166" spans="1:7" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
       <c r="A166" s="23" t="s">
@@ -32923,10 +32926,10 @@
       <c r="B168" s="46"/>
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A169" s="196" t="s">
+      <c r="A169" s="199" t="s">
         <v>490</v>
       </c>
-      <c r="B169" s="196"/>
+      <c r="B169" s="199"/>
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A170" s="23" t="s">
@@ -32958,13 +32961,13 @@
       <c r="B173" s="46"/>
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A174" s="196" t="s">
+      <c r="A174" s="199" t="s">
         <v>215</v>
       </c>
-      <c r="B174" s="196"/>
-      <c r="C174" s="196"/>
-      <c r="D174" s="196"/>
-      <c r="E174" s="196"/>
+      <c r="B174" s="199"/>
+      <c r="C174" s="199"/>
+      <c r="D174" s="199"/>
+      <c r="E174" s="199"/>
     </row>
     <row r="175" spans="1:7" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
       <c r="A175" s="23" t="s">
@@ -32984,13 +32987,13 @@
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A178" s="196" t="s">
+      <c r="A178" s="199" t="s">
         <v>208</v>
       </c>
-      <c r="B178" s="196"/>
-      <c r="C178" s="196"/>
-      <c r="D178" s="196"/>
-      <c r="E178" s="196"/>
+      <c r="B178" s="199"/>
+      <c r="C178" s="199"/>
+      <c r="D178" s="199"/>
+      <c r="E178" s="199"/>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A179" s="25" t="s">
@@ -33018,13 +33021,13 @@
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A183" s="196" t="s">
+      <c r="A183" s="199" t="s">
         <v>210</v>
       </c>
-      <c r="B183" s="196"/>
-      <c r="C183" s="196"/>
-      <c r="D183" s="196"/>
-      <c r="E183" s="196"/>
+      <c r="B183" s="199"/>
+      <c r="C183" s="199"/>
+      <c r="D183" s="199"/>
+      <c r="E183" s="199"/>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A184" s="23" t="s">
@@ -33079,13 +33082,13 @@
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A191" s="196" t="s">
+      <c r="A191" s="199" t="s">
         <v>227</v>
       </c>
-      <c r="B191" s="196"/>
-      <c r="C191" s="196"/>
-      <c r="D191" s="196"/>
-      <c r="E191" s="196"/>
+      <c r="B191" s="199"/>
+      <c r="C191" s="199"/>
+      <c r="D191" s="199"/>
+      <c r="E191" s="199"/>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A192" s="21" t="s">
@@ -33145,6 +33148,12 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A191:E191"/>
+    <mergeCell ref="A165:E165"/>
+    <mergeCell ref="A178:E178"/>
+    <mergeCell ref="A183:E183"/>
+    <mergeCell ref="A174:E174"/>
+    <mergeCell ref="A169:B169"/>
     <mergeCell ref="B136:E136"/>
     <mergeCell ref="B137:C137"/>
     <mergeCell ref="D137:E137"/>
@@ -33159,12 +33168,6 @@
     <mergeCell ref="A113:E113"/>
     <mergeCell ref="A109:E109"/>
     <mergeCell ref="A124:E124"/>
-    <mergeCell ref="A191:E191"/>
-    <mergeCell ref="A165:E165"/>
-    <mergeCell ref="A178:E178"/>
-    <mergeCell ref="A183:E183"/>
-    <mergeCell ref="A174:E174"/>
-    <mergeCell ref="A169:B169"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
Updates made to WebAppData descriptions
</commit_message>
<xml_diff>
--- a/WebAppData.xlsx
+++ b/WebAppData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swenzel\Dropbox (Energy Innovation)\My PC (energy044)\Documents\GitHub_Repositories\eps-alberta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9255780-8773-4AFB-8CEE-8049CEAB5B84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30249D53-227C-43BF-AA60-9E34A29740FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12600" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12600" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="824" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="10" r:id="rId1"/>
@@ -257,7 +257,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5446" uniqueCount="1216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5446" uniqueCount="1215">
   <si>
     <t>Short Name</t>
   </si>
@@ -4074,21 +4074,12 @@
     <t>**Description:** This policy causes the specified quantity of otherwise non-retiring capacity of the selected type(s) to be retired each year. // **Guidance for setting values:** // **Hard Coal:** The BAU scenario projects roughly 5.4 GW of coal retirements through 2050, most of it by 2029.  0.9 GW remain in 2050. // **Nuclear:** The BAU scenario projects rougly 6 GW of cogeneration retirements through 2050, all of it by 2022.  9 GW remain in 2050.</t>
   </si>
   <si>
-    <t>**Description:** This policy increases or decreases the amount of electricity imported to Canada from the United States.  It does not cause the construction or removal of transmission lines linking these countries. // **Guidance for setting values:** From 2017-2050, in the BAU case, electricity imports are expected to remain stable.</t>
-  </si>
-  <si>
-    <t>**Description:** This policy increases or decreases the amount of electricity exported from Canada to the United States.  It does not cause the construction or removal of transmission lines linking these countries. // **Guidance for setting values:** From 2017-2050, in the BAU case, electricity exports are expected to remain stable.</t>
-  </si>
-  <si>
     <t>**Description:** This policy prevents new capacity of the selected type(s) from being built or deployed.</t>
   </si>
   <si>
     <t>**Description:** This policy represents a modest rebate paid to customers who purchase energy-efficient building equipment of the selected type(s).  Typical rebate amounts represented by this policy are $50-100 for a clothes washer and $25-50 for a dishwasher or refrigerator.</t>
   </si>
   <si>
-    <t>**Description:** Each year, the specified percentage of the selected building type(s) that existed at the start of the model run will be retrofit with more efficient heating, cooling, and envelope components. // **Guidance for setting values:** // **Heating:** Heating systems have a normal lifespan of 19 years, so without this retrofitting policy, 5.3% of these systems retire annually.  Setting this policy to 1% will decrease the average lifespan of heating systems to 16 years. // **Cooling and Ventilation:** Cooling and ventilation systems have a normal lifespan of 16 years, so without this retrofitting policy, 6.3% of these systems retire annually.  Setting this policy to 1% will decrease the average lifespan of cooling and ventilation systems to 14 years. // **Envelope:** Envelope components have a normal lifespan of 52 years, so without this retrofitting policy, 1.9% of these systems retire annually.  Setting this policy to 1% will decrease the average lifespan of envelope components to 34 years. // **Lighting:** Lighting components have a normal lifespan of 9 years, so without this retrofitting policy, 11.1% of these systems retire annually.  Setting this policy to 1% will decrease the average lifespan of lighting components to 8 years. // **Appliances:** Appliances have a normal lifespan of 14 years, so without this retrofitting policy, 7.1% of these systems retire annually.  Setting this policy to 1% will decrease the average lifespan of appliances to 12 years. // **Other Components:** Other energy-using components have a normal lifespan of 15 years, so without this retrofitting policy, 6.7% of these systems retire annually.  Setting this policy to 1% will decrease the average lifespan of other energy-using components to 13 years.</t>
-  </si>
-  <si>
     <t>**Description:** This policy tightens energy efficiency standards for the selected component(s) in the selected building type(s).  The policy only applies to newly sold components each year (whether for new buildings or replacement of old components of existing buildings). // **Guidance for setting values:** In "Assessment of Electricity Savings in the U.S. Achievable through New Appliance/Equipment Efficiency Standards and Building Efficiency Codes, 2010-2025" (2011), the Edison Foundation considered a 30% reduction in whole-building energy use (moderate case) and 40-45% (aggressive case) relative to BAU from 2010 to 2025.  Similar potentials may be possible in Alberta, with further improvement post-2025.</t>
   </si>
   <si>
@@ -4120,6 +4111,12 @@
   </si>
   <si>
     <t>**Description:** This policy applies a tax on fuels used in the selected sector(s) based on their greenhouse gas emissions.  It also increases the base cost of capital equipment (e.g., vehicles, power plants, building components) according to their embedded carbon content. // **Guidance for setting values:** The Canadian government's revised 2016 Social Cost of Carbon estimates for the year 2050 range from CAD$75 in the central estimate to CAD$320 per ton in the 95th percnetile estimate (in inflation-adjusted 2012 Canadian dollars).</t>
+  </si>
+  <si>
+    <t>**Description:** Each year, the specified percentage of the selected building type(s) that existed at the start of the model run will be retrofit with more efficient heating, cooling, and envelope components.  This is in addtion to the retirement and replacement of these systems that have lived out their lifetimes.  The systems replaced by this policy are assumed to have an efficiency equal to that of the average deployed system and 33% of their useful lives remaining. // **Guidance for setting values:** // **Heating:** Heating systems have a normal lifespan of 19 years, so without this retrofitting policy, 5.3% of these systems retire annually.  Setting this policy to 1% will decrease the average lifespan of heating systems to 16 years. // **Cooling and Ventilation:** Cooling and ventilation systems have a normal lifespan of 16 years, so without this retrofitting policy, 6.3% of these systems retire annually.  Setting this policy to 1% will decrease the average lifespan of cooling and ventilation systems to 14 years. // **Envelope:** Envelope components have a normal lifespan of 52 years, so without this retrofitting policy, 1.9% of these systems retire annually.  Setting this policy to 1% will decrease the average lifespan of envelope components to 34 years. // **Lighting:** Lighting components have a normal lifespan of 9 years, so without this retrofitting policy, 11.1% of these systems retire annually.  Setting this policy to 1% will decrease the average lifespan of lighting components to 8 years. // **Appliances:** Appliances have a normal lifespan of 14 years, so without this retrofitting policy, 7.1% of these systems retire annually.  Setting this policy to 1% will decrease the average lifespan of appliances to 12 years. // **Other Components:** Other energy-using components have a normal lifespan of 15 years, so without this retrofitting policy, 6.7% of these systems retire annually.  Setting this policy to 1% will decrease the average lifespan of other energy-using components to 13 years.</t>
+  </si>
+  <si>
+    <t>**Description:** This policy increases or decreases the amount of electricity exported from Alberta to the United States.  It does not cause the construction or removal of transmission lines linking these jurisdictions. // **Guidance for setting values:** From 2017-2050, in the BAU case, electricity imports are expected to remain stable.</t>
   </si>
 </sst>
 </file>
@@ -5340,6 +5337,9 @@
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -5354,9 +5354,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="56">
@@ -6422,20 +6419,21 @@
   </sheetPr>
   <dimension ref="A1:N105"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J59" sqref="J59"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5:K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="1" max="1" width="13.54296875" style="97" customWidth="1"/>
     <col min="2" max="2" width="18.2265625" style="97" customWidth="1"/>
-    <col min="3" max="5" width="20.1796875" style="97" customWidth="1"/>
-    <col min="6" max="6" width="8.54296875" style="97" customWidth="1"/>
-    <col min="7" max="7" width="8.81640625" style="97" customWidth="1"/>
-    <col min="8" max="8" width="8.6328125" style="97" customWidth="1"/>
-    <col min="9" max="9" width="12.26953125" style="97" customWidth="1"/>
-    <col min="10" max="10" width="153.26953125" style="97" customWidth="1"/>
+    <col min="3" max="3" width="20.1796875" style="97" customWidth="1"/>
+    <col min="4" max="5" width="20.1796875" style="97" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="8.54296875" style="97" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="8.81640625" style="97" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="8.6328125" style="97" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="12.26953125" style="97" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="99.6796875" style="97" customWidth="1"/>
     <col min="11" max="12" width="20.1796875" style="97" customWidth="1"/>
     <col min="13" max="13" width="129.26953125" style="97" customWidth="1"/>
     <col min="14" max="14" width="67.54296875" style="97" customWidth="1"/>
@@ -6444,7 +6442,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A1" s="190" t="s">
-        <v>1212</v>
+        <v>1209</v>
       </c>
       <c r="B1" s="188"/>
       <c r="C1" s="188"/>
@@ -6462,7 +6460,7 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A2" s="189" t="s">
-        <v>1211</v>
+        <v>1208</v>
       </c>
       <c r="B2" s="188"/>
       <c r="C2" s="188"/>
@@ -6522,7 +6520,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="44.4" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:14" ht="114.75" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
@@ -6551,7 +6549,7 @@
         <v>1023</v>
       </c>
       <c r="J4" s="169" t="s">
-        <v>1214</v>
+        <v>1211</v>
       </c>
       <c r="K4" s="75" t="s">
         <v>1024</v>
@@ -6560,7 +6558,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="44.4" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:14" ht="142.5" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A5" s="168" t="s">
         <v>4</v>
       </c>
@@ -6627,7 +6625,7 @@
         <v>579</v>
       </c>
       <c r="J6" s="169" t="s">
-        <v>1213</v>
+        <v>1210</v>
       </c>
       <c r="K6" s="75" t="s">
         <v>580</v>
@@ -6665,7 +6663,7 @@
         <v>567</v>
       </c>
       <c r="J7" s="169" t="s">
-        <v>1210</v>
+        <v>1207</v>
       </c>
       <c r="K7" s="75" t="s">
         <v>568</v>
@@ -6703,7 +6701,7 @@
         <v>547</v>
       </c>
       <c r="J8" s="169" t="s">
-        <v>1209</v>
+        <v>1206</v>
       </c>
       <c r="K8" s="169" t="s">
         <v>234</v>
@@ -6718,7 +6716,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="169.25" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:14" ht="278" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A9" s="169" t="s">
         <v>4</v>
       </c>
@@ -6747,7 +6745,7 @@
         <v>127</v>
       </c>
       <c r="J9" s="169" t="s">
-        <v>1208</v>
+        <v>1205</v>
       </c>
       <c r="K9" s="169" t="s">
         <v>236</v>
@@ -6825,7 +6823,7 @@
         <v>44</v>
       </c>
       <c r="J11" s="169" t="s">
-        <v>1207</v>
+        <v>1204</v>
       </c>
       <c r="K11" s="169" t="s">
         <v>238</v>
@@ -6866,7 +6864,7 @@
         <v>129</v>
       </c>
       <c r="J12" s="169" t="s">
-        <v>1206</v>
+        <v>1203</v>
       </c>
       <c r="K12" s="169" t="s">
         <v>240</v>
@@ -6904,7 +6902,7 @@
         <v>38</v>
       </c>
       <c r="J13" s="169" t="s">
-        <v>1205</v>
+        <v>1202</v>
       </c>
       <c r="K13" s="169" t="s">
         <v>242</v>
@@ -7108,7 +7106,7 @@
         <v>43</v>
       </c>
       <c r="J18" s="169" t="s">
-        <v>1204</v>
+        <v>1213</v>
       </c>
       <c r="K18" s="169" t="s">
         <v>248</v>
@@ -7152,7 +7150,7 @@
         <v>35</v>
       </c>
       <c r="J19" s="169" t="s">
-        <v>1203</v>
+        <v>1201</v>
       </c>
       <c r="K19" s="169" t="s">
         <v>250</v>
@@ -7190,7 +7188,7 @@
         <v>35</v>
       </c>
       <c r="J20" s="169" t="s">
-        <v>1202</v>
+        <v>1200</v>
       </c>
       <c r="K20" s="169" t="s">
         <v>414</v>
@@ -7228,7 +7226,7 @@
         <v>330</v>
       </c>
       <c r="J21" s="169" t="s">
-        <v>1201</v>
+        <v>1088</v>
       </c>
       <c r="K21" s="169" t="s">
         <v>332</v>
@@ -7268,7 +7266,7 @@
         <v>331</v>
       </c>
       <c r="J22" s="169" t="s">
-        <v>1200</v>
+        <v>1214</v>
       </c>
       <c r="K22" s="169" t="s">
         <v>333</v>
@@ -7704,8 +7702,8 @@
       <c r="A34" s="169" t="s">
         <v>8</v>
       </c>
-      <c r="B34" s="169" t="s">
-        <v>1194</v>
+      <c r="B34" s="55" t="s">
+        <v>18</v>
       </c>
       <c r="C34" s="169" t="s">
         <v>368</v>
@@ -8734,8 +8732,8 @@
       <c r="I59" s="169" t="s">
         <v>981</v>
       </c>
-      <c r="J59" s="201" t="s">
-        <v>1215</v>
+      <c r="J59" s="196" t="s">
+        <v>1212</v>
       </c>
       <c r="K59" s="169" t="s">
         <v>295</v>
@@ -9277,9 +9275,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:T327"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A299" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E279" sqref="E279"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A182" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B183" sqref="B183"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -15117,7 +15115,7 @@
       </c>
       <c r="P98" s="195" t="str">
         <f>INDEX('Policy Characteristics'!J:J,MATCH($C98,'Policy Characteristics'!$C:$C,0))</f>
-        <v>**Description:** Each year, the specified percentage of the selected building type(s) that existed at the start of the model run will be retrofit with more efficient heating, cooling, and envelope components. // **Guidance for setting values:** // **Heating:** Heating systems have a normal lifespan of 19 years, so without this retrofitting policy, 5.3% of these systems retire annually.  Setting this policy to 1% will decrease the average lifespan of heating systems to 16 years. // **Cooling and Ventilation:** Cooling and ventilation systems have a normal lifespan of 16 years, so without this retrofitting policy, 6.3% of these systems retire annually.  Setting this policy to 1% will decrease the average lifespan of cooling and ventilation systems to 14 years. // **Envelope:** Envelope components have a normal lifespan of 52 years, so without this retrofitting policy, 1.9% of these systems retire annually.  Setting this policy to 1% will decrease the average lifespan of envelope components to 34 years. // **Lighting:** Lighting components have a normal lifespan of 9 years, so without this retrofitting policy, 11.1% of these systems retire annually.  Setting this policy to 1% will decrease the average lifespan of lighting components to 8 years. // **Appliances:** Appliances have a normal lifespan of 14 years, so without this retrofitting policy, 7.1% of these systems retire annually.  Setting this policy to 1% will decrease the average lifespan of appliances to 12 years. // **Other Components:** Other energy-using components have a normal lifespan of 15 years, so without this retrofitting policy, 6.7% of these systems retire annually.  Setting this policy to 1% will decrease the average lifespan of other energy-using components to 13 years.</v>
+        <v>**Description:** Each year, the specified percentage of the selected building type(s) that existed at the start of the model run will be retrofit with more efficient heating, cooling, and envelope components.  This is in addtion to the retirement and replacement of these systems that have lived out their lifetimes.  The systems replaced by this policy are assumed to have an efficiency equal to that of the average deployed system and 33% of their useful lives remaining. // **Guidance for setting values:** // **Heating:** Heating systems have a normal lifespan of 19 years, so without this retrofitting policy, 5.3% of these systems retire annually.  Setting this policy to 1% will decrease the average lifespan of heating systems to 16 years. // **Cooling and Ventilation:** Cooling and ventilation systems have a normal lifespan of 16 years, so without this retrofitting policy, 6.3% of these systems retire annually.  Setting this policy to 1% will decrease the average lifespan of cooling and ventilation systems to 14 years. // **Envelope:** Envelope components have a normal lifespan of 52 years, so without this retrofitting policy, 1.9% of these systems retire annually.  Setting this policy to 1% will decrease the average lifespan of envelope components to 34 years. // **Lighting:** Lighting components have a normal lifespan of 9 years, so without this retrofitting policy, 11.1% of these systems retire annually.  Setting this policy to 1% will decrease the average lifespan of lighting components to 8 years. // **Appliances:** Appliances have a normal lifespan of 14 years, so without this retrofitting policy, 7.1% of these systems retire annually.  Setting this policy to 1% will decrease the average lifespan of appliances to 12 years. // **Other Components:** Other energy-using components have a normal lifespan of 15 years, so without this retrofitting policy, 6.7% of these systems retire annually.  Setting this policy to 1% will decrease the average lifespan of other energy-using components to 13 years.</v>
       </c>
       <c r="Q98" s="55" t="s">
         <v>248</v>
@@ -15185,7 +15183,7 @@
       </c>
       <c r="P99" s="195" t="str">
         <f>INDEX('Policy Characteristics'!J:J,MATCH($C99,'Policy Characteristics'!$C:$C,0))</f>
-        <v>**Description:** Each year, the specified percentage of the selected building type(s) that existed at the start of the model run will be retrofit with more efficient heating, cooling, and envelope components. // **Guidance for setting values:** // **Heating:** Heating systems have a normal lifespan of 19 years, so without this retrofitting policy, 5.3% of these systems retire annually.  Setting this policy to 1% will decrease the average lifespan of heating systems to 16 years. // **Cooling and Ventilation:** Cooling and ventilation systems have a normal lifespan of 16 years, so without this retrofitting policy, 6.3% of these systems retire annually.  Setting this policy to 1% will decrease the average lifespan of cooling and ventilation systems to 14 years. // **Envelope:** Envelope components have a normal lifespan of 52 years, so without this retrofitting policy, 1.9% of these systems retire annually.  Setting this policy to 1% will decrease the average lifespan of envelope components to 34 years. // **Lighting:** Lighting components have a normal lifespan of 9 years, so without this retrofitting policy, 11.1% of these systems retire annually.  Setting this policy to 1% will decrease the average lifespan of lighting components to 8 years. // **Appliances:** Appliances have a normal lifespan of 14 years, so without this retrofitting policy, 7.1% of these systems retire annually.  Setting this policy to 1% will decrease the average lifespan of appliances to 12 years. // **Other Components:** Other energy-using components have a normal lifespan of 15 years, so without this retrofitting policy, 6.7% of these systems retire annually.  Setting this policy to 1% will decrease the average lifespan of other energy-using components to 13 years.</v>
+        <v>**Description:** Each year, the specified percentage of the selected building type(s) that existed at the start of the model run will be retrofit with more efficient heating, cooling, and envelope components.  This is in addtion to the retirement and replacement of these systems that have lived out their lifetimes.  The systems replaced by this policy are assumed to have an efficiency equal to that of the average deployed system and 33% of their useful lives remaining. // **Guidance for setting values:** // **Heating:** Heating systems have a normal lifespan of 19 years, so without this retrofitting policy, 5.3% of these systems retire annually.  Setting this policy to 1% will decrease the average lifespan of heating systems to 16 years. // **Cooling and Ventilation:** Cooling and ventilation systems have a normal lifespan of 16 years, so without this retrofitting policy, 6.3% of these systems retire annually.  Setting this policy to 1% will decrease the average lifespan of cooling and ventilation systems to 14 years. // **Envelope:** Envelope components have a normal lifespan of 52 years, so without this retrofitting policy, 1.9% of these systems retire annually.  Setting this policy to 1% will decrease the average lifespan of envelope components to 34 years. // **Lighting:** Lighting components have a normal lifespan of 9 years, so without this retrofitting policy, 11.1% of these systems retire annually.  Setting this policy to 1% will decrease the average lifespan of lighting components to 8 years. // **Appliances:** Appliances have a normal lifespan of 14 years, so without this retrofitting policy, 7.1% of these systems retire annually.  Setting this policy to 1% will decrease the average lifespan of appliances to 12 years. // **Other Components:** Other energy-using components have a normal lifespan of 15 years, so without this retrofitting policy, 6.7% of these systems retire annually.  Setting this policy to 1% will decrease the average lifespan of other energy-using components to 13 years.</v>
       </c>
       <c r="Q99" s="55" t="s">
         <v>248</v>
@@ -15252,7 +15250,7 @@
       </c>
       <c r="P100" s="195" t="str">
         <f>INDEX('Policy Characteristics'!J:J,MATCH($C100,'Policy Characteristics'!$C:$C,0))</f>
-        <v>**Description:** Each year, the specified percentage of the selected building type(s) that existed at the start of the model run will be retrofit with more efficient heating, cooling, and envelope components. // **Guidance for setting values:** // **Heating:** Heating systems have a normal lifespan of 19 years, so without this retrofitting policy, 5.3% of these systems retire annually.  Setting this policy to 1% will decrease the average lifespan of heating systems to 16 years. // **Cooling and Ventilation:** Cooling and ventilation systems have a normal lifespan of 16 years, so without this retrofitting policy, 6.3% of these systems retire annually.  Setting this policy to 1% will decrease the average lifespan of cooling and ventilation systems to 14 years. // **Envelope:** Envelope components have a normal lifespan of 52 years, so without this retrofitting policy, 1.9% of these systems retire annually.  Setting this policy to 1% will decrease the average lifespan of envelope components to 34 years. // **Lighting:** Lighting components have a normal lifespan of 9 years, so without this retrofitting policy, 11.1% of these systems retire annually.  Setting this policy to 1% will decrease the average lifespan of lighting components to 8 years. // **Appliances:** Appliances have a normal lifespan of 14 years, so without this retrofitting policy, 7.1% of these systems retire annually.  Setting this policy to 1% will decrease the average lifespan of appliances to 12 years. // **Other Components:** Other energy-using components have a normal lifespan of 15 years, so without this retrofitting policy, 6.7% of these systems retire annually.  Setting this policy to 1% will decrease the average lifespan of other energy-using components to 13 years.</v>
+        <v>**Description:** Each year, the specified percentage of the selected building type(s) that existed at the start of the model run will be retrofit with more efficient heating, cooling, and envelope components.  This is in addtion to the retirement and replacement of these systems that have lived out their lifetimes.  The systems replaced by this policy are assumed to have an efficiency equal to that of the average deployed system and 33% of their useful lives remaining. // **Guidance for setting values:** // **Heating:** Heating systems have a normal lifespan of 19 years, so without this retrofitting policy, 5.3% of these systems retire annually.  Setting this policy to 1% will decrease the average lifespan of heating systems to 16 years. // **Cooling and Ventilation:** Cooling and ventilation systems have a normal lifespan of 16 years, so without this retrofitting policy, 6.3% of these systems retire annually.  Setting this policy to 1% will decrease the average lifespan of cooling and ventilation systems to 14 years. // **Envelope:** Envelope components have a normal lifespan of 52 years, so without this retrofitting policy, 1.9% of these systems retire annually.  Setting this policy to 1% will decrease the average lifespan of envelope components to 34 years. // **Lighting:** Lighting components have a normal lifespan of 9 years, so without this retrofitting policy, 11.1% of these systems retire annually.  Setting this policy to 1% will decrease the average lifespan of lighting components to 8 years. // **Appliances:** Appliances have a normal lifespan of 14 years, so without this retrofitting policy, 7.1% of these systems retire annually.  Setting this policy to 1% will decrease the average lifespan of appliances to 12 years. // **Other Components:** Other energy-using components have a normal lifespan of 15 years, so without this retrofitting policy, 6.7% of these systems retire annually.  Setting this policy to 1% will decrease the average lifespan of other energy-using components to 13 years.</v>
       </c>
       <c r="Q100" s="55" t="s">
         <v>248</v>
@@ -15319,7 +15317,7 @@
       </c>
       <c r="P101" s="195" t="str">
         <f>INDEX('Policy Characteristics'!J:J,MATCH($C101,'Policy Characteristics'!$C:$C,0))</f>
-        <v>**Description:** Each year, the specified percentage of the selected building type(s) that existed at the start of the model run will be retrofit with more efficient heating, cooling, and envelope components. // **Guidance for setting values:** // **Heating:** Heating systems have a normal lifespan of 19 years, so without this retrofitting policy, 5.3% of these systems retire annually.  Setting this policy to 1% will decrease the average lifespan of heating systems to 16 years. // **Cooling and Ventilation:** Cooling and ventilation systems have a normal lifespan of 16 years, so without this retrofitting policy, 6.3% of these systems retire annually.  Setting this policy to 1% will decrease the average lifespan of cooling and ventilation systems to 14 years. // **Envelope:** Envelope components have a normal lifespan of 52 years, so without this retrofitting policy, 1.9% of these systems retire annually.  Setting this policy to 1% will decrease the average lifespan of envelope components to 34 years. // **Lighting:** Lighting components have a normal lifespan of 9 years, so without this retrofitting policy, 11.1% of these systems retire annually.  Setting this policy to 1% will decrease the average lifespan of lighting components to 8 years. // **Appliances:** Appliances have a normal lifespan of 14 years, so without this retrofitting policy, 7.1% of these systems retire annually.  Setting this policy to 1% will decrease the average lifespan of appliances to 12 years. // **Other Components:** Other energy-using components have a normal lifespan of 15 years, so without this retrofitting policy, 6.7% of these systems retire annually.  Setting this policy to 1% will decrease the average lifespan of other energy-using components to 13 years.</v>
+        <v>**Description:** Each year, the specified percentage of the selected building type(s) that existed at the start of the model run will be retrofit with more efficient heating, cooling, and envelope components.  This is in addtion to the retirement and replacement of these systems that have lived out their lifetimes.  The systems replaced by this policy are assumed to have an efficiency equal to that of the average deployed system and 33% of their useful lives remaining. // **Guidance for setting values:** // **Heating:** Heating systems have a normal lifespan of 19 years, so without this retrofitting policy, 5.3% of these systems retire annually.  Setting this policy to 1% will decrease the average lifespan of heating systems to 16 years. // **Cooling and Ventilation:** Cooling and ventilation systems have a normal lifespan of 16 years, so without this retrofitting policy, 6.3% of these systems retire annually.  Setting this policy to 1% will decrease the average lifespan of cooling and ventilation systems to 14 years. // **Envelope:** Envelope components have a normal lifespan of 52 years, so without this retrofitting policy, 1.9% of these systems retire annually.  Setting this policy to 1% will decrease the average lifespan of envelope components to 34 years. // **Lighting:** Lighting components have a normal lifespan of 9 years, so without this retrofitting policy, 11.1% of these systems retire annually.  Setting this policy to 1% will decrease the average lifespan of lighting components to 8 years. // **Appliances:** Appliances have a normal lifespan of 14 years, so without this retrofitting policy, 7.1% of these systems retire annually.  Setting this policy to 1% will decrease the average lifespan of appliances to 12 years. // **Other Components:** Other energy-using components have a normal lifespan of 15 years, so without this retrofitting policy, 6.7% of these systems retire annually.  Setting this policy to 1% will decrease the average lifespan of other energy-using components to 13 years.</v>
       </c>
       <c r="Q101" s="55" t="s">
         <v>248</v>
@@ -15386,7 +15384,7 @@
       </c>
       <c r="P102" s="195" t="str">
         <f>INDEX('Policy Characteristics'!J:J,MATCH($C102,'Policy Characteristics'!$C:$C,0))</f>
-        <v>**Description:** Each year, the specified percentage of the selected building type(s) that existed at the start of the model run will be retrofit with more efficient heating, cooling, and envelope components. // **Guidance for setting values:** // **Heating:** Heating systems have a normal lifespan of 19 years, so without this retrofitting policy, 5.3% of these systems retire annually.  Setting this policy to 1% will decrease the average lifespan of heating systems to 16 years. // **Cooling and Ventilation:** Cooling and ventilation systems have a normal lifespan of 16 years, so without this retrofitting policy, 6.3% of these systems retire annually.  Setting this policy to 1% will decrease the average lifespan of cooling and ventilation systems to 14 years. // **Envelope:** Envelope components have a normal lifespan of 52 years, so without this retrofitting policy, 1.9% of these systems retire annually.  Setting this policy to 1% will decrease the average lifespan of envelope components to 34 years. // **Lighting:** Lighting components have a normal lifespan of 9 years, so without this retrofitting policy, 11.1% of these systems retire annually.  Setting this policy to 1% will decrease the average lifespan of lighting components to 8 years. // **Appliances:** Appliances have a normal lifespan of 14 years, so without this retrofitting policy, 7.1% of these systems retire annually.  Setting this policy to 1% will decrease the average lifespan of appliances to 12 years. // **Other Components:** Other energy-using components have a normal lifespan of 15 years, so without this retrofitting policy, 6.7% of these systems retire annually.  Setting this policy to 1% will decrease the average lifespan of other energy-using components to 13 years.</v>
+        <v>**Description:** Each year, the specified percentage of the selected building type(s) that existed at the start of the model run will be retrofit with more efficient heating, cooling, and envelope components.  This is in addtion to the retirement and replacement of these systems that have lived out their lifetimes.  The systems replaced by this policy are assumed to have an efficiency equal to that of the average deployed system and 33% of their useful lives remaining. // **Guidance for setting values:** // **Heating:** Heating systems have a normal lifespan of 19 years, so without this retrofitting policy, 5.3% of these systems retire annually.  Setting this policy to 1% will decrease the average lifespan of heating systems to 16 years. // **Cooling and Ventilation:** Cooling and ventilation systems have a normal lifespan of 16 years, so without this retrofitting policy, 6.3% of these systems retire annually.  Setting this policy to 1% will decrease the average lifespan of cooling and ventilation systems to 14 years. // **Envelope:** Envelope components have a normal lifespan of 52 years, so without this retrofitting policy, 1.9% of these systems retire annually.  Setting this policy to 1% will decrease the average lifespan of envelope components to 34 years. // **Lighting:** Lighting components have a normal lifespan of 9 years, so without this retrofitting policy, 11.1% of these systems retire annually.  Setting this policy to 1% will decrease the average lifespan of lighting components to 8 years. // **Appliances:** Appliances have a normal lifespan of 14 years, so without this retrofitting policy, 7.1% of these systems retire annually.  Setting this policy to 1% will decrease the average lifespan of appliances to 12 years. // **Other Components:** Other energy-using components have a normal lifespan of 15 years, so without this retrofitting policy, 6.7% of these systems retire annually.  Setting this policy to 1% will decrease the average lifespan of other energy-using components to 13 years.</v>
       </c>
       <c r="Q102" s="55" t="s">
         <v>248</v>
@@ -15453,7 +15451,7 @@
       </c>
       <c r="P103" s="195" t="str">
         <f>INDEX('Policy Characteristics'!J:J,MATCH($C103,'Policy Characteristics'!$C:$C,0))</f>
-        <v>**Description:** Each year, the specified percentage of the selected building type(s) that existed at the start of the model run will be retrofit with more efficient heating, cooling, and envelope components. // **Guidance for setting values:** // **Heating:** Heating systems have a normal lifespan of 19 years, so without this retrofitting policy, 5.3% of these systems retire annually.  Setting this policy to 1% will decrease the average lifespan of heating systems to 16 years. // **Cooling and Ventilation:** Cooling and ventilation systems have a normal lifespan of 16 years, so without this retrofitting policy, 6.3% of these systems retire annually.  Setting this policy to 1% will decrease the average lifespan of cooling and ventilation systems to 14 years. // **Envelope:** Envelope components have a normal lifespan of 52 years, so without this retrofitting policy, 1.9% of these systems retire annually.  Setting this policy to 1% will decrease the average lifespan of envelope components to 34 years. // **Lighting:** Lighting components have a normal lifespan of 9 years, so without this retrofitting policy, 11.1% of these systems retire annually.  Setting this policy to 1% will decrease the average lifespan of lighting components to 8 years. // **Appliances:** Appliances have a normal lifespan of 14 years, so without this retrofitting policy, 7.1% of these systems retire annually.  Setting this policy to 1% will decrease the average lifespan of appliances to 12 years. // **Other Components:** Other energy-using components have a normal lifespan of 15 years, so without this retrofitting policy, 6.7% of these systems retire annually.  Setting this policy to 1% will decrease the average lifespan of other energy-using components to 13 years.</v>
+        <v>**Description:** Each year, the specified percentage of the selected building type(s) that existed at the start of the model run will be retrofit with more efficient heating, cooling, and envelope components.  This is in addtion to the retirement and replacement of these systems that have lived out their lifetimes.  The systems replaced by this policy are assumed to have an efficiency equal to that of the average deployed system and 33% of their useful lives remaining. // **Guidance for setting values:** // **Heating:** Heating systems have a normal lifespan of 19 years, so without this retrofitting policy, 5.3% of these systems retire annually.  Setting this policy to 1% will decrease the average lifespan of heating systems to 16 years. // **Cooling and Ventilation:** Cooling and ventilation systems have a normal lifespan of 16 years, so without this retrofitting policy, 6.3% of these systems retire annually.  Setting this policy to 1% will decrease the average lifespan of cooling and ventilation systems to 14 years. // **Envelope:** Envelope components have a normal lifespan of 52 years, so without this retrofitting policy, 1.9% of these systems retire annually.  Setting this policy to 1% will decrease the average lifespan of envelope components to 34 years. // **Lighting:** Lighting components have a normal lifespan of 9 years, so without this retrofitting policy, 11.1% of these systems retire annually.  Setting this policy to 1% will decrease the average lifespan of lighting components to 8 years. // **Appliances:** Appliances have a normal lifespan of 14 years, so without this retrofitting policy, 7.1% of these systems retire annually.  Setting this policy to 1% will decrease the average lifespan of appliances to 12 years. // **Other Components:** Other energy-using components have a normal lifespan of 15 years, so without this retrofitting policy, 6.7% of these systems retire annually.  Setting this policy to 1% will decrease the average lifespan of other energy-using components to 13 years.</v>
       </c>
       <c r="Q103" s="55" t="s">
         <v>248</v>
@@ -16524,7 +16522,7 @@
       </c>
       <c r="P122" s="195" t="str">
         <f>INDEX('Policy Characteristics'!J:J,MATCH($C122,'Policy Characteristics'!$C:$C,0))</f>
-        <v>**Description:** This policy increases or decreases the amount of electricity exported from Canada to the United States.  It does not cause the construction or removal of transmission lines linking these countries. // **Guidance for setting values:** From 2017-2050, in the BAU case, electricity exports are expected to remain stable.</v>
+        <v>**Description:** This policy increases or decreases the amount of electricity exported from Alberta to the United States.  It does not cause the construction or removal of transmission lines linking these jurisdictions. // **Guidance for setting values:** From 2017-2050, in the BAU case, electricity exports are expected to remain stable.</v>
       </c>
       <c r="Q122" s="55" t="s">
         <v>332</v>
@@ -16575,7 +16573,7 @@
       </c>
       <c r="P123" s="195" t="str">
         <f>INDEX('Policy Characteristics'!J:J,MATCH($C123,'Policy Characteristics'!$C:$C,0))</f>
-        <v>**Description:** This policy increases or decreases the amount of electricity imported to Canada from the United States.  It does not cause the construction or removal of transmission lines linking these countries. // **Guidance for setting values:** From 2017-2050, in the BAU case, electricity imports are expected to remain stable.</v>
+        <v>**Description:** This policy increases or decreases the amount of electricity exported from Alberta to the United States.  It does not cause the construction or removal of transmission lines linking these jurisdictions. // **Guidance for setting values:** From 2017-2050, in the BAU case, electricity imports are expected to remain stable.</v>
       </c>
       <c r="Q123" s="55" t="s">
         <v>333</v>
@@ -22199,7 +22197,7 @@
       <c r="S229" s="86"/>
       <c r="T229" s="57"/>
     </row>
-    <row r="230" spans="1:20" s="5" customFormat="1" ht="132.75" x14ac:dyDescent="0.75">
+    <row r="230" spans="1:20" s="5" customFormat="1" ht="88.5" x14ac:dyDescent="0.75">
       <c r="A230" s="57" t="str">
         <f t="shared" si="48"/>
         <v>Cross-Sector</v>
@@ -22245,7 +22243,7 @@
       <c r="S230" s="86"/>
       <c r="T230" s="57"/>
     </row>
-    <row r="231" spans="1:20" s="5" customFormat="1" ht="132.75" x14ac:dyDescent="0.75">
+    <row r="231" spans="1:20" s="5" customFormat="1" ht="88.5" x14ac:dyDescent="0.75">
       <c r="A231" s="57" t="str">
         <f t="shared" si="48"/>
         <v>Cross-Sector</v>
@@ -31739,22 +31737,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A1" s="199" t="s">
+      <c r="A1" s="200" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="199"/>
-      <c r="C1" s="199"/>
-      <c r="D1" s="199"/>
-      <c r="E1" s="199"/>
+      <c r="B1" s="200"/>
+      <c r="C1" s="200"/>
+      <c r="D1" s="200"/>
+      <c r="E1" s="200"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A2" s="200" t="s">
+      <c r="A2" s="201" t="s">
         <v>192</v>
       </c>
-      <c r="B2" s="200"/>
-      <c r="C2" s="200"/>
-      <c r="D2" s="200"/>
-      <c r="E2" s="200"/>
+      <c r="B2" s="201"/>
+      <c r="C2" s="201"/>
+      <c r="D2" s="201"/>
+      <c r="E2" s="201"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A19" s="9" t="s">
@@ -31770,13 +31768,13 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A21" s="200" t="s">
+      <c r="A21" s="201" t="s">
         <v>195</v>
       </c>
-      <c r="B21" s="200"/>
-      <c r="C21" s="200"/>
-      <c r="D21" s="200"/>
-      <c r="E21" s="200"/>
+      <c r="B21" s="201"/>
+      <c r="C21" s="201"/>
+      <c r="D21" s="201"/>
+      <c r="E21" s="201"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A38" s="9" t="s">
@@ -31792,13 +31790,13 @@
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A40" s="200" t="s">
+      <c r="A40" s="201" t="s">
         <v>196</v>
       </c>
-      <c r="B40" s="200"/>
-      <c r="C40" s="200"/>
-      <c r="D40" s="200"/>
-      <c r="E40" s="200"/>
+      <c r="B40" s="201"/>
+      <c r="C40" s="201"/>
+      <c r="D40" s="201"/>
+      <c r="E40" s="201"/>
     </row>
     <row r="57" spans="1:5" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
       <c r="A57" s="9" t="s">
@@ -31814,13 +31812,13 @@
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A60" s="199" t="s">
+      <c r="A60" s="200" t="s">
         <v>198</v>
       </c>
-      <c r="B60" s="199"/>
-      <c r="C60" s="199"/>
-      <c r="D60" s="199"/>
-      <c r="E60" s="199"/>
+      <c r="B60" s="200"/>
+      <c r="C60" s="200"/>
+      <c r="D60" s="200"/>
+      <c r="E60" s="200"/>
     </row>
     <row r="85" spans="1:39" s="12" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A85" s="9" t="s">
@@ -31925,13 +31923,13 @@
       </c>
     </row>
     <row r="89" spans="1:39" x14ac:dyDescent="0.75">
-      <c r="A89" s="199" t="s">
+      <c r="A89" s="200" t="s">
         <v>199</v>
       </c>
-      <c r="B89" s="199"/>
-      <c r="C89" s="199"/>
-      <c r="D89" s="199"/>
-      <c r="E89" s="199"/>
+      <c r="B89" s="200"/>
+      <c r="C89" s="200"/>
+      <c r="D89" s="200"/>
+      <c r="E89" s="200"/>
     </row>
     <row r="90" spans="1:39" x14ac:dyDescent="0.75">
       <c r="A90" s="9">
@@ -32018,13 +32016,13 @@
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A98" s="199" t="s">
+      <c r="A98" s="200" t="s">
         <v>200</v>
       </c>
-      <c r="B98" s="199"/>
-      <c r="C98" s="199"/>
-      <c r="D98" s="199"/>
-      <c r="E98" s="199"/>
+      <c r="B98" s="200"/>
+      <c r="C98" s="200"/>
+      <c r="D98" s="200"/>
+      <c r="E98" s="200"/>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A99" s="17">
@@ -32108,13 +32106,13 @@
       <c r="A108" s="20"/>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A109" s="199" t="s">
+      <c r="A109" s="200" t="s">
         <v>202</v>
       </c>
-      <c r="B109" s="199"/>
-      <c r="C109" s="199"/>
-      <c r="D109" s="199"/>
-      <c r="E109" s="199"/>
+      <c r="B109" s="200"/>
+      <c r="C109" s="200"/>
+      <c r="D109" s="200"/>
+      <c r="E109" s="200"/>
     </row>
     <row r="110" spans="1:5" ht="15.5" thickBot="1" x14ac:dyDescent="0.9"/>
     <row r="111" spans="1:5" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
@@ -32127,13 +32125,13 @@
       </c>
     </row>
     <row r="113" spans="1:14" x14ac:dyDescent="0.75">
-      <c r="A113" s="199" t="s">
+      <c r="A113" s="200" t="s">
         <v>201</v>
       </c>
-      <c r="B113" s="199"/>
-      <c r="C113" s="199"/>
-      <c r="D113" s="199"/>
-      <c r="E113" s="199"/>
+      <c r="B113" s="200"/>
+      <c r="C113" s="200"/>
+      <c r="D113" s="200"/>
+      <c r="E113" s="200"/>
     </row>
     <row r="114" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A114" s="17">
@@ -32214,13 +32212,13 @@
       </c>
     </row>
     <row r="124" spans="1:14" x14ac:dyDescent="0.75">
-      <c r="A124" s="199" t="s">
+      <c r="A124" s="200" t="s">
         <v>482</v>
       </c>
-      <c r="B124" s="199"/>
-      <c r="C124" s="199"/>
-      <c r="D124" s="199"/>
-      <c r="E124" s="199"/>
+      <c r="B124" s="200"/>
+      <c r="C124" s="200"/>
+      <c r="D124" s="200"/>
+      <c r="E124" s="200"/>
       <c r="L124" s="21"/>
     </row>
     <row r="125" spans="1:14" x14ac:dyDescent="0.75">
@@ -32311,13 +32309,13 @@
       <c r="C133" s="15"/>
     </row>
     <row r="134" spans="1:14" x14ac:dyDescent="0.75">
-      <c r="A134" s="199" t="s">
+      <c r="A134" s="200" t="s">
         <v>115</v>
       </c>
-      <c r="B134" s="199"/>
-      <c r="C134" s="199"/>
-      <c r="D134" s="199"/>
-      <c r="E134" s="199"/>
+      <c r="B134" s="200"/>
+      <c r="C134" s="200"/>
+      <c r="D134" s="200"/>
+      <c r="E134" s="200"/>
     </row>
     <row r="135" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A135" s="27" t="s">
@@ -32332,25 +32330,25 @@
     </row>
     <row r="136" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A136" s="29"/>
-      <c r="B136" s="196" t="s">
+      <c r="B136" s="197" t="s">
         <v>502</v>
       </c>
-      <c r="C136" s="197"/>
-      <c r="D136" s="197"/>
-      <c r="E136" s="198"/>
+      <c r="C136" s="198"/>
+      <c r="D136" s="198"/>
+      <c r="E136" s="199"/>
       <c r="F136" s="28"/>
       <c r="G136" s="28"/>
     </row>
     <row r="137" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A137" s="30"/>
-      <c r="B137" s="196" t="s">
+      <c r="B137" s="197" t="s">
         <v>503</v>
       </c>
-      <c r="C137" s="198"/>
-      <c r="D137" s="196" t="s">
+      <c r="C137" s="199"/>
+      <c r="D137" s="197" t="s">
         <v>504</v>
       </c>
-      <c r="E137" s="198"/>
+      <c r="E137" s="199"/>
       <c r="F137" s="28"/>
       <c r="G137" s="28"/>
     </row>
@@ -32897,13 +32895,13 @@
       <c r="G163" s="28"/>
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A165" s="199" t="s">
+      <c r="A165" s="200" t="s">
         <v>205</v>
       </c>
-      <c r="B165" s="199"/>
-      <c r="C165" s="199"/>
-      <c r="D165" s="199"/>
-      <c r="E165" s="199"/>
+      <c r="B165" s="200"/>
+      <c r="C165" s="200"/>
+      <c r="D165" s="200"/>
+      <c r="E165" s="200"/>
     </row>
     <row r="166" spans="1:7" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
       <c r="A166" s="23" t="s">
@@ -32926,10 +32924,10 @@
       <c r="B168" s="46"/>
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A169" s="199" t="s">
+      <c r="A169" s="200" t="s">
         <v>490</v>
       </c>
-      <c r="B169" s="199"/>
+      <c r="B169" s="200"/>
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A170" s="23" t="s">
@@ -32961,13 +32959,13 @@
       <c r="B173" s="46"/>
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A174" s="199" t="s">
+      <c r="A174" s="200" t="s">
         <v>215</v>
       </c>
-      <c r="B174" s="199"/>
-      <c r="C174" s="199"/>
-      <c r="D174" s="199"/>
-      <c r="E174" s="199"/>
+      <c r="B174" s="200"/>
+      <c r="C174" s="200"/>
+      <c r="D174" s="200"/>
+      <c r="E174" s="200"/>
     </row>
     <row r="175" spans="1:7" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
       <c r="A175" s="23" t="s">
@@ -32987,13 +32985,13 @@
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A178" s="199" t="s">
+      <c r="A178" s="200" t="s">
         <v>208</v>
       </c>
-      <c r="B178" s="199"/>
-      <c r="C178" s="199"/>
-      <c r="D178" s="199"/>
-      <c r="E178" s="199"/>
+      <c r="B178" s="200"/>
+      <c r="C178" s="200"/>
+      <c r="D178" s="200"/>
+      <c r="E178" s="200"/>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A179" s="25" t="s">
@@ -33021,13 +33019,13 @@
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A183" s="199" t="s">
+      <c r="A183" s="200" t="s">
         <v>210</v>
       </c>
-      <c r="B183" s="199"/>
-      <c r="C183" s="199"/>
-      <c r="D183" s="199"/>
-      <c r="E183" s="199"/>
+      <c r="B183" s="200"/>
+      <c r="C183" s="200"/>
+      <c r="D183" s="200"/>
+      <c r="E183" s="200"/>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A184" s="23" t="s">
@@ -33082,13 +33080,13 @@
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A191" s="199" t="s">
+      <c r="A191" s="200" t="s">
         <v>227</v>
       </c>
-      <c r="B191" s="199"/>
-      <c r="C191" s="199"/>
-      <c r="D191" s="199"/>
-      <c r="E191" s="199"/>
+      <c r="B191" s="200"/>
+      <c r="C191" s="200"/>
+      <c r="D191" s="200"/>
+      <c r="E191" s="200"/>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A192" s="21" t="s">

</xml_diff>

<commit_message>
Updated descriptions in WebAppData file
</commit_message>
<xml_diff>
--- a/WebAppData.xlsx
+++ b/WebAppData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swenzel\Dropbox (Energy Innovation)\My PC (energy044)\Documents\GitHub_Repositories\eps-alberta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30249D53-227C-43BF-AA60-9E34A29740FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91A64F54-15DF-4921-8A5C-C5ADB446E497}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12600" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="824" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4083,9 +4083,6 @@
     <t>**Description:** This policy tightens energy efficiency standards for the selected component(s) in the selected building type(s).  The policy only applies to newly sold components each year (whether for new buildings or replacement of old components of existing buildings). // **Guidance for setting values:** In "Assessment of Electricity Savings in the U.S. Achievable through New Appliance/Equipment Efficiency Standards and Building Efficiency Codes, 2010-2025" (2011), the Edison Foundation considered a 30% reduction in whole-building energy use (moderate case) and 40-45% (aggressive case) relative to BAU from 2010 to 2025.  Similar potentials may be possible in Alberta, with further improvement post-2025.</t>
   </si>
   <si>
-    <t xml:space="preserve">**Description:** This policy replaces the specified fraction of newly sold non-electric building components of the selected type(s) in buildings of the selected type(s) with electricity-using components. // **Guidance for setting values:** // **Urban Residential:** In the BAU case, the share of electricity among fuels used by urban, residential buildings will rise between 2017 and 2050.  // **Rural Residential:** In the BAU case, the share of electricity among fuels used by urban, residential buildings will rise between 2017 and 2050.  // **Commercial:** In the BAU case, the share of electricity among fuels used by urban, residential buildings will rise between 2017 and 2050. </t>
-  </si>
-  <si>
     <t xml:space="preserve">**Description:** Transportation Demand Management (TDM) represents a set of policies aimed at reducing demand for certain modes of travel. Passenger Transportation Demand Management (TDM) is aimed at reducing demand for passenger travel, especially in private automobiles.  These policies can include improved public transit systems, more walking and bike paths, zoning for higher density along transit corridors, zoning for mixed-use developments, roadway and congestion pricing, and increased parking fees.  Freight Transportation Demand Management (TDM) represents a set of policies aimed primarily at shifting freight from trucks to rail.  We use the International Energy Agency's BLUE Shifts scenario (from the 2009 report "Transport, Energy, and CO2: Moving Toward Sustainability") to represent passenger TDM policies as a whole. // **Guidance for setting values:** A value of "100%" fully implements the IEA's BLUE Shifts scenario by 2050, which is in line with IEA expectations (since their scenario assumes implementation by 2050). </t>
   </si>
   <si>
@@ -4095,9 +4092,6 @@
     <t>**Description:** This policy implements a fee on sales of inefficient light-duty vehicles (LDVs; namely cars and SUVs) that is rebated to buyers of efficient LDVs.  The feebate policy is revenue-neutral, as the pivot point (the efficiency level that incurs neither a rebate nor a fee) is set such that the total of all fees equals the total of all rebates. // **Guidance for setting values:** The feebate is set as a fraction of the global best practice feebate rate.  The global best practice feebate rate would levy a fee of approximately $1350 CDN on a vehicle that consumes 12 liters per 100 km if the pivot point is 10 liters per 100 km.</t>
   </si>
   <si>
-    <t>**Description:** This policy causes government to pay for the specified percentage of the purchase price of new battery electric passenger LDVs.  This is in addition to EV subsidies that exist in the BAU case.  // **Guidance for setting values:** In Canada, several provinces have EV subsidy programs, paying for between $5000 and $14000 of the cost of a new EV.  This is roughly between 10% and 35% of the cost of a new EV.</t>
-  </si>
-  <si>
     <t>It matches policies to the listing in the "PolicyLevers" tab using the "Vensim Variable Name" column.</t>
   </si>
   <si>
@@ -4107,9 +4101,6 @@
     <t>**Description:** This policy requires the specified percentage of newly sold vehicles of the selected type(s) to consist of battery electric vehicles. If that percentage would already be achieved through BAU sales plus the effects of other policies, such as an EV subsidy, this policy has no effect. Manufactures may meet a sales standard through techniques such as more heavily marketing electric vehicles, lowering the price of electric vehicles, or raising the price of non-electric vehicles. // **Guidance for setting values:** Under the Pan-Canadian Framework, Canada has a target of a 30% market share for electric vehicles among new on-road vehicles by 2030.</t>
   </si>
   <si>
-    <t xml:space="preserve">**Description:** This policy represents strengthening standards for the selected pollutant(s) emitted by the selected vehicle type(s).  Conventional pollutants' most important, harmful impacts are on human health rather than on climate change. // **Guidance for setting values:** In Canada, the 24-hour national ambient air quality standard (Canadian Ambient Air Quality Standards – CAAQS) for PM2.5, the most harmful type of particulate for human health, is 28 µg/m^3 for the period 2015-2020. </t>
-  </si>
-  <si>
     <t>**Description:** This policy applies a tax on fuels used in the selected sector(s) based on their greenhouse gas emissions.  It also increases the base cost of capital equipment (e.g., vehicles, power plants, building components) according to their embedded carbon content. // **Guidance for setting values:** The Canadian government's revised 2016 Social Cost of Carbon estimates for the year 2050 range from CAD$75 in the central estimate to CAD$320 per ton in the 95th percnetile estimate (in inflation-adjusted 2012 Canadian dollars).</t>
   </si>
   <si>
@@ -4117,6 +4108,15 @@
   </si>
   <si>
     <t>**Description:** This policy increases or decreases the amount of electricity exported from Alberta to the United States.  It does not cause the construction or removal of transmission lines linking these jurisdictions. // **Guidance for setting values:** From 2017-2050, in the BAU case, electricity imports are expected to remain stable.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">**Description:** This policy represents strengthening the standards for regulated pollutants other than greenhouse gases (such as NOx or particulate matter) emitted by the selected vehicle type(s).  Conventional pollutants' most important, harmful impacts are on human health rather than on climate change. // **Guidance for setting values:** In Canada, the 24-hour national ambient air quality standard (Canadian Ambient Air Quality Standards – CAAQS) for PM2.5, the most harmful type of particulate for human health, is 28 µg/m^3 for the period 2015-2020. </t>
+  </si>
+  <si>
+    <t>**Description:** This policy causes government to pay for the specified percentage of the purchase price of new battery electric vehicles for the selected type(s).  This is in addition to EV subsidies that exist in the BAU case.  // **Guidance for setting values:** In Canada, several provinces have EV subsidy programs, paying for between $5000 and $14000 of the cost of a new EV.  This is roughly between 10% and 35% of the cost of a new EV.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">**Description:** This policy replaces the specified fraction of newly sold non-electric building components in buildings of the selected type(s) with electricity-using components. // **Guidance for setting values:** // **Urban Residential:** In the BAU case, the share of electricity among fuels used by urban, residential buildings will rise between 2017 and 2050.  // **Rural Residential:** In the BAU case, the share of electricity among fuels used by urban, residential buildings will rise between 2017 and 2050.  // **Commercial:** In the BAU case, the share of electricity among fuels used by urban, residential buildings will rise between 2017 and 2050. </t>
   </si>
 </sst>
 </file>
@@ -6419,8 +6419,8 @@
   </sheetPr>
   <dimension ref="A1:N105"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5:K5"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -6442,7 +6442,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A1" s="190" t="s">
-        <v>1209</v>
+        <v>1207</v>
       </c>
       <c r="B1" s="188"/>
       <c r="C1" s="188"/>
@@ -6460,7 +6460,7 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A2" s="189" t="s">
-        <v>1208</v>
+        <v>1206</v>
       </c>
       <c r="B2" s="188"/>
       <c r="C2" s="188"/>
@@ -6549,7 +6549,7 @@
         <v>1023</v>
       </c>
       <c r="J4" s="169" t="s">
-        <v>1211</v>
+        <v>1212</v>
       </c>
       <c r="K4" s="75" t="s">
         <v>1024</v>
@@ -6625,7 +6625,7 @@
         <v>579</v>
       </c>
       <c r="J6" s="169" t="s">
-        <v>1210</v>
+        <v>1208</v>
       </c>
       <c r="K6" s="75" t="s">
         <v>580</v>
@@ -6634,7 +6634,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="44.4" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:14" ht="62.25" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A7" s="168" t="s">
         <v>4</v>
       </c>
@@ -6663,7 +6663,7 @@
         <v>567</v>
       </c>
       <c r="J7" s="169" t="s">
-        <v>1207</v>
+        <v>1213</v>
       </c>
       <c r="K7" s="75" t="s">
         <v>568</v>
@@ -6701,7 +6701,7 @@
         <v>547</v>
       </c>
       <c r="J8" s="169" t="s">
-        <v>1206</v>
+        <v>1205</v>
       </c>
       <c r="K8" s="169" t="s">
         <v>234</v>
@@ -6745,7 +6745,7 @@
         <v>127</v>
       </c>
       <c r="J9" s="169" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
       <c r="K9" s="169" t="s">
         <v>236</v>
@@ -6756,7 +6756,7 @@
       <c r="M9" s="174"/>
       <c r="N9" s="169"/>
     </row>
-    <row r="10" spans="1:14" ht="44.4" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:14" ht="92.25" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A10" s="168" t="s">
         <v>4</v>
       </c>
@@ -6823,7 +6823,7 @@
         <v>44</v>
       </c>
       <c r="J11" s="169" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
       <c r="K11" s="169" t="s">
         <v>238</v>
@@ -6864,7 +6864,7 @@
         <v>129</v>
       </c>
       <c r="J12" s="169" t="s">
-        <v>1203</v>
+        <v>1214</v>
       </c>
       <c r="K12" s="169" t="s">
         <v>240</v>
@@ -6873,7 +6873,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="60" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:14" ht="127.5" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A13" s="169" t="s">
         <v>83</v>
       </c>
@@ -6917,7 +6917,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="44.4" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:14" ht="84.9" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A14" s="169" t="s">
         <v>83</v>
       </c>
@@ -6955,7 +6955,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="44.4" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:14" ht="77.25" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A15" s="169" t="s">
         <v>83</v>
       </c>
@@ -7000,7 +7000,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="44.4" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:14" ht="88.5" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A16" s="169" t="s">
         <v>83</v>
       </c>
@@ -7038,7 +7038,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="44.4" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="17" spans="1:14" ht="51.75" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A17" s="169" t="s">
         <v>83</v>
       </c>
@@ -7076,7 +7076,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="152.25" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="18" spans="1:14" ht="258" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A18" s="169" t="s">
         <v>83</v>
       </c>
@@ -7106,7 +7106,7 @@
         <v>43</v>
       </c>
       <c r="J18" s="169" t="s">
-        <v>1213</v>
+        <v>1210</v>
       </c>
       <c r="K18" s="169" t="s">
         <v>248</v>
@@ -7266,7 +7266,7 @@
         <v>331</v>
       </c>
       <c r="J22" s="169" t="s">
-        <v>1214</v>
+        <v>1211</v>
       </c>
       <c r="K22" s="169" t="s">
         <v>333</v>
@@ -7389,7 +7389,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="44.4" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="26" spans="1:14" ht="92.25" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A26" s="169" t="s">
         <v>8</v>
       </c>
@@ -7433,7 +7433,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="44.4" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="27" spans="1:14" ht="93.75" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A27" s="169" t="s">
         <v>8</v>
       </c>
@@ -7619,7 +7619,7 @@
       <c r="M31" s="173"/>
       <c r="N31" s="168"/>
     </row>
-    <row r="32" spans="1:14" ht="44.4" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="32" spans="1:14" ht="90" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A32" s="168" t="s">
         <v>8</v>
       </c>
@@ -7657,7 +7657,7 @@
         <v>945</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="44.4" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="33" spans="1:14" ht="69" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A33" s="168" t="s">
         <v>8</v>
       </c>
@@ -7735,7 +7735,7 @@
       <c r="L34" s="168"/>
       <c r="M34" s="173"/>
     </row>
-    <row r="35" spans="1:14" ht="170" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="35" spans="1:14" ht="250.25" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A35" s="169" t="s">
         <v>8</v>
       </c>
@@ -7776,7 +7776,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="44.4" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="36" spans="1:14" ht="71.25" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A36" s="169" t="s">
         <v>9</v>
       </c>
@@ -7817,7 +7817,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="44.4" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="37" spans="1:14" ht="58.5" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A37" s="169" t="s">
         <v>9</v>
       </c>
@@ -7858,7 +7858,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="44.4" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="38" spans="1:14" ht="93" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A38" s="169" t="s">
         <v>9</v>
       </c>
@@ -7899,7 +7899,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="63" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="39" spans="1:14" ht="98.25" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A39" s="169" t="s">
         <v>9</v>
       </c>
@@ -7984,7 +7984,7 @@
       </c>
       <c r="N40" s="175"/>
     </row>
-    <row r="41" spans="1:14" ht="77.5" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="41" spans="1:14" ht="93.25" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A41" s="169" t="s">
         <v>9</v>
       </c>
@@ -8024,7 +8024,7 @@
       <c r="M41" s="174"/>
       <c r="N41" s="169"/>
     </row>
-    <row r="42" spans="1:14" ht="70.25" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="42" spans="1:14" ht="152" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A42" s="169" t="s">
         <v>9</v>
       </c>
@@ -8064,7 +8064,7 @@
       <c r="M42" s="174"/>
       <c r="N42" s="169"/>
     </row>
-    <row r="43" spans="1:14" ht="44.4" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="43" spans="1:14" ht="83.25" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A43" s="169" t="s">
         <v>9</v>
       </c>
@@ -8106,7 +8106,7 @@
       </c>
       <c r="N43" s="169"/>
     </row>
-    <row r="44" spans="1:14" ht="44.4" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="44" spans="1:14" ht="71.25" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A44" s="169" t="s">
         <v>9</v>
       </c>
@@ -8148,7 +8148,7 @@
       </c>
       <c r="N44" s="169"/>
     </row>
-    <row r="45" spans="1:14" ht="44.4" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="45" spans="1:14" ht="69" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A45" s="169" t="s">
         <v>9</v>
       </c>
@@ -8190,7 +8190,7 @@
       </c>
       <c r="N45" s="169"/>
     </row>
-    <row r="46" spans="1:14" ht="44.4" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="46" spans="1:14" ht="83.25" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A46" s="169" t="s">
         <v>9</v>
       </c>
@@ -8232,7 +8232,7 @@
       </c>
       <c r="N46" s="169"/>
     </row>
-    <row r="47" spans="1:14" ht="44.4" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="47" spans="1:14" ht="74.25" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A47" s="169" t="s">
         <v>166</v>
       </c>
@@ -8578,7 +8578,7 @@
       </c>
       <c r="N55" s="169"/>
     </row>
-    <row r="56" spans="1:14" ht="44.4" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="56" spans="1:14" ht="75" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A56" s="168" t="s">
         <v>436</v>
       </c>
@@ -8620,7 +8620,7 @@
       </c>
       <c r="N56" s="168"/>
     </row>
-    <row r="57" spans="1:14" ht="44.4" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="57" spans="1:14" ht="76.5" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A57" s="168" t="s">
         <v>436</v>
       </c>
@@ -8662,7 +8662,7 @@
       </c>
       <c r="N57" s="168"/>
     </row>
-    <row r="58" spans="1:14" ht="44.4" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="58" spans="1:14" ht="83.25" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A58" s="169" t="s">
         <v>10</v>
       </c>
@@ -8704,7 +8704,7 @@
       </c>
       <c r="N58" s="169"/>
     </row>
-    <row r="59" spans="1:14" ht="56.25" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="59" spans="1:14" ht="106.5" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A59" s="169" t="s">
         <v>10</v>
       </c>
@@ -8733,7 +8733,7 @@
         <v>981</v>
       </c>
       <c r="J59" s="196" t="s">
-        <v>1212</v>
+        <v>1209</v>
       </c>
       <c r="K59" s="169" t="s">
         <v>295</v>
@@ -8845,7 +8845,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="63" spans="1:14" ht="76.5" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="63" spans="1:14" ht="128.25" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A63" s="169" t="s">
         <v>32</v>
       </c>
@@ -8883,7 +8883,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="64" spans="1:14" ht="44.4" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="64" spans="1:14" ht="72.75" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A64" s="169" t="s">
         <v>32</v>
       </c>
@@ -9039,7 +9039,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="68" spans="1:14" ht="71" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="68" spans="1:14" ht="89" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A68" s="169" t="s">
         <v>32</v>
       </c>
@@ -9276,8 +9276,8 @@
   <dimension ref="A1:T327"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A182" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B183" sqref="B183"/>
+      <pane ySplit="1" topLeftCell="A73" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A73" sqref="A73:XFD73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -9362,7 +9362,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="2" spans="1:20" s="3" customFormat="1" ht="73.75" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:20" s="3" customFormat="1" ht="88.5" x14ac:dyDescent="0.75">
       <c r="A2" s="101" t="s">
         <v>4</v>
       </c>
@@ -9406,7 +9406,7 @@
       </c>
       <c r="P2" s="195" t="str">
         <f>INDEX('Policy Characteristics'!J:J,MATCH($C2,'Policy Characteristics'!$C:$C,0))</f>
-        <v xml:space="preserve">**Description:** This policy represents strengthening standards for the selected pollutant(s) emitted by the selected vehicle type(s).  Conventional pollutants' most important, harmful impacts are on human health rather than on climate change. // **Guidance for setting values:** In Canada, the 24-hour national ambient air quality standard (Canadian Ambient Air Quality Standards – CAAQS) for PM2.5, the most harmful type of particulate for human health, is 28 µg/m^3 for the period 2015-2020. </v>
+        <v xml:space="preserve">**Description:** This policy represents strengthening the standards for regulated pollutants other than greenhouse gases (such as NOx or particulate matter) emitted by the selected vehicle type(s).  Conventional pollutants' most important, harmful impacts are on human health rather than on climate change. // **Guidance for setting values:** In Canada, the 24-hour national ambient air quality standard (Canadian Ambient Air Quality Standards – CAAQS) for PM2.5, the most harmful type of particulate for human health, is 28 µg/m^3 for the period 2015-2020. </v>
       </c>
       <c r="Q2" s="75" t="s">
         <v>1024</v>
@@ -9416,7 +9416,7 @@
       </c>
       <c r="S2" s="150"/>
     </row>
-    <row r="3" spans="1:20" s="3" customFormat="1" ht="73.75" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:20" s="3" customFormat="1" ht="88.5" x14ac:dyDescent="0.75">
       <c r="A3" s="193" t="str">
         <f>A$2</f>
         <v>Transportation</v>
@@ -9469,7 +9469,7 @@
       </c>
       <c r="P3" s="195" t="str">
         <f>INDEX('Policy Characteristics'!J:J,MATCH($C3,'Policy Characteristics'!$C:$C,0))</f>
-        <v xml:space="preserve">**Description:** This policy represents strengthening standards for the selected pollutant(s) emitted by the selected vehicle type(s).  Conventional pollutants' most important, harmful impacts are on human health rather than on climate change. // **Guidance for setting values:** In Canada, the 24-hour national ambient air quality standard (Canadian Ambient Air Quality Standards – CAAQS) for PM2.5, the most harmful type of particulate for human health, is 28 µg/m^3 for the period 2015-2020. </v>
+        <v xml:space="preserve">**Description:** This policy represents strengthening the standards for regulated pollutants other than greenhouse gases (such as NOx or particulate matter) emitted by the selected vehicle type(s).  Conventional pollutants' most important, harmful impacts are on human health rather than on climate change. // **Guidance for setting values:** In Canada, the 24-hour national ambient air quality standard (Canadian Ambient Air Quality Standards – CAAQS) for PM2.5, the most harmful type of particulate for human health, is 28 µg/m^3 for the period 2015-2020. </v>
       </c>
       <c r="Q3" s="5" t="str">
         <f t="shared" si="1"/>
@@ -9481,7 +9481,7 @@
       </c>
       <c r="S3" s="150"/>
     </row>
-    <row r="4" spans="1:20" s="3" customFormat="1" ht="73.75" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:20" s="3" customFormat="1" ht="88.5" x14ac:dyDescent="0.75">
       <c r="A4" s="193" t="str">
         <f t="shared" ref="A4:A7" si="2">A$2</f>
         <v>Transportation</v>
@@ -9534,7 +9534,7 @@
       </c>
       <c r="P4" s="195" t="str">
         <f>INDEX('Policy Characteristics'!J:J,MATCH($C4,'Policy Characteristics'!$C:$C,0))</f>
-        <v xml:space="preserve">**Description:** This policy represents strengthening standards for the selected pollutant(s) emitted by the selected vehicle type(s).  Conventional pollutants' most important, harmful impacts are on human health rather than on climate change. // **Guidance for setting values:** In Canada, the 24-hour national ambient air quality standard (Canadian Ambient Air Quality Standards – CAAQS) for PM2.5, the most harmful type of particulate for human health, is 28 µg/m^3 for the period 2015-2020. </v>
+        <v xml:space="preserve">**Description:** This policy represents strengthening the standards for regulated pollutants other than greenhouse gases (such as NOx or particulate matter) emitted by the selected vehicle type(s).  Conventional pollutants' most important, harmful impacts are on human health rather than on climate change. // **Guidance for setting values:** In Canada, the 24-hour national ambient air quality standard (Canadian Ambient Air Quality Standards – CAAQS) for PM2.5, the most harmful type of particulate for human health, is 28 µg/m^3 for the period 2015-2020. </v>
       </c>
       <c r="Q4" s="5" t="str">
         <f t="shared" si="1"/>
@@ -9546,7 +9546,7 @@
       </c>
       <c r="S4" s="150"/>
     </row>
-    <row r="5" spans="1:20" s="3" customFormat="1" ht="73.75" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:20" s="3" customFormat="1" ht="88.5" x14ac:dyDescent="0.75">
       <c r="A5" s="193" t="str">
         <f t="shared" si="2"/>
         <v>Transportation</v>
@@ -9599,7 +9599,7 @@
       </c>
       <c r="P5" s="195" t="str">
         <f>INDEX('Policy Characteristics'!J:J,MATCH($C5,'Policy Characteristics'!$C:$C,0))</f>
-        <v xml:space="preserve">**Description:** This policy represents strengthening standards for the selected pollutant(s) emitted by the selected vehicle type(s).  Conventional pollutants' most important, harmful impacts are on human health rather than on climate change. // **Guidance for setting values:** In Canada, the 24-hour national ambient air quality standard (Canadian Ambient Air Quality Standards – CAAQS) for PM2.5, the most harmful type of particulate for human health, is 28 µg/m^3 for the period 2015-2020. </v>
+        <v xml:space="preserve">**Description:** This policy represents strengthening the standards for regulated pollutants other than greenhouse gases (such as NOx or particulate matter) emitted by the selected vehicle type(s).  Conventional pollutants' most important, harmful impacts are on human health rather than on climate change. // **Guidance for setting values:** In Canada, the 24-hour national ambient air quality standard (Canadian Ambient Air Quality Standards – CAAQS) for PM2.5, the most harmful type of particulate for human health, is 28 µg/m^3 for the period 2015-2020. </v>
       </c>
       <c r="Q5" s="5" t="str">
         <f t="shared" si="1"/>
@@ -9611,7 +9611,7 @@
       </c>
       <c r="S5" s="150"/>
     </row>
-    <row r="6" spans="1:20" s="3" customFormat="1" ht="73.75" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:20" s="3" customFormat="1" ht="88.5" x14ac:dyDescent="0.75">
       <c r="A6" s="193" t="str">
         <f t="shared" si="2"/>
         <v>Transportation</v>
@@ -9664,7 +9664,7 @@
       </c>
       <c r="P6" s="195" t="str">
         <f>INDEX('Policy Characteristics'!J:J,MATCH($C6,'Policy Characteristics'!$C:$C,0))</f>
-        <v xml:space="preserve">**Description:** This policy represents strengthening standards for the selected pollutant(s) emitted by the selected vehicle type(s).  Conventional pollutants' most important, harmful impacts are on human health rather than on climate change. // **Guidance for setting values:** In Canada, the 24-hour national ambient air quality standard (Canadian Ambient Air Quality Standards – CAAQS) for PM2.5, the most harmful type of particulate for human health, is 28 µg/m^3 for the period 2015-2020. </v>
+        <v xml:space="preserve">**Description:** This policy represents strengthening the standards for regulated pollutants other than greenhouse gases (such as NOx or particulate matter) emitted by the selected vehicle type(s).  Conventional pollutants' most important, harmful impacts are on human health rather than on climate change. // **Guidance for setting values:** In Canada, the 24-hour national ambient air quality standard (Canadian Ambient Air Quality Standards – CAAQS) for PM2.5, the most harmful type of particulate for human health, is 28 µg/m^3 for the period 2015-2020. </v>
       </c>
       <c r="Q6" s="5" t="str">
         <f t="shared" si="1"/>
@@ -9676,7 +9676,7 @@
       </c>
       <c r="S6" s="150"/>
     </row>
-    <row r="7" spans="1:20" s="3" customFormat="1" ht="73.75" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:20" s="3" customFormat="1" ht="88.5" x14ac:dyDescent="0.75">
       <c r="A7" s="193" t="str">
         <f t="shared" si="2"/>
         <v>Transportation</v>
@@ -9729,7 +9729,7 @@
       </c>
       <c r="P7" s="195" t="str">
         <f>INDEX('Policy Characteristics'!J:J,MATCH($C7,'Policy Characteristics'!$C:$C,0))</f>
-        <v xml:space="preserve">**Description:** This policy represents strengthening standards for the selected pollutant(s) emitted by the selected vehicle type(s).  Conventional pollutants' most important, harmful impacts are on human health rather than on climate change. // **Guidance for setting values:** In Canada, the 24-hour national ambient air quality standard (Canadian Ambient Air Quality Standards – CAAQS) for PM2.5, the most harmful type of particulate for human health, is 28 µg/m^3 for the period 2015-2020. </v>
+        <v xml:space="preserve">**Description:** This policy represents strengthening the standards for regulated pollutants other than greenhouse gases (such as NOx or particulate matter) emitted by the selected vehicle type(s).  Conventional pollutants' most important, harmful impacts are on human health rather than on climate change. // **Guidance for setting values:** In Canada, the 24-hour national ambient air quality standard (Canadian Ambient Air Quality Standards – CAAQS) for PM2.5, the most harmful type of particulate for human health, is 28 µg/m^3 for the period 2015-2020. </v>
       </c>
       <c r="Q7" s="5" t="str">
         <f t="shared" si="1"/>
@@ -10529,7 +10529,7 @@
       </c>
       <c r="P21" s="195" t="str">
         <f>INDEX('Policy Characteristics'!J:J,MATCH($C21,'Policy Characteristics'!$C:$C,0))</f>
-        <v>**Description:** This policy causes government to pay for the specified percentage of the purchase price of new battery electric passenger LDVs.  This is in addition to EV subsidies that exist in the BAU case.  // **Guidance for setting values:** In Canada, several provinces have EV subsidy programs, paying for between $5000 and $14000 of the cost of a new EV.  This is roughly between 10% and 35% of the cost of a new EV.</v>
+        <v>**Description:** This policy causes government to pay for the specified percentage of the purchase price of new battery electric vehicles for the selected type(s).  This is in addition to EV subsidies that exist in the BAU case.  // **Guidance for setting values:** In Canada, several provinces have EV subsidy programs, paying for between $5000 and $14000 of the cost of a new EV.  This is roughly between 10% and 35% of the cost of a new EV.</v>
       </c>
       <c r="Q21" s="75" t="s">
         <v>568</v>
@@ -10583,7 +10583,7 @@
       <c r="O22" s="77"/>
       <c r="P22" s="195" t="str">
         <f>INDEX('Policy Characteristics'!J:J,MATCH($C22,'Policy Characteristics'!$C:$C,0))</f>
-        <v>**Description:** This policy causes government to pay for the specified percentage of the purchase price of new battery electric passenger LDVs.  This is in addition to EV subsidies that exist in the BAU case.  // **Guidance for setting values:** In Canada, several provinces have EV subsidy programs, paying for between $5000 and $14000 of the cost of a new EV.  This is roughly between 10% and 35% of the cost of a new EV.</v>
+        <v>**Description:** This policy causes government to pay for the specified percentage of the purchase price of new battery electric vehicles for the selected type(s).  This is in addition to EV subsidies that exist in the BAU case.  // **Guidance for setting values:** In Canada, several provinces have EV subsidy programs, paying for between $5000 and $14000 of the cost of a new EV.  This is roughly between 10% and 35% of the cost of a new EV.</v>
       </c>
       <c r="Q22" s="77"/>
       <c r="R22" s="77"/>
@@ -10633,7 +10633,7 @@
       <c r="O23" s="77"/>
       <c r="P23" s="195" t="str">
         <f>INDEX('Policy Characteristics'!J:J,MATCH($C23,'Policy Characteristics'!$C:$C,0))</f>
-        <v>**Description:** This policy causes government to pay for the specified percentage of the purchase price of new battery electric passenger LDVs.  This is in addition to EV subsidies that exist in the BAU case.  // **Guidance for setting values:** In Canada, several provinces have EV subsidy programs, paying for between $5000 and $14000 of the cost of a new EV.  This is roughly between 10% and 35% of the cost of a new EV.</v>
+        <v>**Description:** This policy causes government to pay for the specified percentage of the purchase price of new battery electric vehicles for the selected type(s).  This is in addition to EV subsidies that exist in the BAU case.  // **Guidance for setting values:** In Canada, several provinces have EV subsidy programs, paying for between $5000 and $14000 of the cost of a new EV.  This is roughly between 10% and 35% of the cost of a new EV.</v>
       </c>
       <c r="Q23" s="77"/>
       <c r="R23" s="77"/>
@@ -10697,7 +10697,7 @@
       </c>
       <c r="P24" s="195" t="str">
         <f>INDEX('Policy Characteristics'!J:J,MATCH($C24,'Policy Characteristics'!$C:$C,0))</f>
-        <v>**Description:** This policy causes government to pay for the specified percentage of the purchase price of new battery electric passenger LDVs.  This is in addition to EV subsidies that exist in the BAU case.  // **Guidance for setting values:** In Canada, several provinces have EV subsidy programs, paying for between $5000 and $14000 of the cost of a new EV.  This is roughly between 10% and 35% of the cost of a new EV.</v>
+        <v>**Description:** This policy causes government to pay for the specified percentage of the purchase price of new battery electric vehicles for the selected type(s).  This is in addition to EV subsidies that exist in the BAU case.  // **Guidance for setting values:** In Canada, several provinces have EV subsidy programs, paying for between $5000 and $14000 of the cost of a new EV.  This is roughly between 10% and 35% of the cost of a new EV.</v>
       </c>
       <c r="Q24" s="57" t="str">
         <f t="shared" si="8"/>
@@ -10753,7 +10753,7 @@
       <c r="O25" s="77"/>
       <c r="P25" s="195" t="str">
         <f>INDEX('Policy Characteristics'!J:J,MATCH($C25,'Policy Characteristics'!$C:$C,0))</f>
-        <v>**Description:** This policy causes government to pay for the specified percentage of the purchase price of new battery electric passenger LDVs.  This is in addition to EV subsidies that exist in the BAU case.  // **Guidance for setting values:** In Canada, several provinces have EV subsidy programs, paying for between $5000 and $14000 of the cost of a new EV.  This is roughly between 10% and 35% of the cost of a new EV.</v>
+        <v>**Description:** This policy causes government to pay for the specified percentage of the purchase price of new battery electric vehicles for the selected type(s).  This is in addition to EV subsidies that exist in the BAU case.  // **Guidance for setting values:** In Canada, several provinces have EV subsidy programs, paying for between $5000 and $14000 of the cost of a new EV.  This is roughly between 10% and 35% of the cost of a new EV.</v>
       </c>
       <c r="Q25" s="77"/>
       <c r="R25" s="77"/>
@@ -10803,7 +10803,7 @@
       <c r="O26" s="77"/>
       <c r="P26" s="195" t="str">
         <f>INDEX('Policy Characteristics'!J:J,MATCH($C26,'Policy Characteristics'!$C:$C,0))</f>
-        <v>**Description:** This policy causes government to pay for the specified percentage of the purchase price of new battery electric passenger LDVs.  This is in addition to EV subsidies that exist in the BAU case.  // **Guidance for setting values:** In Canada, several provinces have EV subsidy programs, paying for between $5000 and $14000 of the cost of a new EV.  This is roughly between 10% and 35% of the cost of a new EV.</v>
+        <v>**Description:** This policy causes government to pay for the specified percentage of the purchase price of new battery electric vehicles for the selected type(s).  This is in addition to EV subsidies that exist in the BAU case.  // **Guidance for setting values:** In Canada, several provinces have EV subsidy programs, paying for between $5000 and $14000 of the cost of a new EV.  This is roughly between 10% and 35% of the cost of a new EV.</v>
       </c>
       <c r="Q26" s="77"/>
       <c r="R26" s="77"/>
@@ -10853,7 +10853,7 @@
       <c r="O27" s="77"/>
       <c r="P27" s="195" t="str">
         <f>INDEX('Policy Characteristics'!J:J,MATCH($C27,'Policy Characteristics'!$C:$C,0))</f>
-        <v>**Description:** This policy causes government to pay for the specified percentage of the purchase price of new battery electric passenger LDVs.  This is in addition to EV subsidies that exist in the BAU case.  // **Guidance for setting values:** In Canada, several provinces have EV subsidy programs, paying for between $5000 and $14000 of the cost of a new EV.  This is roughly between 10% and 35% of the cost of a new EV.</v>
+        <v>**Description:** This policy causes government to pay for the specified percentage of the purchase price of new battery electric vehicles for the selected type(s).  This is in addition to EV subsidies that exist in the BAU case.  // **Guidance for setting values:** In Canada, several provinces have EV subsidy programs, paying for between $5000 and $14000 of the cost of a new EV.  This is roughly between 10% and 35% of the cost of a new EV.</v>
       </c>
       <c r="Q27" s="77"/>
       <c r="R27" s="77"/>
@@ -10903,7 +10903,7 @@
       <c r="O28" s="77"/>
       <c r="P28" s="195" t="str">
         <f>INDEX('Policy Characteristics'!J:J,MATCH($C28,'Policy Characteristics'!$C:$C,0))</f>
-        <v>**Description:** This policy causes government to pay for the specified percentage of the purchase price of new battery electric passenger LDVs.  This is in addition to EV subsidies that exist in the BAU case.  // **Guidance for setting values:** In Canada, several provinces have EV subsidy programs, paying for between $5000 and $14000 of the cost of a new EV.  This is roughly between 10% and 35% of the cost of a new EV.</v>
+        <v>**Description:** This policy causes government to pay for the specified percentage of the purchase price of new battery electric vehicles for the selected type(s).  This is in addition to EV subsidies that exist in the BAU case.  // **Guidance for setting values:** In Canada, several provinces have EV subsidy programs, paying for between $5000 and $14000 of the cost of a new EV.  This is roughly between 10% and 35% of the cost of a new EV.</v>
       </c>
       <c r="Q28" s="77"/>
       <c r="R28" s="77"/>
@@ -10953,7 +10953,7 @@
       <c r="O29" s="77"/>
       <c r="P29" s="195" t="str">
         <f>INDEX('Policy Characteristics'!J:J,MATCH($C29,'Policy Characteristics'!$C:$C,0))</f>
-        <v>**Description:** This policy causes government to pay for the specified percentage of the purchase price of new battery electric passenger LDVs.  This is in addition to EV subsidies that exist in the BAU case.  // **Guidance for setting values:** In Canada, several provinces have EV subsidy programs, paying for between $5000 and $14000 of the cost of a new EV.  This is roughly between 10% and 35% of the cost of a new EV.</v>
+        <v>**Description:** This policy causes government to pay for the specified percentage of the purchase price of new battery electric vehicles for the selected type(s).  This is in addition to EV subsidies that exist in the BAU case.  // **Guidance for setting values:** In Canada, several provinces have EV subsidy programs, paying for between $5000 and $14000 of the cost of a new EV.  This is roughly between 10% and 35% of the cost of a new EV.</v>
       </c>
       <c r="Q29" s="77"/>
       <c r="R29" s="77"/>
@@ -11003,7 +11003,7 @@
       <c r="O30" s="77"/>
       <c r="P30" s="195" t="str">
         <f>INDEX('Policy Characteristics'!J:J,MATCH($C30,'Policy Characteristics'!$C:$C,0))</f>
-        <v>**Description:** This policy causes government to pay for the specified percentage of the purchase price of new battery electric passenger LDVs.  This is in addition to EV subsidies that exist in the BAU case.  // **Guidance for setting values:** In Canada, several provinces have EV subsidy programs, paying for between $5000 and $14000 of the cost of a new EV.  This is roughly between 10% and 35% of the cost of a new EV.</v>
+        <v>**Description:** This policy causes government to pay for the specified percentage of the purchase price of new battery electric vehicles for the selected type(s).  This is in addition to EV subsidies that exist in the BAU case.  // **Guidance for setting values:** In Canada, several provinces have EV subsidy programs, paying for between $5000 and $14000 of the cost of a new EV.  This is roughly between 10% and 35% of the cost of a new EV.</v>
       </c>
       <c r="Q30" s="77"/>
       <c r="R30" s="77"/>
@@ -11053,7 +11053,7 @@
       <c r="O31" s="77"/>
       <c r="P31" s="195" t="str">
         <f>INDEX('Policy Characteristics'!J:J,MATCH($C31,'Policy Characteristics'!$C:$C,0))</f>
-        <v>**Description:** This policy causes government to pay for the specified percentage of the purchase price of new battery electric passenger LDVs.  This is in addition to EV subsidies that exist in the BAU case.  // **Guidance for setting values:** In Canada, several provinces have EV subsidy programs, paying for between $5000 and $14000 of the cost of a new EV.  This is roughly between 10% and 35% of the cost of a new EV.</v>
+        <v>**Description:** This policy causes government to pay for the specified percentage of the purchase price of new battery electric vehicles for the selected type(s).  This is in addition to EV subsidies that exist in the BAU case.  // **Guidance for setting values:** In Canada, several provinces have EV subsidy programs, paying for between $5000 and $14000 of the cost of a new EV.  This is roughly between 10% and 35% of the cost of a new EV.</v>
       </c>
       <c r="Q31" s="77"/>
       <c r="R31" s="77"/>
@@ -11103,7 +11103,7 @@
       <c r="O32" s="77"/>
       <c r="P32" s="195" t="str">
         <f>INDEX('Policy Characteristics'!J:J,MATCH($C32,'Policy Characteristics'!$C:$C,0))</f>
-        <v>**Description:** This policy causes government to pay for the specified percentage of the purchase price of new battery electric passenger LDVs.  This is in addition to EV subsidies that exist in the BAU case.  // **Guidance for setting values:** In Canada, several provinces have EV subsidy programs, paying for between $5000 and $14000 of the cost of a new EV.  This is roughly between 10% and 35% of the cost of a new EV.</v>
+        <v>**Description:** This policy causes government to pay for the specified percentage of the purchase price of new battery electric vehicles for the selected type(s).  This is in addition to EV subsidies that exist in the BAU case.  // **Guidance for setting values:** In Canada, several provinces have EV subsidy programs, paying for between $5000 and $14000 of the cost of a new EV.  This is roughly between 10% and 35% of the cost of a new EV.</v>
       </c>
       <c r="Q32" s="77"/>
       <c r="R32" s="77"/>
@@ -13296,7 +13296,7 @@
       </c>
       <c r="P73" s="195" t="str">
         <f>INDEX('Policy Characteristics'!J:J,MATCH($C73,'Policy Characteristics'!$C:$C,0))</f>
-        <v xml:space="preserve">**Description:** This policy replaces the specified fraction of newly sold non-electric building components of the selected type(s) in buildings of the selected type(s) with electricity-using components. // **Guidance for setting values:** // **Urban Residential:** In the BAU case, the share of electricity among fuels used by urban, residential buildings will rise between 2017 and 2050.  // **Rural Residential:** In the BAU case, the share of electricity among fuels used by urban, residential buildings will rise between 2017 and 2050.  // **Commercial:** In the BAU case, the share of electricity among fuels used by urban, residential buildings will rise between 2017 and 2050. </v>
+        <v xml:space="preserve">**Description:** This policy replaces the specified fraction of newly sold non-electric building components in buildings of the selected type(s) with electricity-using components. // **Guidance for setting values:** // **Urban Residential:** In the BAU case, the share of electricity among fuels used by urban, residential buildings will rise between 2017 and 2050.  // **Rural Residential:** In the BAU case, the share of electricity among fuels used by urban, residential buildings will rise between 2017 and 2050.  // **Commercial:** In the BAU case, the share of electricity among fuels used by urban, residential buildings will rise between 2017 and 2050. </v>
       </c>
       <c r="Q73" s="55" t="s">
         <v>240</v>
@@ -13360,7 +13360,7 @@
       </c>
       <c r="P74" s="195" t="str">
         <f>INDEX('Policy Characteristics'!J:J,MATCH($C74,'Policy Characteristics'!$C:$C,0))</f>
-        <v xml:space="preserve">**Description:** This policy replaces the specified fraction of newly sold non-electric building components of the selected type(s) in buildings of the selected type(s) with electricity-using components. // **Guidance for setting values:** // **Urban Residential:** In the BAU case, the share of electricity among fuels used by urban, residential buildings will rise between 2017 and 2050.  // **Rural Residential:** In the BAU case, the share of electricity among fuels used by urban, residential buildings will rise between 2017 and 2050.  // **Commercial:** In the BAU case, the share of electricity among fuels used by urban, residential buildings will rise between 2017 and 2050. </v>
+        <v xml:space="preserve">**Description:** This policy replaces the specified fraction of newly sold non-electric building components in buildings of the selected type(s) with electricity-using components. // **Guidance for setting values:** // **Urban Residential:** In the BAU case, the share of electricity among fuels used by urban, residential buildings will rise between 2017 and 2050.  // **Rural Residential:** In the BAU case, the share of electricity among fuels used by urban, residential buildings will rise between 2017 and 2050.  // **Commercial:** In the BAU case, the share of electricity among fuels used by urban, residential buildings will rise between 2017 and 2050. </v>
       </c>
       <c r="Q74" s="60" t="str">
         <f t="shared" si="15"/>
@@ -13426,7 +13426,7 @@
       </c>
       <c r="P75" s="195" t="str">
         <f>INDEX('Policy Characteristics'!J:J,MATCH($C75,'Policy Characteristics'!$C:$C,0))</f>
-        <v xml:space="preserve">**Description:** This policy replaces the specified fraction of newly sold non-electric building components of the selected type(s) in buildings of the selected type(s) with electricity-using components. // **Guidance for setting values:** // **Urban Residential:** In the BAU case, the share of electricity among fuels used by urban, residential buildings will rise between 2017 and 2050.  // **Rural Residential:** In the BAU case, the share of electricity among fuels used by urban, residential buildings will rise between 2017 and 2050.  // **Commercial:** In the BAU case, the share of electricity among fuels used by urban, residential buildings will rise between 2017 and 2050. </v>
+        <v xml:space="preserve">**Description:** This policy replaces the specified fraction of newly sold non-electric building components in buildings of the selected type(s) with electricity-using components. // **Guidance for setting values:** // **Urban Residential:** In the BAU case, the share of electricity among fuels used by urban, residential buildings will rise between 2017 and 2050.  // **Rural Residential:** In the BAU case, the share of electricity among fuels used by urban, residential buildings will rise between 2017 and 2050.  // **Commercial:** In the BAU case, the share of electricity among fuels used by urban, residential buildings will rise between 2017 and 2050. </v>
       </c>
       <c r="Q75" s="60" t="str">
         <f t="shared" si="15"/>
@@ -15070,7 +15070,7 @@
       </c>
       <c r="T97" s="57"/>
     </row>
-    <row r="98" spans="1:20" s="5" customFormat="1" ht="265.5" x14ac:dyDescent="0.75">
+    <row r="98" spans="1:20" s="5" customFormat="1" ht="309.75" x14ac:dyDescent="0.75">
       <c r="A98" s="55" t="s">
         <v>83</v>
       </c>
@@ -15130,7 +15130,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="99" spans="1:20" s="5" customFormat="1" ht="265.5" x14ac:dyDescent="0.75">
+    <row r="99" spans="1:20" s="5" customFormat="1" ht="309.75" x14ac:dyDescent="0.75">
       <c r="A99" s="57" t="str">
         <f>A$98</f>
         <v>Buildings and Appliances</v>
@@ -15197,7 +15197,7 @@
       </c>
       <c r="T99" s="57"/>
     </row>
-    <row r="100" spans="1:20" s="5" customFormat="1" ht="265.5" x14ac:dyDescent="0.75">
+    <row r="100" spans="1:20" s="5" customFormat="1" ht="309.75" x14ac:dyDescent="0.75">
       <c r="A100" s="57" t="str">
         <f>A$98</f>
         <v>Buildings and Appliances</v>
@@ -15264,7 +15264,7 @@
       </c>
       <c r="T100" s="57"/>
     </row>
-    <row r="101" spans="1:20" s="5" customFormat="1" ht="265.5" x14ac:dyDescent="0.75">
+    <row r="101" spans="1:20" s="5" customFormat="1" ht="309.75" x14ac:dyDescent="0.75">
       <c r="A101" s="57" t="str">
         <f>A$98</f>
         <v>Buildings and Appliances</v>
@@ -15331,7 +15331,7 @@
       </c>
       <c r="T101" s="57"/>
     </row>
-    <row r="102" spans="1:20" s="5" customFormat="1" ht="265.5" x14ac:dyDescent="0.75">
+    <row r="102" spans="1:20" s="5" customFormat="1" ht="309.75" x14ac:dyDescent="0.75">
       <c r="A102" s="57" t="str">
         <f>A$98</f>
         <v>Buildings and Appliances</v>
@@ -15398,7 +15398,7 @@
       </c>
       <c r="T102" s="57"/>
     </row>
-    <row r="103" spans="1:20" s="5" customFormat="1" ht="265.5" x14ac:dyDescent="0.75">
+    <row r="103" spans="1:20" s="5" customFormat="1" ht="309.75" x14ac:dyDescent="0.75">
       <c r="A103" s="57" t="str">
         <f>A$98</f>
         <v>Buildings and Appliances</v>

</xml_diff>

<commit_message>
Update to WebAppData file Renewable Portfolio Standard description
</commit_message>
<xml_diff>
--- a/WebAppData.xlsx
+++ b/WebAppData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swenzel\Dropbox (Energy Innovation)\My PC (energy044)\Documents\GitHub_Repositories\eps-alberta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91A64F54-15DF-4921-8A5C-C5ADB446E497}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{252D21EB-AB70-49F4-989E-467C09717357}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12600" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="824" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21120" yWindow="-16155" windowWidth="19905" windowHeight="15195" tabRatio="824" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="10" r:id="rId1"/>
@@ -4053,9 +4053,6 @@
     <t>**Description:** This policy is a subsidy paid by the government to suppliers of electricity per unit of electricity generated from the selected plant type(s). // **Guidance for setting values:** Note that the Energy Policy Simulator chooses which new power plants to build based on lifetime plant costs. // **Cogeneration:** Canada does not currently offer subsidies for utility-scale renewable electricity generation.  In the U.S., until its expiration in 2013, the Renewable Electricity Production Tax Credit (PTC) offered between US$11/MWh and US$23/MWh for electricity from wind, geothermal, and biomass.  State-level tax credits and feed-in tariffs for renewable energy range as high as US$54/MWh. // **Onshore Wind, Solar PV, Solar Thermal, Offshore Wind:** Canada does not currently offer subsidies for utility-scale renewable electricity generation.  In the U.S., until its expiration in 2013, the Renewable Electricity Production Tax Credit (PTC) offered between US$11/MWh and US$23/MWh for electricity from wind, geothermal, and biomass.  State-level tax credits and feed-in tariffs for renewable energy range as high as US$54/MWh. // **Biomass:** Canada does not currently offer subsidies for utility-scale renewable electricity generation.  In the U.S., until its expiration in 2013, the Renewable Electricity Production Tax Credit (PTC) offered between US$11/MWh and US$23/MWh for electricity from wind, geothermal, and biomass.  State-level tax credits and feed-in tariffs for renewable energy range as high as US$54/MWh. // **Geothermal:** Canada does not currently offer subsidies for utility-scale renewable electricity generation.  In the U.S., until its expiration in 2013, the Renewable Electricity Production Tax Credit (PTC) offered between US$11/MWh and US$23/MWh for electricity from wind, geothermal, and biomass.  State-level tax credits and feed-in tariffs for renewable energy range as high as US$54/MWh.</t>
   </si>
   <si>
-    <t xml:space="preserve">**Description:** This policy specifies the fraction of potential electricity generation that must come from qualifying clean energy sources (hydro, wind, solar, and biomass) in 2050. // **Guidance for setting values:** In the BAU case, the share of Alberta's electricity from qualifying sources rises from 8% in 2017 to 15% in 2050. </t>
-  </si>
-  <si>
     <t>Clean Energy Standard</t>
   </si>
   <si>
@@ -4117,6 +4114,9 @@
   </si>
   <si>
     <t xml:space="preserve">**Description:** This policy replaces the specified fraction of newly sold non-electric building components in buildings of the selected type(s) with electricity-using components. // **Guidance for setting values:** // **Urban Residential:** In the BAU case, the share of electricity among fuels used by urban, residential buildings will rise between 2017 and 2050.  // **Rural Residential:** In the BAU case, the share of electricity among fuels used by urban, residential buildings will rise between 2017 and 2050.  // **Commercial:** In the BAU case, the share of electricity among fuels used by urban, residential buildings will rise between 2017 and 2050. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">**Description:** This policy specifies the fraction of potential electricity generation that must come from qualifying clean energy sources (wind, solar, geothermal, and biomass) in 2050. // **Guidance for setting values:** In the BAU case, the share of Alberta's electricity from qualifying sources rises from 8% in 2017 to 15% in 2050. </t>
   </si>
 </sst>
 </file>
@@ -5340,6 +5340,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -5348,9 +5351,6 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -6419,8 +6419,8 @@
   </sheetPr>
   <dimension ref="A1:N105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -6442,7 +6442,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A1" s="190" t="s">
-        <v>1207</v>
+        <v>1206</v>
       </c>
       <c r="B1" s="188"/>
       <c r="C1" s="188"/>
@@ -6460,7 +6460,7 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A2" s="189" t="s">
-        <v>1206</v>
+        <v>1205</v>
       </c>
       <c r="B2" s="188"/>
       <c r="C2" s="188"/>
@@ -6549,7 +6549,7 @@
         <v>1023</v>
       </c>
       <c r="J4" s="169" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
       <c r="K4" s="75" t="s">
         <v>1024</v>
@@ -6625,7 +6625,7 @@
         <v>579</v>
       </c>
       <c r="J6" s="169" t="s">
-        <v>1208</v>
+        <v>1207</v>
       </c>
       <c r="K6" s="75" t="s">
         <v>580</v>
@@ -6663,7 +6663,7 @@
         <v>567</v>
       </c>
       <c r="J7" s="169" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
       <c r="K7" s="75" t="s">
         <v>568</v>
@@ -6701,7 +6701,7 @@
         <v>547</v>
       </c>
       <c r="J8" s="169" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
       <c r="K8" s="169" t="s">
         <v>234</v>
@@ -6745,7 +6745,7 @@
         <v>127</v>
       </c>
       <c r="J9" s="169" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
       <c r="K9" s="169" t="s">
         <v>236</v>
@@ -6823,7 +6823,7 @@
         <v>44</v>
       </c>
       <c r="J11" s="169" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
       <c r="K11" s="169" t="s">
         <v>238</v>
@@ -6864,7 +6864,7 @@
         <v>129</v>
       </c>
       <c r="J12" s="169" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
       <c r="K12" s="169" t="s">
         <v>240</v>
@@ -6902,7 +6902,7 @@
         <v>38</v>
       </c>
       <c r="J13" s="169" t="s">
-        <v>1202</v>
+        <v>1201</v>
       </c>
       <c r="K13" s="169" t="s">
         <v>242</v>
@@ -7106,7 +7106,7 @@
         <v>43</v>
       </c>
       <c r="J18" s="169" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="K18" s="169" t="s">
         <v>248</v>
@@ -7150,7 +7150,7 @@
         <v>35</v>
       </c>
       <c r="J19" s="169" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
       <c r="K19" s="169" t="s">
         <v>250</v>
@@ -7188,7 +7188,7 @@
         <v>35</v>
       </c>
       <c r="J20" s="169" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
       <c r="K20" s="169" t="s">
         <v>414</v>
@@ -7266,7 +7266,7 @@
         <v>331</v>
       </c>
       <c r="J22" s="169" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
       <c r="K22" s="169" t="s">
         <v>333</v>
@@ -7374,7 +7374,7 @@
         <v>230</v>
       </c>
       <c r="J25" s="169" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="K25" s="169" t="s">
         <v>254</v>
@@ -7418,7 +7418,7 @@
         <v>36</v>
       </c>
       <c r="J26" s="169" t="s">
-        <v>1198</v>
+        <v>1197</v>
       </c>
       <c r="K26" s="169" t="s">
         <v>256</v>
@@ -7504,7 +7504,7 @@
         <v>35</v>
       </c>
       <c r="J28" s="169" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
       <c r="K28" s="175"/>
       <c r="L28" s="168"/>
@@ -7608,7 +7608,7 @@
         <v>313</v>
       </c>
       <c r="J31" s="169" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
       <c r="K31" s="168" t="s">
         <v>612</v>
@@ -7648,7 +7648,7 @@
         <v>815</v>
       </c>
       <c r="J32" s="169" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
       <c r="K32" s="168" t="s">
         <v>946</v>
@@ -7709,7 +7709,7 @@
         <v>368</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
       <c r="E34" s="4" t="s">
         <v>678</v>
@@ -7727,7 +7727,7 @@
         <v>42</v>
       </c>
       <c r="J34" s="169" t="s">
-        <v>1193</v>
+        <v>1214</v>
       </c>
       <c r="K34" s="169" t="s">
         <v>261</v>
@@ -8733,7 +8733,7 @@
         <v>981</v>
       </c>
       <c r="J59" s="196" t="s">
-        <v>1209</v>
+        <v>1208</v>
       </c>
       <c r="K59" s="169" t="s">
         <v>295</v>
@@ -19531,7 +19531,7 @@
       </c>
       <c r="P183" s="195" t="str">
         <f>INDEX('Policy Characteristics'!J:J,MATCH($C183,'Policy Characteristics'!$C:$C,0))</f>
-        <v xml:space="preserve">**Description:** This policy specifies the fraction of potential electricity generation that must come from qualifying clean energy sources (hydro, wind, solar, and biomass) in 2050. // **Guidance for setting values:** In the BAU case, the share of Alberta's electricity from qualifying sources rises from 8% in 2017 to 15% in 2050. </v>
+        <v xml:space="preserve">**Description:** This policy specifies the fraction of potential electricity generation that must come from qualifying clean energy sources (wind, solar, geothermal, and biomass) in 2050. // **Guidance for setting values:** In the BAU case, the share of Alberta's electricity from qualifying sources rises from 8% in 2017 to 15% in 2050. </v>
       </c>
       <c r="Q183" s="55" t="s">
         <v>261</v>
@@ -31737,13 +31737,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A1" s="200" t="s">
+      <c r="A1" s="197" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="200"/>
-      <c r="C1" s="200"/>
-      <c r="D1" s="200"/>
-      <c r="E1" s="200"/>
+      <c r="B1" s="197"/>
+      <c r="C1" s="197"/>
+      <c r="D1" s="197"/>
+      <c r="E1" s="197"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A2" s="201" t="s">
@@ -31812,13 +31812,13 @@
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A60" s="200" t="s">
+      <c r="A60" s="197" t="s">
         <v>198</v>
       </c>
-      <c r="B60" s="200"/>
-      <c r="C60" s="200"/>
-      <c r="D60" s="200"/>
-      <c r="E60" s="200"/>
+      <c r="B60" s="197"/>
+      <c r="C60" s="197"/>
+      <c r="D60" s="197"/>
+      <c r="E60" s="197"/>
     </row>
     <row r="85" spans="1:39" s="12" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A85" s="9" t="s">
@@ -31923,13 +31923,13 @@
       </c>
     </row>
     <row r="89" spans="1:39" x14ac:dyDescent="0.75">
-      <c r="A89" s="200" t="s">
+      <c r="A89" s="197" t="s">
         <v>199</v>
       </c>
-      <c r="B89" s="200"/>
-      <c r="C89" s="200"/>
-      <c r="D89" s="200"/>
-      <c r="E89" s="200"/>
+      <c r="B89" s="197"/>
+      <c r="C89" s="197"/>
+      <c r="D89" s="197"/>
+      <c r="E89" s="197"/>
     </row>
     <row r="90" spans="1:39" x14ac:dyDescent="0.75">
       <c r="A90" s="9">
@@ -32016,13 +32016,13 @@
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A98" s="200" t="s">
+      <c r="A98" s="197" t="s">
         <v>200</v>
       </c>
-      <c r="B98" s="200"/>
-      <c r="C98" s="200"/>
-      <c r="D98" s="200"/>
-      <c r="E98" s="200"/>
+      <c r="B98" s="197"/>
+      <c r="C98" s="197"/>
+      <c r="D98" s="197"/>
+      <c r="E98" s="197"/>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A99" s="17">
@@ -32106,13 +32106,13 @@
       <c r="A108" s="20"/>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A109" s="200" t="s">
+      <c r="A109" s="197" t="s">
         <v>202</v>
       </c>
-      <c r="B109" s="200"/>
-      <c r="C109" s="200"/>
-      <c r="D109" s="200"/>
-      <c r="E109" s="200"/>
+      <c r="B109" s="197"/>
+      <c r="C109" s="197"/>
+      <c r="D109" s="197"/>
+      <c r="E109" s="197"/>
     </row>
     <row r="110" spans="1:5" ht="15.5" thickBot="1" x14ac:dyDescent="0.9"/>
     <row r="111" spans="1:5" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
@@ -32125,13 +32125,13 @@
       </c>
     </row>
     <row r="113" spans="1:14" x14ac:dyDescent="0.75">
-      <c r="A113" s="200" t="s">
+      <c r="A113" s="197" t="s">
         <v>201</v>
       </c>
-      <c r="B113" s="200"/>
-      <c r="C113" s="200"/>
-      <c r="D113" s="200"/>
-      <c r="E113" s="200"/>
+      <c r="B113" s="197"/>
+      <c r="C113" s="197"/>
+      <c r="D113" s="197"/>
+      <c r="E113" s="197"/>
     </row>
     <row r="114" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A114" s="17">
@@ -32212,13 +32212,13 @@
       </c>
     </row>
     <row r="124" spans="1:14" x14ac:dyDescent="0.75">
-      <c r="A124" s="200" t="s">
+      <c r="A124" s="197" t="s">
         <v>482</v>
       </c>
-      <c r="B124" s="200"/>
-      <c r="C124" s="200"/>
-      <c r="D124" s="200"/>
-      <c r="E124" s="200"/>
+      <c r="B124" s="197"/>
+      <c r="C124" s="197"/>
+      <c r="D124" s="197"/>
+      <c r="E124" s="197"/>
       <c r="L124" s="21"/>
     </row>
     <row r="125" spans="1:14" x14ac:dyDescent="0.75">
@@ -32309,13 +32309,13 @@
       <c r="C133" s="15"/>
     </row>
     <row r="134" spans="1:14" x14ac:dyDescent="0.75">
-      <c r="A134" s="200" t="s">
+      <c r="A134" s="197" t="s">
         <v>115</v>
       </c>
-      <c r="B134" s="200"/>
-      <c r="C134" s="200"/>
-      <c r="D134" s="200"/>
-      <c r="E134" s="200"/>
+      <c r="B134" s="197"/>
+      <c r="C134" s="197"/>
+      <c r="D134" s="197"/>
+      <c r="E134" s="197"/>
     </row>
     <row r="135" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A135" s="27" t="s">
@@ -32330,25 +32330,25 @@
     </row>
     <row r="136" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A136" s="29"/>
-      <c r="B136" s="197" t="s">
+      <c r="B136" s="198" t="s">
         <v>502</v>
       </c>
-      <c r="C136" s="198"/>
-      <c r="D136" s="198"/>
-      <c r="E136" s="199"/>
+      <c r="C136" s="199"/>
+      <c r="D136" s="199"/>
+      <c r="E136" s="200"/>
       <c r="F136" s="28"/>
       <c r="G136" s="28"/>
     </row>
     <row r="137" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A137" s="30"/>
-      <c r="B137" s="197" t="s">
+      <c r="B137" s="198" t="s">
         <v>503</v>
       </c>
-      <c r="C137" s="199"/>
-      <c r="D137" s="197" t="s">
+      <c r="C137" s="200"/>
+      <c r="D137" s="198" t="s">
         <v>504</v>
       </c>
-      <c r="E137" s="199"/>
+      <c r="E137" s="200"/>
       <c r="F137" s="28"/>
       <c r="G137" s="28"/>
     </row>
@@ -32895,13 +32895,13 @@
       <c r="G163" s="28"/>
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A165" s="200" t="s">
+      <c r="A165" s="197" t="s">
         <v>205</v>
       </c>
-      <c r="B165" s="200"/>
-      <c r="C165" s="200"/>
-      <c r="D165" s="200"/>
-      <c r="E165" s="200"/>
+      <c r="B165" s="197"/>
+      <c r="C165" s="197"/>
+      <c r="D165" s="197"/>
+      <c r="E165" s="197"/>
     </row>
     <row r="166" spans="1:7" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
       <c r="A166" s="23" t="s">
@@ -32924,10 +32924,10 @@
       <c r="B168" s="46"/>
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A169" s="200" t="s">
+      <c r="A169" s="197" t="s">
         <v>490</v>
       </c>
-      <c r="B169" s="200"/>
+      <c r="B169" s="197"/>
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A170" s="23" t="s">
@@ -32959,13 +32959,13 @@
       <c r="B173" s="46"/>
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A174" s="200" t="s">
+      <c r="A174" s="197" t="s">
         <v>215</v>
       </c>
-      <c r="B174" s="200"/>
-      <c r="C174" s="200"/>
-      <c r="D174" s="200"/>
-      <c r="E174" s="200"/>
+      <c r="B174" s="197"/>
+      <c r="C174" s="197"/>
+      <c r="D174" s="197"/>
+      <c r="E174" s="197"/>
     </row>
     <row r="175" spans="1:7" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
       <c r="A175" s="23" t="s">
@@ -32985,13 +32985,13 @@
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A178" s="200" t="s">
+      <c r="A178" s="197" t="s">
         <v>208</v>
       </c>
-      <c r="B178" s="200"/>
-      <c r="C178" s="200"/>
-      <c r="D178" s="200"/>
-      <c r="E178" s="200"/>
+      <c r="B178" s="197"/>
+      <c r="C178" s="197"/>
+      <c r="D178" s="197"/>
+      <c r="E178" s="197"/>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A179" s="25" t="s">
@@ -33019,13 +33019,13 @@
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A183" s="200" t="s">
+      <c r="A183" s="197" t="s">
         <v>210</v>
       </c>
-      <c r="B183" s="200"/>
-      <c r="C183" s="200"/>
-      <c r="D183" s="200"/>
-      <c r="E183" s="200"/>
+      <c r="B183" s="197"/>
+      <c r="C183" s="197"/>
+      <c r="D183" s="197"/>
+      <c r="E183" s="197"/>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A184" s="23" t="s">
@@ -33080,13 +33080,13 @@
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A191" s="200" t="s">
+      <c r="A191" s="197" t="s">
         <v>227</v>
       </c>
-      <c r="B191" s="200"/>
-      <c r="C191" s="200"/>
-      <c r="D191" s="200"/>
-      <c r="E191" s="200"/>
+      <c r="B191" s="197"/>
+      <c r="C191" s="197"/>
+      <c r="D191" s="197"/>
+      <c r="E191" s="197"/>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A192" s="21" t="s">
@@ -33146,12 +33146,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A191:E191"/>
-    <mergeCell ref="A165:E165"/>
-    <mergeCell ref="A178:E178"/>
-    <mergeCell ref="A183:E183"/>
-    <mergeCell ref="A174:E174"/>
-    <mergeCell ref="A169:B169"/>
     <mergeCell ref="B136:E136"/>
     <mergeCell ref="B137:C137"/>
     <mergeCell ref="D137:E137"/>
@@ -33166,6 +33160,12 @@
     <mergeCell ref="A113:E113"/>
     <mergeCell ref="A109:E109"/>
     <mergeCell ref="A124:E124"/>
+    <mergeCell ref="A191:E191"/>
+    <mergeCell ref="A165:E165"/>
+    <mergeCell ref="A178:E178"/>
+    <mergeCell ref="A183:E183"/>
+    <mergeCell ref="A174:E174"/>
+    <mergeCell ref="A169:B169"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
add a missing second tier graph title
</commit_message>
<xml_diff>
--- a/WebAppData.xlsx
+++ b/WebAppData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10514"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/todd/eps/eps-alberta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46D45410-1983-6C4D-A2C3-6C93D86279EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D26C47C4-4A3F-CD43-9D4C-C4036EA958E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="60160" windowHeight="33340" tabRatio="824" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="60160" windowHeight="33340" tabRatio="824" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="10" r:id="rId1"/>
@@ -257,7 +257,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5446" uniqueCount="1215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5447" uniqueCount="1216">
   <si>
     <t>Short Name</t>
   </si>
@@ -4117,6 +4117,9 @@
   </si>
   <si>
     <t xml:space="preserve">**Description:** This policy specifies the fraction of potential electricity generation that must come from qualifying clean energy sources (wind, solar, geothermal, and biomass) in 2050. // **Guidance for setting values:** In the BAU case, the share of Alberta's electricity from qualifying sources rises from 8% in 2017 to 15% in 2050. </t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -5189,6 +5192,9 @@
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -5197,9 +5203,6 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -8800,8 +8803,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:T327"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A132" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A147" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B142" sqref="B142"/>
     </sheetView>
   </sheetViews>
@@ -27426,9 +27429,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:S79"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E22" sqref="E22"/>
+      <selection pane="bottomLeft" activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -28023,7 +28026,9 @@
       <c r="A22" s="3" t="s">
         <v>451</v>
       </c>
-      <c r="B22" s="3"/>
+      <c r="B22" s="3" t="s">
+        <v>1215</v>
+      </c>
       <c r="C22" s="46">
         <v>1</v>
       </c>
@@ -31063,13 +31068,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="145" t="s">
+      <c r="A1" s="142" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="145"/>
-      <c r="C1" s="145"/>
-      <c r="D1" s="145"/>
-      <c r="E1" s="145"/>
+      <c r="B1" s="142"/>
+      <c r="C1" s="142"/>
+      <c r="D1" s="142"/>
+      <c r="E1" s="142"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="146" t="s">
@@ -31138,13 +31143,13 @@
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A60" s="145" t="s">
+      <c r="A60" s="142" t="s">
         <v>198</v>
       </c>
-      <c r="B60" s="145"/>
-      <c r="C60" s="145"/>
-      <c r="D60" s="145"/>
-      <c r="E60" s="145"/>
+      <c r="B60" s="142"/>
+      <c r="C60" s="142"/>
+      <c r="D60" s="142"/>
+      <c r="E60" s="142"/>
     </row>
     <row r="85" spans="1:39" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
@@ -31249,13 +31254,13 @@
       </c>
     </row>
     <row r="89" spans="1:39" x14ac:dyDescent="0.2">
-      <c r="A89" s="145" t="s">
+      <c r="A89" s="142" t="s">
         <v>199</v>
       </c>
-      <c r="B89" s="145"/>
-      <c r="C89" s="145"/>
-      <c r="D89" s="145"/>
-      <c r="E89" s="145"/>
+      <c r="B89" s="142"/>
+      <c r="C89" s="142"/>
+      <c r="D89" s="142"/>
+      <c r="E89" s="142"/>
     </row>
     <row r="90" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A90">
@@ -31342,13 +31347,13 @@
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A98" s="145" t="s">
+      <c r="A98" s="142" t="s">
         <v>200</v>
       </c>
-      <c r="B98" s="145"/>
-      <c r="C98" s="145"/>
-      <c r="D98" s="145"/>
-      <c r="E98" s="145"/>
+      <c r="B98" s="142"/>
+      <c r="C98" s="142"/>
+      <c r="D98" s="142"/>
+      <c r="E98" s="142"/>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99" s="14">
@@ -31432,13 +31437,13 @@
       <c r="A108" s="16"/>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A109" s="145" t="s">
+      <c r="A109" s="142" t="s">
         <v>202</v>
       </c>
-      <c r="B109" s="145"/>
-      <c r="C109" s="145"/>
-      <c r="D109" s="145"/>
-      <c r="E109" s="145"/>
+      <c r="B109" s="142"/>
+      <c r="C109" s="142"/>
+      <c r="D109" s="142"/>
+      <c r="E109" s="142"/>
     </row>
     <row r="110" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="111" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -31451,13 +31456,13 @@
       </c>
     </row>
     <row r="113" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A113" s="145" t="s">
+      <c r="A113" s="142" t="s">
         <v>201</v>
       </c>
-      <c r="B113" s="145"/>
-      <c r="C113" s="145"/>
-      <c r="D113" s="145"/>
-      <c r="E113" s="145"/>
+      <c r="B113" s="142"/>
+      <c r="C113" s="142"/>
+      <c r="D113" s="142"/>
+      <c r="E113" s="142"/>
     </row>
     <row r="114" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A114" s="14">
@@ -31538,13 +31543,13 @@
       </c>
     </row>
     <row r="124" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A124" s="145" t="s">
+      <c r="A124" s="142" t="s">
         <v>482</v>
       </c>
-      <c r="B124" s="145"/>
-      <c r="C124" s="145"/>
-      <c r="D124" s="145"/>
-      <c r="E124" s="145"/>
+      <c r="B124" s="142"/>
+      <c r="C124" s="142"/>
+      <c r="D124" s="142"/>
+      <c r="E124" s="142"/>
       <c r="L124" s="17"/>
     </row>
     <row r="125" spans="1:14" x14ac:dyDescent="0.2">
@@ -31634,13 +31639,13 @@
       <c r="C133" s="12"/>
     </row>
     <row r="134" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A134" s="145" t="s">
+      <c r="A134" s="142" t="s">
         <v>115</v>
       </c>
-      <c r="B134" s="145"/>
-      <c r="C134" s="145"/>
-      <c r="D134" s="145"/>
-      <c r="E134" s="145"/>
+      <c r="B134" s="142"/>
+      <c r="C134" s="142"/>
+      <c r="D134" s="142"/>
+      <c r="E134" s="142"/>
     </row>
     <row r="135" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A135" s="21" t="s">
@@ -31655,25 +31660,25 @@
     </row>
     <row r="136" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A136" s="23"/>
-      <c r="B136" s="142" t="s">
+      <c r="B136" s="143" t="s">
         <v>502</v>
       </c>
-      <c r="C136" s="143"/>
-      <c r="D136" s="143"/>
-      <c r="E136" s="144"/>
+      <c r="C136" s="144"/>
+      <c r="D136" s="144"/>
+      <c r="E136" s="145"/>
       <c r="F136" s="22"/>
       <c r="G136" s="22"/>
     </row>
     <row r="137" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A137" s="24"/>
-      <c r="B137" s="142" t="s">
+      <c r="B137" s="143" t="s">
         <v>503</v>
       </c>
-      <c r="C137" s="144"/>
-      <c r="D137" s="142" t="s">
+      <c r="C137" s="145"/>
+      <c r="D137" s="143" t="s">
         <v>504</v>
       </c>
-      <c r="E137" s="144"/>
+      <c r="E137" s="145"/>
       <c r="F137" s="22"/>
       <c r="G137" s="22"/>
     </row>
@@ -32220,13 +32225,13 @@
       <c r="G163" s="22"/>
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A165" s="145" t="s">
+      <c r="A165" s="142" t="s">
         <v>205</v>
       </c>
-      <c r="B165" s="145"/>
-      <c r="C165" s="145"/>
-      <c r="D165" s="145"/>
-      <c r="E165" s="145"/>
+      <c r="B165" s="142"/>
+      <c r="C165" s="142"/>
+      <c r="D165" s="142"/>
+      <c r="E165" s="142"/>
     </row>
     <row r="166" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
@@ -32249,10 +32254,10 @@
       <c r="B168" s="40"/>
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A169" s="145" t="s">
+      <c r="A169" s="142" t="s">
         <v>490</v>
       </c>
-      <c r="B169" s="145"/>
+      <c r="B169" s="142"/>
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
@@ -32284,13 +32289,13 @@
       <c r="B173" s="40"/>
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A174" s="145" t="s">
+      <c r="A174" s="142" t="s">
         <v>215</v>
       </c>
-      <c r="B174" s="145"/>
-      <c r="C174" s="145"/>
-      <c r="D174" s="145"/>
-      <c r="E174" s="145"/>
+      <c r="B174" s="142"/>
+      <c r="C174" s="142"/>
+      <c r="D174" s="142"/>
+      <c r="E174" s="142"/>
     </row>
     <row r="175" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
@@ -32310,13 +32315,13 @@
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A178" s="145" t="s">
+      <c r="A178" s="142" t="s">
         <v>208</v>
       </c>
-      <c r="B178" s="145"/>
-      <c r="C178" s="145"/>
-      <c r="D178" s="145"/>
-      <c r="E178" s="145"/>
+      <c r="B178" s="142"/>
+      <c r="C178" s="142"/>
+      <c r="D178" s="142"/>
+      <c r="E178" s="142"/>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
@@ -32344,13 +32349,13 @@
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A183" s="145" t="s">
+      <c r="A183" s="142" t="s">
         <v>210</v>
       </c>
-      <c r="B183" s="145"/>
-      <c r="C183" s="145"/>
-      <c r="D183" s="145"/>
-      <c r="E183" s="145"/>
+      <c r="B183" s="142"/>
+      <c r="C183" s="142"/>
+      <c r="D183" s="142"/>
+      <c r="E183" s="142"/>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
@@ -32405,13 +32410,13 @@
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A191" s="145" t="s">
+      <c r="A191" s="142" t="s">
         <v>227</v>
       </c>
-      <c r="B191" s="145"/>
-      <c r="C191" s="145"/>
-      <c r="D191" s="145"/>
-      <c r="E191" s="145"/>
+      <c r="B191" s="142"/>
+      <c r="C191" s="142"/>
+      <c r="D191" s="142"/>
+      <c r="E191" s="142"/>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A192" s="17" t="s">
@@ -32471,12 +32476,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A191:E191"/>
-    <mergeCell ref="A165:E165"/>
-    <mergeCell ref="A178:E178"/>
-    <mergeCell ref="A183:E183"/>
-    <mergeCell ref="A174:E174"/>
-    <mergeCell ref="A169:B169"/>
     <mergeCell ref="B136:E136"/>
     <mergeCell ref="B137:C137"/>
     <mergeCell ref="D137:E137"/>
@@ -32491,6 +32490,12 @@
     <mergeCell ref="A113:E113"/>
     <mergeCell ref="A109:E109"/>
     <mergeCell ref="A124:E124"/>
+    <mergeCell ref="A191:E191"/>
+    <mergeCell ref="A165:E165"/>
+    <mergeCell ref="A178:E178"/>
+    <mergeCell ref="A183:E183"/>
+    <mergeCell ref="A174:E174"/>
+    <mergeCell ref="A169:B169"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>